<commit_message>
Flat: latest data (2021-05-20T06:22:01.961Z) {   "date": "2021-05-20T06:22:01.961Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 37,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t> 内１回目</t>
   </si>
@@ -254,7 +254,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（5月18日時点）</t>
+    <t>（5月19日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -699,7 +699,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -747,537 +747,557 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="6">
-        <f t="shared" ref="C4:C25" si="0">SUM(D4:E4)</f>
-        <v>5730967</v>
+        <f t="shared" ref="C4:C26" si="0">SUM(D4:E4)</f>
+        <v>5998833</v>
       </c>
       <c r="D4" s="6">
-        <v>3695908</v>
+        <v>3784071</v>
       </c>
       <c r="E4" s="6">
-        <v>2035059</v>
+        <v>2214762</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D5" s="6">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E5" s="6">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D6" s="6">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E6" s="6">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="13">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D7" s="6">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E7" s="6">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="13">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D8" s="6">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E8" s="6">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="13">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D9" s="6">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E9" s="6">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="13">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D10" s="6">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E10" s="6">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D11" s="6">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E11" s="6">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="13">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D12" s="6">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E12" s="6">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="13">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D13" s="6">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E13" s="6">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="13">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D14" s="6">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E14" s="6">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="13">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D15" s="6">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E15" s="6">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="13">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D16" s="6">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E16" s="6">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="13">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D17" s="6">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E17" s="6">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="13">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D18" s="6">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E18" s="6">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="13">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D19" s="6">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E19" s="6">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="13">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D20" s="6">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E20" s="6">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="13">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D21" s="6">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E21" s="6">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A22" s="15">
-        <v>44305</v>
-      </c>
-      <c r="B22" s="12" t="str">
-        <f t="shared" ref="B22:B25" si="1">"("&amp;TEXT(A22,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A22" s="13">
+        <v>44306</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D22" s="6">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E22" s="6">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23" s="13">
+      <c r="A23" s="15">
+        <v>44305</v>
+      </c>
+      <c r="B23" s="12" t="str">
+        <f t="shared" ref="B23:B26" si="1">"("&amp;TEXT(A23,"aaa")&amp;")"</f>
+        <v>(月)</v>
+      </c>
+      <c r="C23" s="6">
+        <f t="shared" si="0"/>
+        <v>119032</v>
+      </c>
+      <c r="D23" s="6">
+        <v>64725</v>
+      </c>
+      <c r="E23" s="6">
+        <v>54307</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A24" s="13">
         <v>44302</v>
       </c>
-      <c r="B23" s="12" t="str">
+      <c r="B24" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(金)</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C24" s="6">
         <f t="shared" si="0"/>
         <v>69687</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D24" s="6">
         <v>29696</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E24" s="6">
         <v>39991</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A24" s="13">
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A25" s="13">
         <v>44301</v>
       </c>
-      <c r="B24" s="12" t="str">
+      <c r="B25" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(木)</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C25" s="6">
         <f t="shared" si="0"/>
         <v>52620</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D25" s="6">
         <v>16637</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E25" s="6">
         <v>35983</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A25" s="13">
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26" s="13">
         <v>44300</v>
       </c>
-      <c r="B25" s="12" t="str">
+      <c r="B26" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(水)</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C26" s="6">
         <f t="shared" si="0"/>
         <v>50996</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D26" s="6">
         <v>9569</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E26" s="6">
         <v>41427</v>
-      </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A26" s="10">
-        <v>44299</v>
-      </c>
-      <c r="B26" s="12" t="str">
-        <f t="shared" ref="B26:B27" si="2">"("&amp;TEXT(A26,"aaa")&amp;")"</f>
-        <v>(火)</v>
-      </c>
-      <c r="C26" s="6">
-        <f t="shared" ref="C26:C27" si="3">SUM(D26:E26)</f>
-        <v>53986</v>
-      </c>
-      <c r="D26" s="6">
-        <v>13896</v>
-      </c>
-      <c r="E26" s="6">
-        <v>40090</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="10">
+        <v>44299</v>
+      </c>
+      <c r="B27" s="12" t="str">
+        <f t="shared" ref="B27:B28" si="2">"("&amp;TEXT(A27,"aaa")&amp;")"</f>
+        <v>(火)</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" ref="C27:C28" si="3">SUM(D27:E27)</f>
+        <v>53986</v>
+      </c>
+      <c r="D27" s="6">
+        <v>13896</v>
+      </c>
+      <c r="E27" s="6">
+        <v>40090</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28" s="10">
         <v>44298</v>
       </c>
-      <c r="B27" s="12" t="str">
+      <c r="B28" s="12" t="str">
         <f t="shared" si="2"/>
         <v>(月)</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C28" s="6">
         <f t="shared" si="3"/>
         <v>96936</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D28" s="6">
         <v>26850</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E28" s="6">
         <v>70086</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A28" s="8"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="7"/>
       <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="5"/>
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
         <v>6</v>
       </c>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A32" s="1" t="s">
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
         <v>3</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F34" s="5"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A36" s="1"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F35" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A37" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Flat: latest data (2021-05-21T06:21:50.680Z) {   "date": "2021-05-21T06:21:50.680Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 56,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t> 内１回目</t>
   </si>
@@ -254,7 +254,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（5月19日時点）</t>
+    <t>（5月20日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -699,7 +699,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -747,557 +747,577 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="6">
-        <f t="shared" ref="C4:C26" si="0">SUM(D4:E4)</f>
-        <v>5998833</v>
+        <f t="shared" ref="C4:C27" si="0">SUM(D4:E4)</f>
+        <v>6189366</v>
       </c>
       <c r="D4" s="6">
-        <v>3784071</v>
+        <v>3865493</v>
       </c>
       <c r="E4" s="6">
-        <v>2214762</v>
+        <v>2323873</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D5" s="6">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E5" s="6">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D6" s="6">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E6" s="6">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="13">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D7" s="6">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E7" s="6">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="13">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D8" s="6">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E8" s="6">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="13">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D9" s="6">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E9" s="6">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="13">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D10" s="6">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E10" s="6">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D11" s="6">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E11" s="6">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="13">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D12" s="6">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E12" s="6">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="13">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D13" s="6">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E13" s="6">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="13">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D14" s="6">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E14" s="6">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="13">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D15" s="6">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E15" s="6">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="13">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D16" s="6">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E16" s="6">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="13">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D17" s="6">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E17" s="6">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="13">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D18" s="6">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E18" s="6">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="13">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D19" s="6">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E19" s="6">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="13">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D20" s="6">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E20" s="6">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="13">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D21" s="6">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E21" s="6">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="13">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D22" s="6">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E22" s="6">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23" s="15">
-        <v>44305</v>
-      </c>
-      <c r="B23" s="12" t="str">
-        <f t="shared" ref="B23:B26" si="1">"("&amp;TEXT(A23,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A23" s="13">
+        <v>44306</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D23" s="6">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E23" s="6">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A24" s="13">
+      <c r="A24" s="15">
+        <v>44305</v>
+      </c>
+      <c r="B24" s="12" t="str">
+        <f t="shared" ref="B24:B27" si="1">"("&amp;TEXT(A24,"aaa")&amp;")"</f>
+        <v>(月)</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" si="0"/>
+        <v>119032</v>
+      </c>
+      <c r="D24" s="6">
+        <v>64725</v>
+      </c>
+      <c r="E24" s="6">
+        <v>54307</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A25" s="13">
         <v>44302</v>
       </c>
-      <c r="B24" s="12" t="str">
+      <c r="B25" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(金)</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C25" s="6">
         <f t="shared" si="0"/>
         <v>69687</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D25" s="6">
         <v>29696</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E25" s="6">
         <v>39991</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A25" s="13">
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26" s="13">
         <v>44301</v>
       </c>
-      <c r="B25" s="12" t="str">
+      <c r="B26" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(木)</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C26" s="6">
         <f t="shared" si="0"/>
         <v>52620</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D26" s="6">
         <v>16637</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E26" s="6">
         <v>35983</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A26" s="13">
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A27" s="13">
         <v>44300</v>
       </c>
-      <c r="B26" s="12" t="str">
+      <c r="B27" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(水)</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C27" s="6">
         <f t="shared" si="0"/>
         <v>50996</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D27" s="6">
         <v>9569</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E27" s="6">
         <v>41427</v>
-      </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A27" s="10">
-        <v>44299</v>
-      </c>
-      <c r="B27" s="12" t="str">
-        <f t="shared" ref="B27:B28" si="2">"("&amp;TEXT(A27,"aaa")&amp;")"</f>
-        <v>(火)</v>
-      </c>
-      <c r="C27" s="6">
-        <f t="shared" ref="C27:C28" si="3">SUM(D27:E27)</f>
-        <v>53986</v>
-      </c>
-      <c r="D27" s="6">
-        <v>13896</v>
-      </c>
-      <c r="E27" s="6">
-        <v>40090</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" s="10">
+        <v>44299</v>
+      </c>
+      <c r="B28" s="12" t="str">
+        <f t="shared" ref="B28:B29" si="2">"("&amp;TEXT(A28,"aaa")&amp;")"</f>
+        <v>(火)</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" ref="C28:C29" si="3">SUM(D28:E28)</f>
+        <v>53986</v>
+      </c>
+      <c r="D28" s="6">
+        <v>13896</v>
+      </c>
+      <c r="E28" s="6">
+        <v>40090</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29" s="10">
         <v>44298</v>
       </c>
-      <c r="B28" s="12" t="str">
+      <c r="B29" s="12" t="str">
         <f t="shared" si="2"/>
         <v>(月)</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C29" s="6">
         <f t="shared" si="3"/>
         <v>96936</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D29" s="6">
         <v>26850</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E29" s="6">
         <v>70086</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A29" s="8"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="7"/>
       <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A31" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" s="1" t="s">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F35" s="5"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A37" s="1"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F36" s="5"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A38" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Flat: latest data (2021-05-24T06:24:07.072Z) {   "date": "2021-05-24T06:24:07.072Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 44,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t> 内１回目</t>
   </si>
@@ -254,7 +254,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（5月20日時点）</t>
+    <t>（5月21日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -699,7 +699,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -747,577 +747,597 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="6">
-        <f t="shared" ref="C4:C27" si="0">SUM(D4:E4)</f>
-        <v>6189366</v>
+        <f t="shared" ref="C4:C28" si="0">SUM(D4:E4)</f>
+        <v>6438387</v>
       </c>
       <c r="D4" s="6">
-        <v>3865493</v>
+        <v>3965411</v>
       </c>
       <c r="E4" s="6">
-        <v>2323873</v>
+        <v>2472976</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D5" s="6">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E5" s="6">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D6" s="6">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E6" s="6">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="13">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D7" s="6">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E7" s="6">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="13">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D8" s="6">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E8" s="6">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="13">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D9" s="6">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E9" s="6">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="13">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D10" s="6">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E10" s="6">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D11" s="6">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E11" s="6">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="13">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D12" s="6">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E12" s="6">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="13">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D13" s="6">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E13" s="6">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="13">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D14" s="6">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E14" s="6">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="13">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D15" s="6">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E15" s="6">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="13">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D16" s="6">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E16" s="6">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="13">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D17" s="6">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E17" s="6">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="13">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D18" s="6">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E18" s="6">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="13">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D19" s="6">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E19" s="6">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="13">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D20" s="6">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E20" s="6">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="13">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D21" s="6">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E21" s="6">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="13">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D22" s="6">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E22" s="6">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="13">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D23" s="6">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E23" s="6">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A24" s="15">
-        <v>44305</v>
-      </c>
-      <c r="B24" s="12" t="str">
-        <f t="shared" ref="B24:B27" si="1">"("&amp;TEXT(A24,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A24" s="13">
+        <v>44306</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C24" s="6">
         <f t="shared" si="0"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D24" s="6">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E24" s="6">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A25" s="13">
+      <c r="A25" s="15">
+        <v>44305</v>
+      </c>
+      <c r="B25" s="12" t="str">
+        <f t="shared" ref="B25:B28" si="1">"("&amp;TEXT(A25,"aaa")&amp;")"</f>
+        <v>(月)</v>
+      </c>
+      <c r="C25" s="6">
+        <f t="shared" si="0"/>
+        <v>119032</v>
+      </c>
+      <c r="D25" s="6">
+        <v>64725</v>
+      </c>
+      <c r="E25" s="6">
+        <v>54307</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26" s="13">
         <v>44302</v>
       </c>
-      <c r="B25" s="12" t="str">
+      <c r="B26" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(金)</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C26" s="6">
         <f t="shared" si="0"/>
         <v>69687</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D26" s="6">
         <v>29696</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E26" s="6">
         <v>39991</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A26" s="13">
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A27" s="13">
         <v>44301</v>
       </c>
-      <c r="B26" s="12" t="str">
+      <c r="B27" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(木)</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C27" s="6">
         <f t="shared" si="0"/>
         <v>52620</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D27" s="6">
         <v>16637</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E27" s="6">
         <v>35983</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A27" s="13">
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28" s="13">
         <v>44300</v>
       </c>
-      <c r="B27" s="12" t="str">
+      <c r="B28" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(水)</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C28" s="6">
         <f t="shared" si="0"/>
         <v>50996</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D28" s="6">
         <v>9569</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E28" s="6">
         <v>41427</v>
-      </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A28" s="10">
-        <v>44299</v>
-      </c>
-      <c r="B28" s="12" t="str">
-        <f t="shared" ref="B28:B29" si="2">"("&amp;TEXT(A28,"aaa")&amp;")"</f>
-        <v>(火)</v>
-      </c>
-      <c r="C28" s="6">
-        <f t="shared" ref="C28:C29" si="3">SUM(D28:E28)</f>
-        <v>53986</v>
-      </c>
-      <c r="D28" s="6">
-        <v>13896</v>
-      </c>
-      <c r="E28" s="6">
-        <v>40090</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" s="10">
+        <v>44299</v>
+      </c>
+      <c r="B29" s="12" t="str">
+        <f t="shared" ref="B29:B30" si="2">"("&amp;TEXT(A29,"aaa")&amp;")"</f>
+        <v>(火)</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" ref="C29:C30" si="3">SUM(D29:E29)</f>
+        <v>53986</v>
+      </c>
+      <c r="D29" s="6">
+        <v>13896</v>
+      </c>
+      <c r="E29" s="6">
+        <v>40090</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30" s="10">
         <v>44298</v>
       </c>
-      <c r="B29" s="12" t="str">
+      <c r="B30" s="12" t="str">
         <f t="shared" si="2"/>
         <v>(月)</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C30" s="6">
         <f t="shared" si="3"/>
         <v>96936</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D30" s="6">
         <v>26850</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E30" s="6">
         <v>70086</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A30" s="8"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="7"/>
       <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A32" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="5"/>
       <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A34" s="1" t="s">
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
         <v>3</v>
       </c>
-      <c r="F35" s="7"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F36" s="5"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A38" s="1"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F37" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A39" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Flat: latest data (2021-05-25T06:31:42.998Z) {   "date": "2021-05-25T06:31:42.998Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 60,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t> 内１回目</t>
   </si>
@@ -254,7 +254,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（5月21日時点）</t>
+    <t>（5月24日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -699,7 +699,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -747,597 +747,617 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="6">
-        <f t="shared" ref="C4:C28" si="0">SUM(D4:E4)</f>
-        <v>6438387</v>
+        <f t="shared" ref="C4:C29" si="0">SUM(D4:E4)</f>
+        <v>6768976</v>
       </c>
       <c r="D4" s="6">
-        <v>3965411</v>
+        <v>4102171</v>
       </c>
       <c r="E4" s="6">
-        <v>2472976</v>
+        <v>2666805</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>249021</v>
+        <v>330589</v>
       </c>
       <c r="D5" s="6">
-        <v>99918</v>
+        <v>136760</v>
       </c>
       <c r="E5" s="6">
-        <v>149103</v>
+        <v>193829</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D6" s="6">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E6" s="6">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="13">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D7" s="6">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E7" s="6">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="13">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D8" s="6">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E8" s="6">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="13">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D9" s="6">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E9" s="6">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="13">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D10" s="6">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E10" s="6">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D11" s="6">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E11" s="6">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="13">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D12" s="6">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E12" s="6">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="13">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D13" s="6">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E13" s="6">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="13">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D14" s="6">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E14" s="6">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="13">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D15" s="6">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E15" s="6">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="13">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D16" s="6">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E16" s="6">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="13">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D17" s="6">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E17" s="6">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="13">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D18" s="6">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E18" s="6">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="13">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D19" s="6">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E19" s="6">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="13">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D20" s="6">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E20" s="6">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="13">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D21" s="6">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E21" s="6">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="13">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D22" s="6">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E22" s="6">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="13">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D23" s="6">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E23" s="6">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="13">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C24" s="6">
         <f t="shared" si="0"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D24" s="6">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E24" s="6">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A25" s="15">
-        <v>44305</v>
-      </c>
-      <c r="B25" s="12" t="str">
-        <f t="shared" ref="B25:B28" si="1">"("&amp;TEXT(A25,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A25" s="13">
+        <v>44306</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D25" s="6">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E25" s="6">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A26" s="13">
+      <c r="A26" s="15">
+        <v>44305</v>
+      </c>
+      <c r="B26" s="12" t="str">
+        <f t="shared" ref="B26:B29" si="1">"("&amp;TEXT(A26,"aaa")&amp;")"</f>
+        <v>(月)</v>
+      </c>
+      <c r="C26" s="6">
+        <f t="shared" si="0"/>
+        <v>119032</v>
+      </c>
+      <c r="D26" s="6">
+        <v>64725</v>
+      </c>
+      <c r="E26" s="6">
+        <v>54307</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A27" s="13">
         <v>44302</v>
       </c>
-      <c r="B26" s="12" t="str">
+      <c r="B27" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(金)</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C27" s="6">
         <f t="shared" si="0"/>
         <v>69687</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D27" s="6">
         <v>29696</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E27" s="6">
         <v>39991</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A27" s="13">
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28" s="13">
         <v>44301</v>
       </c>
-      <c r="B27" s="12" t="str">
+      <c r="B28" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(木)</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C28" s="6">
         <f t="shared" si="0"/>
         <v>52620</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D28" s="6">
         <v>16637</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E28" s="6">
         <v>35983</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A28" s="13">
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29" s="13">
         <v>44300</v>
       </c>
-      <c r="B28" s="12" t="str">
+      <c r="B29" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(水)</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C29" s="6">
         <f t="shared" si="0"/>
         <v>50996</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D29" s="6">
         <v>9569</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E29" s="6">
         <v>41427</v>
-      </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A29" s="10">
-        <v>44299</v>
-      </c>
-      <c r="B29" s="12" t="str">
-        <f t="shared" ref="B29:B30" si="2">"("&amp;TEXT(A29,"aaa")&amp;")"</f>
-        <v>(火)</v>
-      </c>
-      <c r="C29" s="6">
-        <f t="shared" ref="C29:C30" si="3">SUM(D29:E29)</f>
-        <v>53986</v>
-      </c>
-      <c r="D29" s="6">
-        <v>13896</v>
-      </c>
-      <c r="E29" s="6">
-        <v>40090</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" s="10">
+        <v>44299</v>
+      </c>
+      <c r="B30" s="12" t="str">
+        <f t="shared" ref="B30:B31" si="2">"("&amp;TEXT(A30,"aaa")&amp;")"</f>
+        <v>(火)</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" ref="C30:C31" si="3">SUM(D30:E30)</f>
+        <v>53986</v>
+      </c>
+      <c r="D30" s="6">
+        <v>13896</v>
+      </c>
+      <c r="E30" s="6">
+        <v>40090</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A31" s="10">
         <v>44298</v>
       </c>
-      <c r="B30" s="12" t="str">
+      <c r="B31" s="12" t="str">
         <f t="shared" si="2"/>
         <v>(月)</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C31" s="6">
         <f t="shared" si="3"/>
         <v>96936</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D31" s="6">
         <v>26850</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E31" s="6">
         <v>70086</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A31" s="8"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="7"/>
       <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A33" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="5"/>
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A35" s="1" t="s">
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
         <v>3</v>
       </c>
-      <c r="F36" s="7"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F37" s="5"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A39" s="1"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F38" s="5"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A40" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Flat: latest data (2021-05-26T06:39:50.646Z) {   "date": "2021-05-26T06:39:50.646Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 58,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t> 内１回目</t>
   </si>
@@ -254,7 +254,11 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（5月24日時点）</t>
+    <t>(火)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>（5月25日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -699,7 +703,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -719,7 +723,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E2" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
@@ -747,617 +751,637 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="6">
-        <f t="shared" ref="C4:C29" si="0">SUM(D4:E4)</f>
-        <v>6768976</v>
+        <f t="shared" ref="C4:C30" si="0">SUM(D4:E4)</f>
+        <v>6908628</v>
       </c>
       <c r="D4" s="6">
-        <v>4102171</v>
+        <v>4189761</v>
       </c>
       <c r="E4" s="6">
-        <v>2666805</v>
+        <v>2718867</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
-        <v>44340</v>
+        <v>44341</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>330589</v>
+        <v>139652</v>
       </c>
       <c r="D5" s="6">
-        <v>136760</v>
+        <v>87590</v>
       </c>
       <c r="E5" s="6">
-        <v>193829</v>
+        <v>52062</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
-        <v>249021</v>
+        <v>330589</v>
       </c>
       <c r="D6" s="6">
-        <v>99918</v>
+        <v>136760</v>
       </c>
       <c r="E6" s="6">
-        <v>149103</v>
+        <v>193829</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="13">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D7" s="6">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E7" s="6">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="13">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D8" s="6">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E8" s="6">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="13">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D9" s="6">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E9" s="6">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="13">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D10" s="6">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E10" s="6">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D11" s="6">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E11" s="6">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="13">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D12" s="6">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E12" s="6">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="13">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D13" s="6">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E13" s="6">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="13">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D14" s="6">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E14" s="6">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="13">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D15" s="6">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E15" s="6">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="13">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D16" s="6">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E16" s="6">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="13">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D17" s="6">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E17" s="6">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="13">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D18" s="6">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E18" s="6">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="13">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D19" s="6">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E19" s="6">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="13">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D20" s="6">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E20" s="6">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="13">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D21" s="6">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E21" s="6">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="13">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D22" s="6">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E22" s="6">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="13">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D23" s="6">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E23" s="6">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="13">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C24" s="6">
         <f t="shared" si="0"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D24" s="6">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E24" s="6">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="13">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D25" s="6">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E25" s="6">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A26" s="15">
-        <v>44305</v>
-      </c>
-      <c r="B26" s="12" t="str">
-        <f t="shared" ref="B26:B29" si="1">"("&amp;TEXT(A26,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A26" s="13">
+        <v>44306</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C26" s="6">
         <f t="shared" si="0"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D26" s="6">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E26" s="6">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A27" s="13">
+      <c r="A27" s="15">
+        <v>44305</v>
+      </c>
+      <c r="B27" s="12" t="str">
+        <f t="shared" ref="B27:B30" si="1">"("&amp;TEXT(A27,"aaa")&amp;")"</f>
+        <v>(月)</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" si="0"/>
+        <v>119032</v>
+      </c>
+      <c r="D27" s="6">
+        <v>64725</v>
+      </c>
+      <c r="E27" s="6">
+        <v>54307</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28" s="13">
         <v>44302</v>
       </c>
-      <c r="B27" s="12" t="str">
+      <c r="B28" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(金)</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C28" s="6">
         <f t="shared" si="0"/>
         <v>69687</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D28" s="6">
         <v>29696</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E28" s="6">
         <v>39991</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A28" s="13">
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29" s="13">
         <v>44301</v>
       </c>
-      <c r="B28" s="12" t="str">
+      <c r="B29" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(木)</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C29" s="6">
         <f t="shared" si="0"/>
         <v>52620</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D29" s="6">
         <v>16637</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E29" s="6">
         <v>35983</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A29" s="13">
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30" s="13">
         <v>44300</v>
       </c>
-      <c r="B29" s="12" t="str">
+      <c r="B30" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(水)</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C30" s="6">
         <f t="shared" si="0"/>
         <v>50996</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D30" s="6">
         <v>9569</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E30" s="6">
         <v>41427</v>
-      </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A30" s="10">
-        <v>44299</v>
-      </c>
-      <c r="B30" s="12" t="str">
-        <f t="shared" ref="B30:B31" si="2">"("&amp;TEXT(A30,"aaa")&amp;")"</f>
-        <v>(火)</v>
-      </c>
-      <c r="C30" s="6">
-        <f t="shared" ref="C30:C31" si="3">SUM(D30:E30)</f>
-        <v>53986</v>
-      </c>
-      <c r="D30" s="6">
-        <v>13896</v>
-      </c>
-      <c r="E30" s="6">
-        <v>40090</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" s="10">
+        <v>44299</v>
+      </c>
+      <c r="B31" s="12" t="str">
+        <f t="shared" ref="B31:B32" si="2">"("&amp;TEXT(A31,"aaa")&amp;")"</f>
+        <v>(火)</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" ref="C31:C32" si="3">SUM(D31:E31)</f>
+        <v>53986</v>
+      </c>
+      <c r="D31" s="6">
+        <v>13896</v>
+      </c>
+      <c r="E31" s="6">
+        <v>40090</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A32" s="10">
         <v>44298</v>
       </c>
-      <c r="B31" s="12" t="str">
+      <c r="B32" s="12" t="str">
         <f t="shared" si="2"/>
         <v>(月)</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C32" s="6">
         <f t="shared" si="3"/>
         <v>96936</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D32" s="6">
         <v>26850</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E32" s="6">
         <v>70086</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A32" s="8"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="7"/>
       <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="5"/>
       <c r="F34" s="7"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
         <v>6</v>
       </c>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A36" s="1" t="s">
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
         <v>3</v>
       </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F38" s="5"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A40" s="1"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F39" s="5"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A41" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Flat: latest data (2021-05-27T06:45:44.886Z) {   "date": "2021-05-27T06:45:44.886Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 46,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t> 内１回目</t>
   </si>
@@ -258,7 +258,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（5月25日時点）</t>
+    <t>（5月26日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -703,7 +703,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -751,637 +751,657 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="6">
-        <f t="shared" ref="C4:C30" si="0">SUM(D4:E4)</f>
-        <v>6908628</v>
+        <f t="shared" ref="C4:C31" si="0">SUM(D4:E4)</f>
+        <v>7051217</v>
       </c>
       <c r="D4" s="6">
-        <v>4189761</v>
+        <v>4283176</v>
       </c>
       <c r="E4" s="6">
-        <v>2718867</v>
+        <v>2768041</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
-        <v>44341</v>
+        <v>44342</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>139652</v>
+        <v>142589</v>
       </c>
       <c r="D5" s="6">
-        <v>87590</v>
+        <v>93415</v>
       </c>
       <c r="E5" s="6">
-        <v>52062</v>
+        <v>49174</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
-        <v>44340</v>
+        <v>44341</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
-        <v>330589</v>
+        <v>139652</v>
       </c>
       <c r="D6" s="6">
-        <v>136760</v>
+        <v>87590</v>
       </c>
       <c r="E6" s="6">
-        <v>193829</v>
+        <v>52062</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="13">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>249021</v>
+        <v>330589</v>
       </c>
       <c r="D7" s="6">
-        <v>99918</v>
+        <v>136760</v>
       </c>
       <c r="E7" s="6">
-        <v>149103</v>
+        <v>193829</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="13">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D8" s="6">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E8" s="6">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="13">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D9" s="6">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E9" s="6">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="13">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D10" s="6">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E10" s="6">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D11" s="6">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E11" s="6">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="13">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D12" s="6">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E12" s="6">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="13">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D13" s="6">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E13" s="6">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="13">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D14" s="6">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E14" s="6">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="13">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D15" s="6">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E15" s="6">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="13">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D16" s="6">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E16" s="6">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="13">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D17" s="6">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E17" s="6">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="13">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D18" s="6">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E18" s="6">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="13">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D19" s="6">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E19" s="6">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="13">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D20" s="6">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E20" s="6">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="13">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D21" s="6">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E21" s="6">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="13">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D22" s="6">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E22" s="6">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="13">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D23" s="6">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E23" s="6">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="13">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" s="6">
         <f t="shared" si="0"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D24" s="6">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E24" s="6">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="13">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D25" s="6">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E25" s="6">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="13">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C26" s="6">
         <f t="shared" si="0"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D26" s="6">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E26" s="6">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A27" s="15">
-        <v>44305</v>
-      </c>
-      <c r="B27" s="12" t="str">
-        <f t="shared" ref="B27:B30" si="1">"("&amp;TEXT(A27,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A27" s="13">
+        <v>44306</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C27" s="6">
         <f t="shared" si="0"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D27" s="6">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E27" s="6">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A28" s="13">
+      <c r="A28" s="15">
+        <v>44305</v>
+      </c>
+      <c r="B28" s="12" t="str">
+        <f t="shared" ref="B28:B31" si="1">"("&amp;TEXT(A28,"aaa")&amp;")"</f>
+        <v>(月)</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="0"/>
+        <v>119032</v>
+      </c>
+      <c r="D28" s="6">
+        <v>64725</v>
+      </c>
+      <c r="E28" s="6">
+        <v>54307</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29" s="13">
         <v>44302</v>
       </c>
-      <c r="B28" s="12" t="str">
+      <c r="B29" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(金)</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C29" s="6">
         <f t="shared" si="0"/>
         <v>69687</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D29" s="6">
         <v>29696</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E29" s="6">
         <v>39991</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A29" s="13">
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30" s="13">
         <v>44301</v>
       </c>
-      <c r="B29" s="12" t="str">
+      <c r="B30" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(木)</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C30" s="6">
         <f t="shared" si="0"/>
         <v>52620</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D30" s="6">
         <v>16637</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E30" s="6">
         <v>35983</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A30" s="13">
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A31" s="13">
         <v>44300</v>
       </c>
-      <c r="B30" s="12" t="str">
+      <c r="B31" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(水)</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C31" s="6">
         <f t="shared" si="0"/>
         <v>50996</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D31" s="6">
         <v>9569</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E31" s="6">
         <v>41427</v>
-      </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A31" s="10">
-        <v>44299</v>
-      </c>
-      <c r="B31" s="12" t="str">
-        <f t="shared" ref="B31:B32" si="2">"("&amp;TEXT(A31,"aaa")&amp;")"</f>
-        <v>(火)</v>
-      </c>
-      <c r="C31" s="6">
-        <f t="shared" ref="C31:C32" si="3">SUM(D31:E31)</f>
-        <v>53986</v>
-      </c>
-      <c r="D31" s="6">
-        <v>13896</v>
-      </c>
-      <c r="E31" s="6">
-        <v>40090</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" s="10">
+        <v>44299</v>
+      </c>
+      <c r="B32" s="12" t="str">
+        <f t="shared" ref="B32:B33" si="2">"("&amp;TEXT(A32,"aaa")&amp;")"</f>
+        <v>(火)</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" ref="C32:C33" si="3">SUM(D32:E32)</f>
+        <v>53986</v>
+      </c>
+      <c r="D32" s="6">
+        <v>13896</v>
+      </c>
+      <c r="E32" s="6">
+        <v>40090</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A33" s="10">
         <v>44298</v>
       </c>
-      <c r="B32" s="12" t="str">
+      <c r="B33" s="12" t="str">
         <f t="shared" si="2"/>
         <v>(月)</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C33" s="6">
         <f t="shared" si="3"/>
         <v>96936</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D33" s="6">
         <v>26850</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E33" s="6">
         <v>70086</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" s="8"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="7"/>
       <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A35" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="5"/>
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
         <v>6</v>
       </c>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A37" s="1" t="s">
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
         <v>3</v>
       </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F39" s="5"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A41" s="1"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F40" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A42" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Flat: latest data (2021-05-28T07:05:19.105Z) {   "date": "2021-05-28T07:05:19.105Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 48,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t> 内１回目</t>
   </si>
@@ -258,7 +258,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（5月26日時点）</t>
+    <t>（5月27日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -703,7 +703,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -751,657 +751,677 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="6">
-        <f t="shared" ref="C4:C31" si="0">SUM(D4:E4)</f>
-        <v>7051217</v>
+        <f t="shared" ref="C4:C32" si="0">SUM(D4:E4)</f>
+        <v>7196366</v>
       </c>
       <c r="D4" s="6">
-        <v>4283176</v>
+        <v>4367433</v>
       </c>
       <c r="E4" s="6">
-        <v>2768041</v>
+        <v>2828933</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
-        <v>44342</v>
+        <v>44343</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>142589</v>
+        <v>145149</v>
       </c>
       <c r="D5" s="6">
-        <v>93415</v>
+        <v>84257</v>
       </c>
       <c r="E5" s="6">
-        <v>49174</v>
+        <v>60892</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
-        <v>44341</v>
+        <v>44342</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
-        <v>139652</v>
+        <v>142589</v>
       </c>
       <c r="D6" s="6">
-        <v>87590</v>
+        <v>93415</v>
       </c>
       <c r="E6" s="6">
-        <v>52062</v>
+        <v>49174</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="13">
-        <v>44340</v>
+        <v>44341</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>330589</v>
+        <v>139652</v>
       </c>
       <c r="D7" s="6">
-        <v>136760</v>
+        <v>87590</v>
       </c>
       <c r="E7" s="6">
-        <v>193829</v>
+        <v>52062</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="13">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>249021</v>
+        <v>330589</v>
       </c>
       <c r="D8" s="6">
-        <v>99918</v>
+        <v>136760</v>
       </c>
       <c r="E8" s="6">
-        <v>149103</v>
+        <v>193829</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="13">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D9" s="6">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E9" s="6">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="13">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D10" s="6">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E10" s="6">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D11" s="6">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E11" s="6">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="13">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D12" s="6">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E12" s="6">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="13">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D13" s="6">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E13" s="6">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="13">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D14" s="6">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E14" s="6">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="13">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D15" s="6">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E15" s="6">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="13">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D16" s="6">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E16" s="6">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="13">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D17" s="6">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E17" s="6">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="13">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D18" s="6">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E18" s="6">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="13">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D19" s="6">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E19" s="6">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="13">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D20" s="6">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E20" s="6">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="13">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D21" s="6">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E21" s="6">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="13">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D22" s="6">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E22" s="6">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="13">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D23" s="6">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E23" s="6">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="13">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C24" s="6">
         <f t="shared" si="0"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D24" s="6">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E24" s="6">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="13">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D25" s="6">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E25" s="6">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="13">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C26" s="6">
         <f t="shared" si="0"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D26" s="6">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E26" s="6">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="13">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C27" s="6">
         <f t="shared" si="0"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D27" s="6">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E27" s="6">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A28" s="15">
-        <v>44305</v>
-      </c>
-      <c r="B28" s="12" t="str">
-        <f t="shared" ref="B28:B31" si="1">"("&amp;TEXT(A28,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A28" s="13">
+        <v>44306</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C28" s="6">
         <f t="shared" si="0"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D28" s="6">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E28" s="6">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A29" s="13">
+      <c r="A29" s="15">
+        <v>44305</v>
+      </c>
+      <c r="B29" s="12" t="str">
+        <f t="shared" ref="B29:B32" si="1">"("&amp;TEXT(A29,"aaa")&amp;")"</f>
+        <v>(月)</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" si="0"/>
+        <v>119032</v>
+      </c>
+      <c r="D29" s="6">
+        <v>64725</v>
+      </c>
+      <c r="E29" s="6">
+        <v>54307</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30" s="13">
         <v>44302</v>
       </c>
-      <c r="B29" s="12" t="str">
+      <c r="B30" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(金)</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C30" s="6">
         <f t="shared" si="0"/>
         <v>69687</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D30" s="6">
         <v>29696</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E30" s="6">
         <v>39991</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A30" s="13">
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A31" s="13">
         <v>44301</v>
       </c>
-      <c r="B30" s="12" t="str">
+      <c r="B31" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(木)</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C31" s="6">
         <f t="shared" si="0"/>
         <v>52620</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D31" s="6">
         <v>16637</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E31" s="6">
         <v>35983</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A31" s="13">
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A32" s="13">
         <v>44300</v>
       </c>
-      <c r="B31" s="12" t="str">
+      <c r="B32" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(水)</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C32" s="6">
         <f t="shared" si="0"/>
         <v>50996</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D32" s="6">
         <v>9569</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E32" s="6">
         <v>41427</v>
-      </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A32" s="10">
-        <v>44299</v>
-      </c>
-      <c r="B32" s="12" t="str">
-        <f t="shared" ref="B32:B33" si="2">"("&amp;TEXT(A32,"aaa")&amp;")"</f>
-        <v>(火)</v>
-      </c>
-      <c r="C32" s="6">
-        <f t="shared" ref="C32:C33" si="3">SUM(D32:E32)</f>
-        <v>53986</v>
-      </c>
-      <c r="D32" s="6">
-        <v>13896</v>
-      </c>
-      <c r="E32" s="6">
-        <v>40090</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="10">
+        <v>44299</v>
+      </c>
+      <c r="B33" s="12" t="str">
+        <f t="shared" ref="B33:B34" si="2">"("&amp;TEXT(A33,"aaa")&amp;")"</f>
+        <v>(火)</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" ref="C33:C34" si="3">SUM(D33:E33)</f>
+        <v>53986</v>
+      </c>
+      <c r="D33" s="6">
+        <v>13896</v>
+      </c>
+      <c r="E33" s="6">
+        <v>40090</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" s="10">
         <v>44298</v>
       </c>
-      <c r="B33" s="12" t="str">
+      <c r="B34" s="12" t="str">
         <f t="shared" si="2"/>
         <v>(月)</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C34" s="6">
         <f t="shared" si="3"/>
         <v>96936</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <v>26850</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E34" s="6">
         <v>70086</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="7"/>
       <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="8"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A36" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="5"/>
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
         <v>6</v>
       </c>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A38" s="1" t="s">
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F38" s="7"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
         <v>3</v>
       </c>
-      <c r="F39" s="7"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F40" s="5"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A42" s="1"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F41" s="5"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A43" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Flat: latest data (2021-06-01T07:49:54.213Z) {   "date": "2021-06-01T07:49:54.213Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 106,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t> 内１回目</t>
   </si>
@@ -258,7 +258,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（5月27日時点）</t>
+    <t>（5月31日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -703,7 +703,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -751,677 +751,717 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="6">
-        <f t="shared" ref="C4:C32" si="0">SUM(D4:E4)</f>
-        <v>7196366</v>
+        <f t="shared" ref="C4:C34" si="0">SUM(D4:E4)</f>
+        <v>7634137</v>
       </c>
       <c r="D4" s="6">
-        <v>4367433</v>
+        <v>4587179</v>
       </c>
       <c r="E4" s="6">
-        <v>2828933</v>
+        <v>3046958</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
-        <v>44343</v>
+        <v>44347</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>145149</v>
+        <v>273255</v>
       </c>
       <c r="D5" s="6">
-        <v>84257</v>
+        <v>132005</v>
       </c>
       <c r="E5" s="6">
-        <v>60892</v>
+        <v>141250</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
-        <v>44342</v>
+        <v>44344</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
-        <v>142589</v>
+        <v>164516</v>
       </c>
       <c r="D6" s="6">
-        <v>93415</v>
+        <v>87741</v>
       </c>
       <c r="E6" s="6">
-        <v>49174</v>
+        <v>76775</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="13">
-        <v>44341</v>
+        <v>44343</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>139652</v>
+        <v>145149</v>
       </c>
       <c r="D7" s="6">
-        <v>87590</v>
+        <v>84257</v>
       </c>
       <c r="E7" s="6">
-        <v>52062</v>
+        <v>60892</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="13">
-        <v>44340</v>
+        <v>44342</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>330589</v>
+        <v>142589</v>
       </c>
       <c r="D8" s="6">
-        <v>136760</v>
+        <v>93415</v>
       </c>
       <c r="E8" s="6">
-        <v>193829</v>
+        <v>49174</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="13">
-        <v>44337</v>
+        <v>44341</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>249021</v>
+        <v>139652</v>
       </c>
       <c r="D9" s="6">
-        <v>99918</v>
+        <v>87590</v>
       </c>
       <c r="E9" s="6">
-        <v>149103</v>
+        <v>52062</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="13">
-        <v>44336</v>
+        <v>44340</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>190533</v>
+        <v>330589</v>
       </c>
       <c r="D10" s="6">
-        <v>81422</v>
+        <v>136760</v>
       </c>
       <c r="E10" s="6">
-        <v>109111</v>
+        <v>193829</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
-        <v>44335</v>
+        <v>44337</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>267866</v>
+        <v>249021</v>
       </c>
       <c r="D11" s="6">
-        <v>88163</v>
+        <v>99918</v>
       </c>
       <c r="E11" s="6">
-        <v>179703</v>
+        <v>149103</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="13">
-        <v>44334</v>
+        <v>44336</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>250244</v>
+        <v>190533</v>
       </c>
       <c r="D12" s="6">
-        <v>94577</v>
+        <v>81422</v>
       </c>
       <c r="E12" s="6">
-        <v>155667</v>
+        <v>109111</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="13">
-        <v>44333</v>
+        <v>44335</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>349566</v>
+        <v>267866</v>
       </c>
       <c r="D13" s="6">
-        <v>133843</v>
+        <v>88163</v>
       </c>
       <c r="E13" s="6">
-        <v>215723</v>
+        <v>179703</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="13">
-        <v>44330</v>
+        <v>44334</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>242878</v>
+        <v>250244</v>
       </c>
       <c r="D14" s="6">
-        <v>99493</v>
+        <v>94577</v>
       </c>
       <c r="E14" s="6">
-        <v>143385</v>
+        <v>155667</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="13">
-        <v>44329</v>
+        <v>44333</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>219139</v>
+        <v>349566</v>
       </c>
       <c r="D15" s="6">
-        <v>93429</v>
+        <v>133843</v>
       </c>
       <c r="E15" s="6">
-        <v>125710</v>
+        <v>215723</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="13">
-        <v>44328</v>
+        <v>44330</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>181720</v>
+        <v>242878</v>
       </c>
       <c r="D16" s="6">
-        <v>82959</v>
+        <v>99493</v>
       </c>
       <c r="E16" s="6">
-        <v>98761</v>
+        <v>143385</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="13">
-        <v>44327</v>
+        <v>44329</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>168738</v>
+        <v>219139</v>
       </c>
       <c r="D17" s="6">
-        <v>90287</v>
+        <v>93429</v>
       </c>
       <c r="E17" s="6">
-        <v>78451</v>
+        <v>125710</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="13">
-        <v>44326</v>
+        <v>44328</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>223504</v>
+        <v>181720</v>
       </c>
       <c r="D18" s="6">
-        <v>155255</v>
+        <v>82959</v>
       </c>
       <c r="E18" s="6">
-        <v>68249</v>
+        <v>98761</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="13">
-        <v>44323</v>
+        <v>44327</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>140344</v>
+        <v>168738</v>
       </c>
       <c r="D19" s="6">
-        <v>97165</v>
+        <v>90287</v>
       </c>
       <c r="E19" s="6">
-        <v>43179</v>
+        <v>78451</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="13">
-        <v>44322</v>
+        <v>44326</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>331914</v>
+        <v>223504</v>
       </c>
       <c r="D20" s="6">
-        <v>268978</v>
+        <v>155255</v>
       </c>
       <c r="E20" s="6">
-        <v>62936</v>
+        <v>68249</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="13">
-        <v>44316</v>
+        <v>44323</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>274907</v>
+        <v>140344</v>
       </c>
       <c r="D21" s="6">
-        <v>227667</v>
+        <v>97165</v>
       </c>
       <c r="E21" s="6">
-        <v>47240</v>
+        <v>43179</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="13">
-        <v>44314</v>
+        <v>44322</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>238273</v>
+        <v>331914</v>
       </c>
       <c r="D22" s="6">
-        <v>194005</v>
+        <v>268978</v>
       </c>
       <c r="E22" s="6">
-        <v>44268</v>
+        <v>62936</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="13">
-        <v>44313</v>
+        <v>44316</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
-        <v>203174</v>
+        <v>274907</v>
       </c>
       <c r="D23" s="6">
-        <v>172069</v>
+        <v>227667</v>
       </c>
       <c r="E23" s="6">
-        <v>31105</v>
+        <v>47240</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="13">
-        <v>44312</v>
+        <v>44314</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C24" s="6">
         <f t="shared" si="0"/>
-        <v>263328</v>
+        <v>238273</v>
       </c>
       <c r="D24" s="6">
-        <v>221677</v>
+        <v>194005</v>
       </c>
       <c r="E24" s="6">
-        <v>41651</v>
+        <v>44268</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="13">
-        <v>44309</v>
+        <v>44313</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
-        <v>177672</v>
+        <v>203174</v>
       </c>
       <c r="D25" s="6">
-        <v>147989</v>
+        <v>172069</v>
       </c>
       <c r="E25" s="6">
-        <v>29683</v>
+        <v>31105</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="13">
-        <v>44308</v>
+        <v>44312</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C26" s="6">
         <f t="shared" si="0"/>
-        <v>150489</v>
+        <v>263328</v>
       </c>
       <c r="D26" s="6">
-        <v>128634</v>
+        <v>221677</v>
       </c>
       <c r="E26" s="6">
-        <v>21855</v>
+        <v>41651</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="13">
-        <v>44307</v>
+        <v>44309</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C27" s="6">
         <f t="shared" si="0"/>
-        <v>152884</v>
+        <v>177672</v>
       </c>
       <c r="D27" s="6">
-        <v>126188</v>
+        <v>147989</v>
       </c>
       <c r="E27" s="6">
-        <v>26696</v>
+        <v>29683</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" s="13">
-        <v>44306</v>
+        <v>44308</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C28" s="6">
         <f t="shared" si="0"/>
-        <v>126419</v>
+        <v>150489</v>
       </c>
       <c r="D28" s="6">
-        <v>98622</v>
+        <v>128634</v>
       </c>
       <c r="E28" s="6">
-        <v>27797</v>
+        <v>21855</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A29" s="15">
-        <v>44305</v>
-      </c>
-      <c r="B29" s="12" t="str">
-        <f t="shared" ref="B29:B32" si="1">"("&amp;TEXT(A29,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A29" s="13">
+        <v>44307</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="C29" s="6">
         <f t="shared" si="0"/>
-        <v>119032</v>
+        <v>152884</v>
       </c>
       <c r="D29" s="6">
-        <v>64725</v>
+        <v>126188</v>
       </c>
       <c r="E29" s="6">
-        <v>54307</v>
+        <v>26696</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" s="13">
+        <v>44306</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="0"/>
+        <v>126419</v>
+      </c>
+      <c r="D30" s="6">
+        <v>98622</v>
+      </c>
+      <c r="E30" s="6">
+        <v>27797</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A31" s="15">
+        <v>44305</v>
+      </c>
+      <c r="B31" s="12" t="str">
+        <f t="shared" ref="B31:B34" si="1">"("&amp;TEXT(A31,"aaa")&amp;")"</f>
+        <v>(月)</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="0"/>
+        <v>119032</v>
+      </c>
+      <c r="D31" s="6">
+        <v>64725</v>
+      </c>
+      <c r="E31" s="6">
+        <v>54307</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A32" s="13">
         <v>44302</v>
       </c>
-      <c r="B30" s="12" t="str">
+      <c r="B32" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(金)</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C32" s="6">
         <f t="shared" si="0"/>
         <v>69687</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D32" s="6">
         <v>29696</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E32" s="6">
         <v>39991</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A31" s="13">
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A33" s="13">
         <v>44301</v>
       </c>
-      <c r="B31" s="12" t="str">
+      <c r="B33" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(木)</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C33" s="6">
         <f t="shared" si="0"/>
         <v>52620</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D33" s="6">
         <v>16637</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E33" s="6">
         <v>35983</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A32" s="13">
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" s="13">
         <v>44300</v>
       </c>
-      <c r="B32" s="12" t="str">
+      <c r="B34" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(水)</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C34" s="6">
         <f t="shared" si="0"/>
         <v>50996</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D34" s="6">
         <v>9569</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E34" s="6">
         <v>41427</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" s="10">
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A35" s="10">
         <v>44299</v>
       </c>
-      <c r="B33" s="12" t="str">
-        <f t="shared" ref="B33:B34" si="2">"("&amp;TEXT(A33,"aaa")&amp;")"</f>
+      <c r="B35" s="12" t="str">
+        <f t="shared" ref="B35:B36" si="2">"("&amp;TEXT(A35,"aaa")&amp;")"</f>
         <v>(火)</v>
       </c>
-      <c r="C33" s="6">
-        <f t="shared" ref="C33:C34" si="3">SUM(D33:E33)</f>
+      <c r="C35" s="6">
+        <f t="shared" ref="C35:C36" si="3">SUM(D35:E35)</f>
         <v>53986</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D35" s="6">
         <v>13896</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E35" s="6">
         <v>40090</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A34" s="10">
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A36" s="10">
         <v>44298</v>
       </c>
-      <c r="B34" s="12" t="str">
+      <c r="B36" s="12" t="str">
         <f t="shared" si="2"/>
         <v>(月)</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C36" s="6">
         <f t="shared" si="3"/>
         <v>96936</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D36" s="6">
         <v>26850</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E36" s="6">
         <v>70086</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A35" s="8"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A36" s="14" t="s">
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A37" s="8"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A38" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" s="7"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A39" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="7"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F41" s="5"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A43" s="1"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A45" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Flat: latest data (2021-06-02T07:51:34.914Z) {   "date": "2021-06-02T07:51:34.914Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 69,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t> 内１回目</t>
   </si>
@@ -258,14 +258,18 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（5月31日時点）</t>
+    <t>(火)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>（6月1日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
-    <rPh sb="5" eb="6">
+    <rPh sb="4" eb="5">
       <t>ニチ</t>
     </rPh>
-    <rPh sb="6" eb="8">
+    <rPh sb="5" eb="7">
       <t>ジテン</t>
     </rPh>
     <phoneticPr fontId="2"/>
@@ -703,7 +707,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -723,7 +727,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E2" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
@@ -751,717 +755,737 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="6">
-        <f t="shared" ref="C4:C34" si="0">SUM(D4:E4)</f>
-        <v>7634137</v>
+        <f t="shared" ref="C4:C35" si="0">SUM(D4:E4)</f>
+        <v>7793194</v>
       </c>
       <c r="D4" s="6">
-        <v>4587179</v>
+        <v>4653566</v>
       </c>
       <c r="E4" s="6">
-        <v>3046958</v>
+        <v>3139628</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
-        <v>44347</v>
+        <v>44348</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>273255</v>
+        <v>159057</v>
       </c>
       <c r="D5" s="6">
-        <v>132005</v>
+        <v>66387</v>
       </c>
       <c r="E5" s="6">
-        <v>141250</v>
+        <v>92670</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
-        <v>44344</v>
+        <v>44347</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
-        <v>164516</v>
+        <v>273255</v>
       </c>
       <c r="D6" s="6">
-        <v>87741</v>
+        <v>132005</v>
       </c>
       <c r="E6" s="6">
-        <v>76775</v>
+        <v>141250</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="13">
-        <v>44343</v>
+        <v>44344</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>145149</v>
+        <v>164516</v>
       </c>
       <c r="D7" s="6">
-        <v>84257</v>
+        <v>87741</v>
       </c>
       <c r="E7" s="6">
-        <v>60892</v>
+        <v>76775</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="13">
-        <v>44342</v>
+        <v>44343</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>142589</v>
+        <v>145149</v>
       </c>
       <c r="D8" s="6">
-        <v>93415</v>
+        <v>84257</v>
       </c>
       <c r="E8" s="6">
-        <v>49174</v>
+        <v>60892</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="13">
-        <v>44341</v>
+        <v>44342</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>139652</v>
+        <v>142589</v>
       </c>
       <c r="D9" s="6">
-        <v>87590</v>
+        <v>93415</v>
       </c>
       <c r="E9" s="6">
-        <v>52062</v>
+        <v>49174</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="13">
-        <v>44340</v>
+        <v>44341</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>330589</v>
+        <v>139652</v>
       </c>
       <c r="D10" s="6">
-        <v>136760</v>
+        <v>87590</v>
       </c>
       <c r="E10" s="6">
-        <v>193829</v>
+        <v>52062</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>249021</v>
+        <v>330589</v>
       </c>
       <c r="D11" s="6">
-        <v>99918</v>
+        <v>136760</v>
       </c>
       <c r="E11" s="6">
-        <v>149103</v>
+        <v>193829</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="13">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D12" s="6">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E12" s="6">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="13">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D13" s="6">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E13" s="6">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="13">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D14" s="6">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E14" s="6">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="13">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D15" s="6">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E15" s="6">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="13">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D16" s="6">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E16" s="6">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="13">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D17" s="6">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E17" s="6">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="13">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D18" s="6">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E18" s="6">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="13">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D19" s="6">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E19" s="6">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="13">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D20" s="6">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E20" s="6">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="13">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D21" s="6">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E21" s="6">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="13">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D22" s="6">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E22" s="6">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="13">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D23" s="6">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E23" s="6">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="13">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C24" s="6">
         <f t="shared" si="0"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D24" s="6">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E24" s="6">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="13">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D25" s="6">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E25" s="6">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="13">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C26" s="6">
         <f t="shared" si="0"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D26" s="6">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E26" s="6">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="13">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C27" s="6">
         <f t="shared" si="0"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D27" s="6">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E27" s="6">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" s="13">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C28" s="6">
         <f t="shared" si="0"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D28" s="6">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E28" s="6">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" s="13">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C29" s="6">
         <f t="shared" si="0"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D29" s="6">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E29" s="6">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" s="13">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C30" s="6">
         <f t="shared" si="0"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D30" s="6">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E30" s="6">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A31" s="15">
-        <v>44305</v>
-      </c>
-      <c r="B31" s="12" t="str">
-        <f t="shared" ref="B31:B34" si="1">"("&amp;TEXT(A31,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A31" s="13">
+        <v>44306</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C31" s="6">
         <f t="shared" si="0"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D31" s="6">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E31" s="6">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A32" s="13">
+      <c r="A32" s="15">
+        <v>44305</v>
+      </c>
+      <c r="B32" s="12" t="str">
+        <f t="shared" ref="B32:B35" si="1">"("&amp;TEXT(A32,"aaa")&amp;")"</f>
+        <v>(月)</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" si="0"/>
+        <v>119032</v>
+      </c>
+      <c r="D32" s="6">
+        <v>64725</v>
+      </c>
+      <c r="E32" s="6">
+        <v>54307</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A33" s="13">
         <v>44302</v>
       </c>
-      <c r="B32" s="12" t="str">
+      <c r="B33" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(金)</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C33" s="6">
         <f t="shared" si="0"/>
         <v>69687</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D33" s="6">
         <v>29696</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E33" s="6">
         <v>39991</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" s="13">
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" s="13">
         <v>44301</v>
       </c>
-      <c r="B33" s="12" t="str">
+      <c r="B34" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(木)</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C34" s="6">
         <f t="shared" si="0"/>
         <v>52620</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <v>16637</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E34" s="6">
         <v>35983</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A34" s="13">
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A35" s="13">
         <v>44300</v>
       </c>
-      <c r="B34" s="12" t="str">
+      <c r="B35" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(水)</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C35" s="6">
         <f t="shared" si="0"/>
         <v>50996</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="6">
         <v>9569</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E35" s="6">
         <v>41427</v>
-      </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A35" s="10">
-        <v>44299</v>
-      </c>
-      <c r="B35" s="12" t="str">
-        <f t="shared" ref="B35:B36" si="2">"("&amp;TEXT(A35,"aaa")&amp;")"</f>
-        <v>(火)</v>
-      </c>
-      <c r="C35" s="6">
-        <f t="shared" ref="C35:C36" si="3">SUM(D35:E35)</f>
-        <v>53986</v>
-      </c>
-      <c r="D35" s="6">
-        <v>13896</v>
-      </c>
-      <c r="E35" s="6">
-        <v>40090</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="10">
+        <v>44299</v>
+      </c>
+      <c r="B36" s="12" t="str">
+        <f t="shared" ref="B36:B37" si="2">"("&amp;TEXT(A36,"aaa")&amp;")"</f>
+        <v>(火)</v>
+      </c>
+      <c r="C36" s="6">
+        <f t="shared" ref="C36:C37" si="3">SUM(D36:E36)</f>
+        <v>53986</v>
+      </c>
+      <c r="D36" s="6">
+        <v>13896</v>
+      </c>
+      <c r="E36" s="6">
+        <v>40090</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A37" s="10">
         <v>44298</v>
       </c>
-      <c r="B36" s="12" t="str">
+      <c r="B37" s="12" t="str">
         <f t="shared" si="2"/>
         <v>(月)</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C37" s="6">
         <f t="shared" si="3"/>
         <v>96936</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D37" s="6">
         <v>26850</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E37" s="6">
         <v>70086</v>
       </c>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A37" s="8"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="7"/>
       <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A39" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="7"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="5"/>
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
         <v>6</v>
       </c>
-      <c r="F40" s="7"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A41" s="1" t="s">
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="7"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F43" s="5"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A45" s="1"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F44" s="5"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A46" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Flat: latest data (2021-06-03T07:25:55.239Z) {   "date": "2021-06-03T07:25:55.239Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 52,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t> 内１回目</t>
   </si>
@@ -262,7 +262,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（6月1日時点）</t>
+    <t>（6月2日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -707,7 +707,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -755,737 +755,757 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="6">
-        <f t="shared" ref="C4:C35" si="0">SUM(D4:E4)</f>
-        <v>7793194</v>
+        <f t="shared" ref="C4:C36" si="0">SUM(D4:E4)</f>
+        <v>7952320</v>
       </c>
       <c r="D4" s="6">
-        <v>4653566</v>
+        <v>4725022</v>
       </c>
       <c r="E4" s="6">
-        <v>3139628</v>
+        <v>3227298</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
-        <v>44348</v>
+        <v>44349</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>159057</v>
+        <v>159126</v>
       </c>
       <c r="D5" s="6">
-        <v>66387</v>
+        <v>71456</v>
       </c>
       <c r="E5" s="6">
-        <v>92670</v>
+        <v>87670</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
-        <v>44347</v>
+        <v>44348</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
-        <v>273255</v>
+        <v>159057</v>
       </c>
       <c r="D6" s="6">
-        <v>132005</v>
+        <v>66387</v>
       </c>
       <c r="E6" s="6">
-        <v>141250</v>
+        <v>92670</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="13">
-        <v>44344</v>
+        <v>44347</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>164516</v>
+        <v>273255</v>
       </c>
       <c r="D7" s="6">
-        <v>87741</v>
+        <v>132005</v>
       </c>
       <c r="E7" s="6">
-        <v>76775</v>
+        <v>141250</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="13">
-        <v>44343</v>
+        <v>44344</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>145149</v>
+        <v>164516</v>
       </c>
       <c r="D8" s="6">
-        <v>84257</v>
+        <v>87741</v>
       </c>
       <c r="E8" s="6">
-        <v>60892</v>
+        <v>76775</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="13">
-        <v>44342</v>
+        <v>44343</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>142589</v>
+        <v>145149</v>
       </c>
       <c r="D9" s="6">
-        <v>93415</v>
+        <v>84257</v>
       </c>
       <c r="E9" s="6">
-        <v>49174</v>
+        <v>60892</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="13">
-        <v>44341</v>
+        <v>44342</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>139652</v>
+        <v>142589</v>
       </c>
       <c r="D10" s="6">
-        <v>87590</v>
+        <v>93415</v>
       </c>
       <c r="E10" s="6">
-        <v>52062</v>
+        <v>49174</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
-        <v>44340</v>
+        <v>44341</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>330589</v>
+        <v>139652</v>
       </c>
       <c r="D11" s="6">
-        <v>136760</v>
+        <v>87590</v>
       </c>
       <c r="E11" s="6">
-        <v>193829</v>
+        <v>52062</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="13">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>249021</v>
+        <v>330589</v>
       </c>
       <c r="D12" s="6">
-        <v>99918</v>
+        <v>136760</v>
       </c>
       <c r="E12" s="6">
-        <v>149103</v>
+        <v>193829</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="13">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D13" s="6">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E13" s="6">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="13">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D14" s="6">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E14" s="6">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="13">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D15" s="6">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E15" s="6">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="13">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D16" s="6">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E16" s="6">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="13">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D17" s="6">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E17" s="6">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="13">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D18" s="6">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E18" s="6">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="13">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D19" s="6">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E19" s="6">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="13">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D20" s="6">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E20" s="6">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="13">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D21" s="6">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E21" s="6">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="13">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D22" s="6">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E22" s="6">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="13">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D23" s="6">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E23" s="6">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="13">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C24" s="6">
         <f t="shared" si="0"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D24" s="6">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E24" s="6">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="13">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D25" s="6">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E25" s="6">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="13">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C26" s="6">
         <f t="shared" si="0"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D26" s="6">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E26" s="6">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="13">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C27" s="6">
         <f t="shared" si="0"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D27" s="6">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E27" s="6">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" s="13">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C28" s="6">
         <f t="shared" si="0"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D28" s="6">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E28" s="6">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" s="13">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C29" s="6">
         <f t="shared" si="0"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D29" s="6">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E29" s="6">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" s="13">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C30" s="6">
         <f t="shared" si="0"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D30" s="6">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E30" s="6">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" s="13">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C31" s="6">
         <f t="shared" si="0"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D31" s="6">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E31" s="6">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A32" s="15">
-        <v>44305</v>
-      </c>
-      <c r="B32" s="12" t="str">
-        <f t="shared" ref="B32:B35" si="1">"("&amp;TEXT(A32,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A32" s="13">
+        <v>44306</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C32" s="6">
         <f t="shared" si="0"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D32" s="6">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E32" s="6">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" s="13">
+      <c r="A33" s="15">
+        <v>44305</v>
+      </c>
+      <c r="B33" s="12" t="str">
+        <f t="shared" ref="B33:B36" si="1">"("&amp;TEXT(A33,"aaa")&amp;")"</f>
+        <v>(月)</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="0"/>
+        <v>119032</v>
+      </c>
+      <c r="D33" s="6">
+        <v>64725</v>
+      </c>
+      <c r="E33" s="6">
+        <v>54307</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" s="13">
         <v>44302</v>
       </c>
-      <c r="B33" s="12" t="str">
+      <c r="B34" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(金)</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C34" s="6">
         <f t="shared" si="0"/>
         <v>69687</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <v>29696</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E34" s="6">
         <v>39991</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A34" s="13">
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A35" s="13">
         <v>44301</v>
       </c>
-      <c r="B34" s="12" t="str">
+      <c r="B35" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(木)</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C35" s="6">
         <f t="shared" si="0"/>
         <v>52620</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="6">
         <v>16637</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E35" s="6">
         <v>35983</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A35" s="13">
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A36" s="13">
         <v>44300</v>
       </c>
-      <c r="B35" s="12" t="str">
+      <c r="B36" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(水)</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C36" s="6">
         <f t="shared" si="0"/>
         <v>50996</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D36" s="6">
         <v>9569</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E36" s="6">
         <v>41427</v>
-      </c>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A36" s="10">
-        <v>44299</v>
-      </c>
-      <c r="B36" s="12" t="str">
-        <f t="shared" ref="B36:B37" si="2">"("&amp;TEXT(A36,"aaa")&amp;")"</f>
-        <v>(火)</v>
-      </c>
-      <c r="C36" s="6">
-        <f t="shared" ref="C36:C37" si="3">SUM(D36:E36)</f>
-        <v>53986</v>
-      </c>
-      <c r="D36" s="6">
-        <v>13896</v>
-      </c>
-      <c r="E36" s="6">
-        <v>40090</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="10">
+        <v>44299</v>
+      </c>
+      <c r="B37" s="12" t="str">
+        <f t="shared" ref="B37:B38" si="2">"("&amp;TEXT(A37,"aaa")&amp;")"</f>
+        <v>(火)</v>
+      </c>
+      <c r="C37" s="6">
+        <f t="shared" ref="C37:C38" si="3">SUM(D37:E37)</f>
+        <v>53986</v>
+      </c>
+      <c r="D37" s="6">
+        <v>13896</v>
+      </c>
+      <c r="E37" s="6">
+        <v>40090</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A38" s="10">
         <v>44298</v>
       </c>
-      <c r="B37" s="12" t="str">
+      <c r="B38" s="12" t="str">
         <f t="shared" si="2"/>
         <v>(月)</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C38" s="6">
         <f t="shared" si="3"/>
         <v>96936</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D38" s="6">
         <v>26850</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E38" s="6">
         <v>70086</v>
       </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="7"/>
       <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="8"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A40" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="7"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="5"/>
       <c r="F40" s="7"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A42" s="1" t="s">
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="7"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F44" s="5"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A46" s="1"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F45" s="5"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A47" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Flat: latest data (2021-06-07T07:38:03.751Z) {   "date": "2021-06-07T07:38:03.751Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 863,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data2.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="医療従事者" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$47</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t> 内１回目</t>
   </si>
@@ -258,11 +261,24 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>(火)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>（6月2日時点）</t>
+    <t>ファイザー社</t>
+    <rPh sb="5" eb="6">
+      <t>シャ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>武田/モデルナ社</t>
+    <rPh sb="0" eb="2">
+      <t>タケダ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>シャ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>（6月4日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -374,7 +390,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -384,12 +400,6 @@
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -422,6 +432,33 @@
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -707,7 +744,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -717,797 +754,994 @@
   <cols>
     <col min="1" max="1" width="18.75" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="7" width="13.875" customWidth="1"/>
+    <col min="3" max="4" width="13.875" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="13.875" customWidth="1"/>
+    <col min="7" max="7" width="15.75" customWidth="1"/>
+    <col min="8" max="9" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="E2" s="14" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G2" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A4" s="18"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="F4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="4">
+        <f t="shared" ref="C5:C8" si="0">SUM(D5:G5)</f>
+        <v>8254680</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4845175</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3176</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3406329</v>
+      </c>
+      <c r="G5" s="4">
         <v>0</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="6">
-        <f t="shared" ref="C4:C36" si="0">SUM(D4:E4)</f>
-        <v>7952320</v>
-      </c>
-      <c r="D4" s="6">
-        <v>4725022</v>
-      </c>
-      <c r="E4" s="6">
-        <v>3227298</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A5" s="13">
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A6" s="15">
+        <v>44351</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>159203</v>
+      </c>
+      <c r="D6" s="4">
+        <v>62634</v>
+      </c>
+      <c r="E6" s="4">
+        <v>929</v>
+      </c>
+      <c r="F6" s="4">
+        <v>95640</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" s="11">
+        <v>44350</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>143157</v>
+      </c>
+      <c r="D7" s="4">
+        <v>59654</v>
+      </c>
+      <c r="E7" s="4">
+        <v>112</v>
+      </c>
+      <c r="F7" s="4">
+        <v>83391</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" s="11">
         <v>44349</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>159126</v>
       </c>
-      <c r="D5" s="6">
-        <v>71456</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="D8" s="4">
+        <v>71140</v>
+      </c>
+      <c r="E8" s="4">
+        <v>316</v>
+      </c>
+      <c r="F8" s="4">
         <v>87670</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" s="13">
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="11">
         <v>44348</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="6">
-        <f t="shared" si="0"/>
+      <c r="B9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" ref="C9:C39" si="1">SUM(D9:G9)</f>
         <v>159057</v>
       </c>
-      <c r="D6" s="6">
-        <v>66387</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="D9" s="4">
+        <v>66264</v>
+      </c>
+      <c r="E9" s="4">
+        <v>123</v>
+      </c>
+      <c r="F9" s="4">
         <v>92670</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="13">
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A10" s="11">
         <v>44347</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6">
-        <f t="shared" si="0"/>
+      <c r="C10" s="4">
+        <f t="shared" si="1"/>
         <v>273255</v>
       </c>
-      <c r="D7" s="6">
-        <v>132005</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="D10" s="4">
+        <v>131423</v>
+      </c>
+      <c r="E10" s="4">
+        <v>582</v>
+      </c>
+      <c r="F10" s="4">
         <v>141250</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="13">
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A11" s="11">
         <v>44344</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="6">
-        <f t="shared" si="0"/>
+      <c r="C11" s="4">
+        <f t="shared" si="1"/>
         <v>164516</v>
       </c>
-      <c r="D8" s="6">
-        <v>87741</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="D11" s="4">
+        <v>87584</v>
+      </c>
+      <c r="E11" s="4">
+        <v>157</v>
+      </c>
+      <c r="F11" s="4">
         <v>76775</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A9" s="13">
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A12" s="11">
         <v>44343</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="6">
-        <f t="shared" si="0"/>
+      <c r="C12" s="4">
+        <f t="shared" si="1"/>
         <v>145149</v>
       </c>
-      <c r="D9" s="6">
-        <v>84257</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="D12" s="4">
+        <v>84217</v>
+      </c>
+      <c r="E12" s="4">
+        <v>40</v>
+      </c>
+      <c r="F12" s="4">
         <v>60892</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A10" s="13">
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A13" s="11">
         <v>44342</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="6">
-        <f t="shared" si="0"/>
+      <c r="C13" s="4">
+        <f t="shared" si="1"/>
         <v>142589</v>
       </c>
-      <c r="D10" s="6">
-        <v>93415</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="D13" s="4">
+        <v>93243</v>
+      </c>
+      <c r="E13" s="4">
+        <v>172</v>
+      </c>
+      <c r="F13" s="4">
         <v>49174</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A11" s="13">
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A14" s="11">
         <v>44341</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="6">
-        <f t="shared" si="0"/>
+      <c r="C14" s="4">
+        <f t="shared" si="1"/>
         <v>139652</v>
       </c>
-      <c r="D11" s="6">
-        <v>87590</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="D14" s="4">
+        <v>87114</v>
+      </c>
+      <c r="E14" s="4">
+        <v>476</v>
+      </c>
+      <c r="F14" s="4">
         <v>52062</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" s="13">
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A15" s="11">
         <v>44340</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="6">
-        <f t="shared" si="0"/>
+      <c r="C15" s="4">
+        <f t="shared" si="1"/>
         <v>330589</v>
       </c>
-      <c r="D12" s="6">
-        <v>136760</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="D15" s="4">
+        <v>136491</v>
+      </c>
+      <c r="E15" s="4">
+        <v>269</v>
+      </c>
+      <c r="F15" s="4">
         <v>193829</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A13" s="13">
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A16" s="11">
         <v>44337</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="6">
-        <f t="shared" si="0"/>
+      <c r="C16" s="4">
+        <f t="shared" si="1"/>
         <v>249021</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D16" s="4">
         <v>99918</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4">
         <v>149103</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A14" s="13">
+      <c r="G16" s="4"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A17" s="11">
         <v>44336</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="6">
-        <f t="shared" si="0"/>
+      <c r="C17" s="4">
+        <f t="shared" si="1"/>
         <v>190533</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D17" s="4">
         <v>81422</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4">
         <v>109111</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A15" s="13">
+      <c r="G17" s="4"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A18" s="11">
         <v>44335</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="6">
-        <f t="shared" si="0"/>
+      <c r="C18" s="4">
+        <f t="shared" si="1"/>
         <v>267866</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D18" s="4">
         <v>88163</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4">
         <v>179703</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A16" s="13">
+      <c r="G18" s="4"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A19" s="11">
         <v>44334</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="6">
-        <f t="shared" si="0"/>
+      <c r="C19" s="4">
+        <f t="shared" si="1"/>
         <v>250244</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D19" s="4">
         <v>94577</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E19" s="4"/>
+      <c r="F19" s="4">
         <v>155667</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A17" s="13">
+      <c r="G19" s="4"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A20" s="11">
         <v>44333</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B20" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="6">
-        <f t="shared" si="0"/>
+      <c r="C20" s="4">
+        <f t="shared" si="1"/>
         <v>349566</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D20" s="4">
         <v>133843</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E20" s="4"/>
+      <c r="F20" s="4">
         <v>215723</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A18" s="13">
+      <c r="G20" s="4"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A21" s="11">
         <v>44330</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="6">
-        <f t="shared" si="0"/>
+      <c r="C21" s="4">
+        <f t="shared" si="1"/>
         <v>242878</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D21" s="4">
         <v>99493</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E21" s="4"/>
+      <c r="F21" s="4">
         <v>143385</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A19" s="13">
+      <c r="G21" s="4"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A22" s="11">
         <v>44329</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="6">
-        <f t="shared" si="0"/>
+      <c r="C22" s="4">
+        <f t="shared" si="1"/>
         <v>219139</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D22" s="4">
         <v>93429</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4">
         <v>125710</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A20" s="13">
+      <c r="G22" s="4"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A23" s="11">
         <v>44328</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B23" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="6">
-        <f t="shared" si="0"/>
+      <c r="C23" s="4">
+        <f t="shared" si="1"/>
         <v>181720</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D23" s="4">
         <v>82959</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E23" s="4"/>
+      <c r="F23" s="4">
         <v>98761</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A21" s="13">
+      <c r="G23" s="4"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A24" s="11">
         <v>44327</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="6">
-        <f t="shared" si="0"/>
+      <c r="C24" s="4">
+        <f t="shared" si="1"/>
         <v>168738</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D24" s="4">
         <v>90287</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4">
         <v>78451</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A22" s="13">
+      <c r="G24" s="4"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A25" s="11">
         <v>44326</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B25" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="6">
-        <f t="shared" si="0"/>
+      <c r="C25" s="4">
+        <f t="shared" si="1"/>
         <v>223504</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D25" s="4">
         <v>155255</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E25" s="4"/>
+      <c r="F25" s="4">
         <v>68249</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23" s="13">
+      <c r="G25" s="4"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A26" s="11">
         <v>44323</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B26" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="6">
-        <f t="shared" si="0"/>
+      <c r="C26" s="4">
+        <f t="shared" si="1"/>
         <v>140344</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D26" s="4">
         <v>97165</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E26" s="4"/>
+      <c r="F26" s="4">
         <v>43179</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A24" s="13">
+      <c r="G26" s="4"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A27" s="11">
         <v>44322</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B27" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="6">
-        <f t="shared" si="0"/>
+      <c r="C27" s="4">
+        <f t="shared" si="1"/>
         <v>331914</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D27" s="4">
         <v>268978</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4">
         <v>62936</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A25" s="13">
+      <c r="G27" s="4"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A28" s="11">
         <v>44316</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B28" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="6">
-        <f t="shared" si="0"/>
+      <c r="C28" s="4">
+        <f t="shared" si="1"/>
         <v>274907</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D28" s="4">
         <v>227667</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E28" s="4"/>
+      <c r="F28" s="4">
         <v>47240</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A26" s="13">
+      <c r="G28" s="4"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A29" s="11">
         <v>44314</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B29" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="6">
-        <f t="shared" si="0"/>
+      <c r="C29" s="4">
+        <f t="shared" si="1"/>
         <v>238273</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D29" s="4">
         <v>194005</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E29" s="4"/>
+      <c r="F29" s="4">
         <v>44268</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A27" s="13">
+      <c r="G29" s="4"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A30" s="11">
         <v>44313</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B30" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="6">
-        <f t="shared" si="0"/>
+      <c r="C30" s="4">
+        <f t="shared" si="1"/>
         <v>203174</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D30" s="4">
         <v>172069</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E30" s="4"/>
+      <c r="F30" s="4">
         <v>31105</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A28" s="13">
+      <c r="G30" s="4"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A31" s="11">
         <v>44312</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B31" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="6">
-        <f t="shared" si="0"/>
+      <c r="C31" s="4">
+        <f t="shared" si="1"/>
         <v>263328</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D31" s="4">
         <v>221677</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E31" s="4"/>
+      <c r="F31" s="4">
         <v>41651</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A29" s="13">
+      <c r="G31" s="4"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A32" s="11">
         <v>44309</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="6">
-        <f t="shared" si="0"/>
+      <c r="C32" s="4">
+        <f t="shared" si="1"/>
         <v>177672</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D32" s="4">
         <v>147989</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4">
         <v>29683</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A30" s="13">
+      <c r="G32" s="4"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A33" s="11">
         <v>44308</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B33" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="6">
-        <f t="shared" si="0"/>
+      <c r="C33" s="4">
+        <f t="shared" si="1"/>
         <v>150489</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D33" s="4">
         <v>128634</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E33" s="4"/>
+      <c r="F33" s="4">
         <v>21855</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A31" s="13">
+      <c r="G33" s="4"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A34" s="11">
         <v>44307</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B34" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="6">
-        <f t="shared" si="0"/>
+      <c r="C34" s="4">
+        <f t="shared" si="1"/>
         <v>152884</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D34" s="4">
         <v>126188</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E34" s="4"/>
+      <c r="F34" s="4">
         <v>26696</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A32" s="13">
+      <c r="G34" s="4"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A35" s="11">
         <v>44306</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B35" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="6">
-        <f t="shared" si="0"/>
+      <c r="C35" s="4">
+        <f t="shared" si="1"/>
         <v>126419</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D35" s="4">
         <v>98622</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E35" s="4"/>
+      <c r="F35" s="4">
         <v>27797</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" s="15">
+      <c r="G35" s="4"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A36" s="13">
         <v>44305</v>
       </c>
-      <c r="B33" s="12" t="str">
-        <f t="shared" ref="B33:B36" si="1">"("&amp;TEXT(A33,"aaa")&amp;")"</f>
+      <c r="B36" s="10" t="str">
+        <f t="shared" ref="B36:B39" si="2">"("&amp;TEXT(A36,"aaa")&amp;")"</f>
         <v>(月)</v>
       </c>
-      <c r="C33" s="6">
-        <f t="shared" si="0"/>
+      <c r="C36" s="4">
+        <f t="shared" si="1"/>
         <v>119032</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D36" s="4">
         <v>64725</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E36" s="4"/>
+      <c r="F36" s="4">
         <v>54307</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A34" s="13">
+      <c r="G36" s="4"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A37" s="11">
         <v>44302</v>
       </c>
-      <c r="B34" s="12" t="str">
-        <f t="shared" si="1"/>
+      <c r="B37" s="10" t="str">
+        <f t="shared" si="2"/>
         <v>(金)</v>
       </c>
-      <c r="C34" s="6">
-        <f t="shared" si="0"/>
+      <c r="C37" s="4">
+        <f t="shared" si="1"/>
         <v>69687</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D37" s="4">
         <v>29696</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E37" s="4"/>
+      <c r="F37" s="4">
         <v>39991</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A35" s="13">
+      <c r="G37" s="4"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A38" s="11">
         <v>44301</v>
       </c>
-      <c r="B35" s="12" t="str">
-        <f t="shared" si="1"/>
+      <c r="B38" s="10" t="str">
+        <f t="shared" si="2"/>
         <v>(木)</v>
       </c>
-      <c r="C35" s="6">
-        <f t="shared" si="0"/>
+      <c r="C38" s="4">
+        <f t="shared" si="1"/>
         <v>52620</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D38" s="4">
         <v>16637</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E38" s="4"/>
+      <c r="F38" s="4">
         <v>35983</v>
       </c>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A36" s="13">
+      <c r="G38" s="4"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A39" s="11">
         <v>44300</v>
       </c>
-      <c r="B36" s="12" t="str">
-        <f t="shared" si="1"/>
+      <c r="B39" s="10" t="str">
+        <f t="shared" si="2"/>
         <v>(水)</v>
       </c>
-      <c r="C36" s="6">
-        <f t="shared" si="0"/>
+      <c r="C39" s="4">
+        <f t="shared" si="1"/>
         <v>50996</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D39" s="4">
         <v>9569</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E39" s="4"/>
+      <c r="F39" s="4">
         <v>41427</v>
       </c>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A37" s="10">
+      <c r="G39" s="4"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A40" s="8">
         <v>44299</v>
       </c>
-      <c r="B37" s="12" t="str">
-        <f t="shared" ref="B37:B38" si="2">"("&amp;TEXT(A37,"aaa")&amp;")"</f>
+      <c r="B40" s="10" t="str">
+        <f t="shared" ref="B40:B41" si="3">"("&amp;TEXT(A40,"aaa")&amp;")"</f>
         <v>(火)</v>
       </c>
-      <c r="C37" s="6">
-        <f t="shared" ref="C37:C38" si="3">SUM(D37:E37)</f>
+      <c r="C40" s="4">
+        <f t="shared" ref="C40:C41" si="4">SUM(D40:G40)</f>
         <v>53986</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D40" s="4">
         <v>13896</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E40" s="4"/>
+      <c r="F40" s="4">
         <v>40090</v>
       </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A38" s="10">
+      <c r="G40" s="4"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A41" s="8">
         <v>44298</v>
       </c>
-      <c r="B38" s="12" t="str">
-        <f t="shared" si="2"/>
+      <c r="B41" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>(月)</v>
       </c>
-      <c r="C38" s="6">
-        <f t="shared" si="3"/>
+      <c r="C41" s="4">
+        <f t="shared" si="4"/>
         <v>96936</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D41" s="4">
         <v>26850</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E41" s="4"/>
+      <c r="F41" s="4">
         <v>70086</v>
       </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A39" s="8"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A40" s="14" t="s">
+      <c r="G41" s="4"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A43" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="7"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
         <v>6</v>
       </c>
-      <c r="F42" s="7"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A43" s="1" t="s">
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F43" s="7"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
         <v>3</v>
       </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F45" s="5"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A47" s="1"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="H48" s="3"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A50" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A4"/>
+  </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="79" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Flat: latest data (2021-06-08T06:32:30.343Z) {   "date": "2021-06-08T06:32:30.343Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 78,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data2.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -10,14 +10,14 @@
     <sheet name="医療従事者" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$48</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t> 内１回目</t>
   </si>
@@ -278,7 +278,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（6月4日時点）</t>
+    <t>（6月7日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -390,7 +390,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -435,6 +435,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -744,7 +750,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -772,30 +778,30 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19" t="s">
+      <c r="E3" s="20"/>
+      <c r="F3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="18"/>
+      <c r="G3" s="20"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="18"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="18"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="14" t="s">
         <v>25</v>
       </c>
@@ -812,22 +818,22 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C8" si="0">SUM(D5:G5)</f>
-        <v>8254680</v>
+        <f t="shared" ref="C5:C9" si="0">SUM(D5:G5)</f>
+        <v>8494017</v>
       </c>
       <c r="D5" s="4">
-        <v>4845175</v>
+        <v>4949610</v>
       </c>
       <c r="E5" s="4">
-        <v>3176</v>
+        <v>5322</v>
       </c>
       <c r="F5" s="4">
-        <v>3406329</v>
+        <v>3539085</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -836,24 +842,24 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="15">
-        <v>44351</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>19</v>
+      <c r="A6" s="17">
+        <v>44354</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>159203</v>
+        <v>239337</v>
       </c>
       <c r="D6" s="4">
-        <v>62634</v>
+        <v>104435</v>
       </c>
       <c r="E6" s="4">
-        <v>929</v>
+        <v>2146</v>
       </c>
       <c r="F6" s="4">
-        <v>95640</v>
+        <v>132756</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -862,24 +868,24 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="11">
-        <v>44350</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>20</v>
+      <c r="A7" s="15">
+        <v>44351</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>143157</v>
+        <v>159203</v>
       </c>
       <c r="D7" s="4">
-        <v>59654</v>
+        <v>62634</v>
       </c>
       <c r="E7" s="4">
-        <v>112</v>
+        <v>929</v>
       </c>
       <c r="F7" s="4">
-        <v>83391</v>
+        <v>95640</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -889,23 +895,23 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="11">
-        <v>44349</v>
+        <v>44350</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>159126</v>
+        <v>143157</v>
       </c>
       <c r="D8" s="4">
-        <v>71140</v>
+        <v>59654</v>
       </c>
       <c r="E8" s="4">
-        <v>316</v>
+        <v>112</v>
       </c>
       <c r="F8" s="4">
-        <v>87670</v>
+        <v>83391</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -915,23 +921,23 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" s="11">
-        <v>44348</v>
+        <v>44349</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4">
-        <f t="shared" ref="C9:C39" si="1">SUM(D9:G9)</f>
-        <v>159057</v>
+        <f t="shared" si="0"/>
+        <v>159126</v>
       </c>
       <c r="D9" s="4">
-        <v>66264</v>
+        <v>71140</v>
       </c>
       <c r="E9" s="4">
-        <v>123</v>
+        <v>316</v>
       </c>
       <c r="F9" s="4">
-        <v>92670</v>
+        <v>87670</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -941,23 +947,23 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="11">
-        <v>44347</v>
+        <v>44348</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C10" s="4">
-        <f t="shared" si="1"/>
-        <v>273255</v>
+        <f t="shared" ref="C10:C40" si="1">SUM(D10:G10)</f>
+        <v>159057</v>
       </c>
       <c r="D10" s="4">
-        <v>131423</v>
+        <v>66264</v>
       </c>
       <c r="E10" s="4">
-        <v>582</v>
+        <v>123</v>
       </c>
       <c r="F10" s="4">
-        <v>141250</v>
+        <v>92670</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -967,23 +973,23 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="11">
-        <v>44344</v>
+        <v>44347</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="1"/>
-        <v>164516</v>
+        <v>273255</v>
       </c>
       <c r="D11" s="4">
-        <v>87584</v>
+        <v>131423</v>
       </c>
       <c r="E11" s="4">
-        <v>157</v>
+        <v>582</v>
       </c>
       <c r="F11" s="4">
-        <v>76775</v>
+        <v>141250</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -993,23 +999,23 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="11">
-        <v>44343</v>
+        <v>44344</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="1"/>
-        <v>145149</v>
+        <v>164516</v>
       </c>
       <c r="D12" s="4">
-        <v>84217</v>
+        <v>87584</v>
       </c>
       <c r="E12" s="4">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="F12" s="4">
-        <v>60892</v>
+        <v>76775</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -1019,23 +1025,23 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="11">
-        <v>44342</v>
+        <v>44343</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="1"/>
-        <v>142589</v>
+        <v>145149</v>
       </c>
       <c r="D13" s="4">
-        <v>93243</v>
+        <v>84217</v>
       </c>
       <c r="E13" s="4">
-        <v>172</v>
+        <v>40</v>
       </c>
       <c r="F13" s="4">
-        <v>49174</v>
+        <v>60892</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -1045,23 +1051,23 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="11">
-        <v>44341</v>
+        <v>44342</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="1"/>
-        <v>139652</v>
+        <v>142589</v>
       </c>
       <c r="D14" s="4">
-        <v>87114</v>
+        <v>93243</v>
       </c>
       <c r="E14" s="4">
-        <v>476</v>
+        <v>172</v>
       </c>
       <c r="F14" s="4">
-        <v>52062</v>
+        <v>49174</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -1071,23 +1077,23 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="11">
-        <v>44340</v>
+        <v>44341</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="1"/>
-        <v>330589</v>
+        <v>139652</v>
       </c>
       <c r="D15" s="4">
-        <v>136491</v>
+        <v>87114</v>
       </c>
       <c r="E15" s="4">
-        <v>269</v>
+        <v>476</v>
       </c>
       <c r="F15" s="4">
-        <v>193829</v>
+        <v>52062</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
@@ -1097,43 +1103,47 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="11">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="1"/>
-        <v>249021</v>
+        <v>330589</v>
       </c>
       <c r="D16" s="4">
-        <v>99918</v>
-      </c>
-      <c r="E16" s="4"/>
+        <v>136491</v>
+      </c>
+      <c r="E16" s="4">
+        <v>269</v>
+      </c>
       <c r="F16" s="4">
-        <v>149103</v>
-      </c>
-      <c r="G16" s="4"/>
+        <v>193829</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="11">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="1"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D17" s="4">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="5"/>
@@ -1141,21 +1151,21 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="11">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="1"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D18" s="4">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="5"/>
@@ -1163,21 +1173,21 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="11">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="1"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D19" s="4">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="5"/>
@@ -1185,21 +1195,21 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="11">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="1"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D20" s="4">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="5"/>
@@ -1207,21 +1217,21 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="11">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="1"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D21" s="4">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="5"/>
@@ -1229,21 +1239,21 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="11">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="1"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D22" s="4">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>
@@ -1251,21 +1261,21 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="11">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="1"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D23" s="4">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="5"/>
@@ -1273,21 +1283,21 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="11">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" si="1"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D24" s="4">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
@@ -1295,21 +1305,21 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="11">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" si="1"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D25" s="4">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
@@ -1317,21 +1327,21 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="11">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="1"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D26" s="4">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5"/>
@@ -1339,21 +1349,21 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="11">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="1"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D27" s="4">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5"/>
@@ -1361,21 +1371,21 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="11">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="1"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D28" s="4">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="5"/>
@@ -1383,21 +1393,21 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="11">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="1"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D29" s="4">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5"/>
@@ -1405,21 +1415,21 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="11">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="1"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D30" s="4">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
@@ -1427,21 +1437,21 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="11">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="1"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D31" s="4">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="5"/>
@@ -1449,21 +1459,21 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="11">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="1"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D32" s="4">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5"/>
@@ -1471,21 +1481,21 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33" s="11">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="1"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D33" s="4">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5"/>
@@ -1493,21 +1503,21 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34" s="11">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="1"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D34" s="4">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="5"/>
@@ -1515,67 +1525,66 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35" s="11">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="1"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D35" s="4">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A36" s="13">
-        <v>44305</v>
-      </c>
-      <c r="B36" s="10" t="str">
-        <f t="shared" ref="B36:B39" si="2">"("&amp;TEXT(A36,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A36" s="11">
+        <v>44306</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="1"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D36" s="4">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A37" s="11">
-        <v>44302</v>
+      <c r="A37" s="13">
+        <v>44305</v>
       </c>
       <c r="B37" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>(金)</v>
+        <f t="shared" ref="B37:B40" si="2">"("&amp;TEXT(A37,"aaa")&amp;")"</f>
+        <v>(月)</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="1"/>
-        <v>69687</v>
+        <v>119032</v>
       </c>
       <c r="D37" s="4">
-        <v>29696</v>
+        <v>64725</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4">
-        <v>39991</v>
+        <v>54307</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
@@ -1583,22 +1592,22 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38" s="11">
-        <v>44301</v>
+        <v>44302</v>
       </c>
       <c r="B38" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(木)</v>
+        <v>(金)</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="1"/>
-        <v>52620</v>
+        <v>69687</v>
       </c>
       <c r="D38" s="4">
-        <v>16637</v>
+        <v>29696</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4">
-        <v>35983</v>
+        <v>39991</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="5"/>
@@ -1606,45 +1615,45 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39" s="11">
-        <v>44300</v>
+        <v>44301</v>
       </c>
       <c r="B39" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(水)</v>
+        <v>(木)</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="1"/>
-        <v>50996</v>
+        <v>52620</v>
       </c>
       <c r="D39" s="4">
-        <v>9569</v>
+        <v>16637</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4">
-        <v>41427</v>
+        <v>35983</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A40" s="8">
-        <v>44299</v>
+      <c r="A40" s="11">
+        <v>44300</v>
       </c>
       <c r="B40" s="10" t="str">
-        <f t="shared" ref="B40:B41" si="3">"("&amp;TEXT(A40,"aaa")&amp;")"</f>
-        <v>(火)</v>
+        <f t="shared" si="2"/>
+        <v>(水)</v>
       </c>
       <c r="C40" s="4">
-        <f t="shared" ref="C40:C41" si="4">SUM(D40:G40)</f>
-        <v>53986</v>
+        <f t="shared" si="1"/>
+        <v>50996</v>
       </c>
       <c r="D40" s="4">
-        <v>13896</v>
+        <v>9569</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4">
-        <v>40090</v>
+        <v>41427</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="5"/>
@@ -1652,86 +1661,109 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41" s="8">
-        <v>44298</v>
+        <v>44299</v>
       </c>
       <c r="B41" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>(月)</v>
+        <f t="shared" ref="B41:B42" si="3">"("&amp;TEXT(A41,"aaa")&amp;")"</f>
+        <v>(火)</v>
       </c>
       <c r="C41" s="4">
-        <f t="shared" si="4"/>
-        <v>96936</v>
+        <f t="shared" ref="C41:C42" si="4">SUM(D41:G41)</f>
+        <v>53986</v>
       </c>
       <c r="D41" s="4">
-        <v>26850</v>
+        <v>13896</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4">
-        <v>70086</v>
+        <v>40090</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A42" s="6"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="5"/>
+      <c r="A42" s="8">
+        <v>44298</v>
+      </c>
+      <c r="B42" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>(月)</v>
+      </c>
+      <c r="C42" s="4">
+        <f t="shared" si="4"/>
+        <v>96936</v>
+      </c>
+      <c r="D42" s="4">
+        <v>26850</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4">
+        <v>70086</v>
+      </c>
+      <c r="G42" s="4"/>
       <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A44" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="3"/>
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
         <v>6</v>
       </c>
-      <c r="H45" s="5"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A46" s="1" t="s">
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H46" s="5"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
         <v>3</v>
       </c>
-      <c r="H47" s="5"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="H48" s="3"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A50" s="1"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H49" s="3"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A51" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Flat: latest data (2021-06-09T06:27:27.657Z) {   "date": "2021-06-09T06:27:27.657Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 77,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data2.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -10,14 +10,14 @@
     <sheet name="医療従事者" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$49</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t> 内１回目</t>
   </si>
@@ -278,7 +278,11 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（6月7日時点）</t>
+    <t>(火)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>（6月8日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -390,7 +394,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -435,6 +439,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -750,7 +760,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -774,34 +784,34 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="G2" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21" t="s">
+      <c r="E3" s="22"/>
+      <c r="F3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="20"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="20"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="20"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="14" t="s">
         <v>25</v>
       </c>
@@ -818,22 +828,22 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C9" si="0">SUM(D5:G5)</f>
-        <v>8494017</v>
+        <f t="shared" ref="C5:C10" si="0">SUM(D5:G5)</f>
+        <v>8655939</v>
       </c>
       <c r="D5" s="4">
-        <v>4949610</v>
+        <v>5021299</v>
       </c>
       <c r="E5" s="4">
-        <v>5322</v>
+        <v>6312</v>
       </c>
       <c r="F5" s="4">
-        <v>3539085</v>
+        <v>3628328</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -842,24 +852,24 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="17">
-        <v>44354</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>21</v>
+      <c r="A6" s="19">
+        <v>44355</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>239337</v>
+        <v>161922</v>
       </c>
       <c r="D6" s="4">
-        <v>104435</v>
+        <v>71689</v>
       </c>
       <c r="E6" s="4">
-        <v>2146</v>
+        <v>990</v>
       </c>
       <c r="F6" s="4">
-        <v>132756</v>
+        <v>89243</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -868,24 +878,24 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="15">
-        <v>44351</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>19</v>
+      <c r="A7" s="17">
+        <v>44354</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>159203</v>
+        <v>239337</v>
       </c>
       <c r="D7" s="4">
-        <v>62634</v>
+        <v>104435</v>
       </c>
       <c r="E7" s="4">
-        <v>929</v>
+        <v>2146</v>
       </c>
       <c r="F7" s="4">
-        <v>95640</v>
+        <v>132756</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -894,24 +904,24 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="11">
-        <v>44350</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>20</v>
+      <c r="A8" s="15">
+        <v>44351</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>143157</v>
+        <v>159203</v>
       </c>
       <c r="D8" s="4">
-        <v>59654</v>
+        <v>62634</v>
       </c>
       <c r="E8" s="4">
-        <v>112</v>
+        <v>929</v>
       </c>
       <c r="F8" s="4">
-        <v>83391</v>
+        <v>95640</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -921,23 +931,23 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" s="11">
-        <v>44349</v>
+        <v>44350</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>159126</v>
+        <v>143157</v>
       </c>
       <c r="D9" s="4">
-        <v>71140</v>
+        <v>59654</v>
       </c>
       <c r="E9" s="4">
-        <v>316</v>
+        <v>112</v>
       </c>
       <c r="F9" s="4">
-        <v>87670</v>
+        <v>83391</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -947,23 +957,23 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="11">
-        <v>44348</v>
+        <v>44349</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4">
-        <f t="shared" ref="C10:C40" si="1">SUM(D10:G10)</f>
-        <v>159057</v>
+        <f t="shared" si="0"/>
+        <v>159126</v>
       </c>
       <c r="D10" s="4">
-        <v>66264</v>
+        <v>71140</v>
       </c>
       <c r="E10" s="4">
-        <v>123</v>
+        <v>316</v>
       </c>
       <c r="F10" s="4">
-        <v>92670</v>
+        <v>87670</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -973,23 +983,23 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="11">
-        <v>44347</v>
+        <v>44348</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C11" s="4">
-        <f t="shared" si="1"/>
-        <v>273255</v>
+        <f t="shared" ref="C11:C41" si="1">SUM(D11:G11)</f>
+        <v>159057</v>
       </c>
       <c r="D11" s="4">
-        <v>131423</v>
+        <v>66264</v>
       </c>
       <c r="E11" s="4">
-        <v>582</v>
+        <v>123</v>
       </c>
       <c r="F11" s="4">
-        <v>141250</v>
+        <v>92670</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -999,23 +1009,23 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="11">
-        <v>44344</v>
+        <v>44347</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="1"/>
-        <v>164516</v>
+        <v>273255</v>
       </c>
       <c r="D12" s="4">
-        <v>87584</v>
+        <v>131423</v>
       </c>
       <c r="E12" s="4">
-        <v>157</v>
+        <v>582</v>
       </c>
       <c r="F12" s="4">
-        <v>76775</v>
+        <v>141250</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -1025,23 +1035,23 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="11">
-        <v>44343</v>
+        <v>44344</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="1"/>
-        <v>145149</v>
+        <v>164516</v>
       </c>
       <c r="D13" s="4">
-        <v>84217</v>
+        <v>87584</v>
       </c>
       <c r="E13" s="4">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="F13" s="4">
-        <v>60892</v>
+        <v>76775</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -1051,23 +1061,23 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="11">
-        <v>44342</v>
+        <v>44343</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="1"/>
-        <v>142589</v>
+        <v>145149</v>
       </c>
       <c r="D14" s="4">
-        <v>93243</v>
+        <v>84217</v>
       </c>
       <c r="E14" s="4">
-        <v>172</v>
+        <v>40</v>
       </c>
       <c r="F14" s="4">
-        <v>49174</v>
+        <v>60892</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -1077,23 +1087,23 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="11">
-        <v>44341</v>
+        <v>44342</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="1"/>
-        <v>139652</v>
+        <v>142589</v>
       </c>
       <c r="D15" s="4">
-        <v>87114</v>
+        <v>93243</v>
       </c>
       <c r="E15" s="4">
-        <v>476</v>
+        <v>172</v>
       </c>
       <c r="F15" s="4">
-        <v>52062</v>
+        <v>49174</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
@@ -1103,23 +1113,23 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="11">
-        <v>44340</v>
+        <v>44341</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="1"/>
-        <v>330589</v>
+        <v>139652</v>
       </c>
       <c r="D16" s="4">
-        <v>136491</v>
+        <v>87114</v>
       </c>
       <c r="E16" s="4">
-        <v>269</v>
+        <v>476</v>
       </c>
       <c r="F16" s="4">
-        <v>193829</v>
+        <v>52062</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
@@ -1129,43 +1139,47 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="11">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="1"/>
-        <v>249021</v>
+        <v>330589</v>
       </c>
       <c r="D17" s="4">
-        <v>99918</v>
-      </c>
-      <c r="E17" s="4"/>
+        <v>136491</v>
+      </c>
+      <c r="E17" s="4">
+        <v>269</v>
+      </c>
       <c r="F17" s="4">
-        <v>149103</v>
-      </c>
-      <c r="G17" s="4"/>
+        <v>193829</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="11">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="1"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D18" s="4">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="5"/>
@@ -1173,21 +1187,21 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="11">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="1"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D19" s="4">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="5"/>
@@ -1195,21 +1209,21 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="11">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="1"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D20" s="4">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="5"/>
@@ -1217,21 +1231,21 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="11">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="1"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D21" s="4">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="5"/>
@@ -1239,21 +1253,21 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="11">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="1"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D22" s="4">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>
@@ -1261,21 +1275,21 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="11">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="1"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D23" s="4">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="5"/>
@@ -1283,21 +1297,21 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="11">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" si="1"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D24" s="4">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
@@ -1305,21 +1319,21 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="11">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" si="1"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D25" s="4">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
@@ -1327,21 +1341,21 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="11">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="1"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D26" s="4">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5"/>
@@ -1349,21 +1363,21 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="11">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="1"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D27" s="4">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5"/>
@@ -1371,21 +1385,21 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="11">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="1"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D28" s="4">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="5"/>
@@ -1393,21 +1407,21 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="11">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="1"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D29" s="4">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5"/>
@@ -1415,21 +1429,21 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="11">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="1"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D30" s="4">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
@@ -1437,21 +1451,21 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="11">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="1"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D31" s="4">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="5"/>
@@ -1459,311 +1473,333 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="11">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="1"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D32" s="4">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="11">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="1"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D33" s="4">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="11">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="1"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D34" s="4">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="11">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="1"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D35" s="4">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="11">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="1"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D36" s="4">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A37" s="13">
-        <v>44305</v>
-      </c>
-      <c r="B37" s="10" t="str">
-        <f t="shared" ref="B37:B40" si="2">"("&amp;TEXT(A37,"aaa")&amp;")"</f>
-        <v>(月)</v>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A37" s="11">
+        <v>44306</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="1"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D37" s="4">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A38" s="11">
-        <v>44302</v>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A38" s="13">
+        <v>44305</v>
       </c>
       <c r="B38" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>(金)</v>
+        <f t="shared" ref="B38:B41" si="2">"("&amp;TEXT(A38,"aaa")&amp;")"</f>
+        <v>(月)</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="1"/>
-        <v>69687</v>
+        <v>119032</v>
       </c>
       <c r="D38" s="4">
-        <v>29696</v>
+        <v>64725</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4">
-        <v>39991</v>
+        <v>54307</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="11">
-        <v>44301</v>
+        <v>44302</v>
       </c>
       <c r="B39" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(木)</v>
+        <v>(金)</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="1"/>
-        <v>52620</v>
+        <v>69687</v>
       </c>
       <c r="D39" s="4">
-        <v>16637</v>
+        <v>29696</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4">
-        <v>35983</v>
+        <v>39991</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="11">
-        <v>44300</v>
+        <v>44301</v>
       </c>
       <c r="B40" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(水)</v>
+        <v>(木)</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="1"/>
-        <v>50996</v>
+        <v>52620</v>
       </c>
       <c r="D40" s="4">
-        <v>9569</v>
+        <v>16637</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4">
-        <v>41427</v>
+        <v>35983</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A41" s="8">
-        <v>44299</v>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A41" s="11">
+        <v>44300</v>
       </c>
       <c r="B41" s="10" t="str">
-        <f t="shared" ref="B41:B42" si="3">"("&amp;TEXT(A41,"aaa")&amp;")"</f>
-        <v>(火)</v>
+        <f t="shared" si="2"/>
+        <v>(水)</v>
       </c>
       <c r="C41" s="4">
-        <f t="shared" ref="C41:C42" si="4">SUM(D41:G41)</f>
-        <v>53986</v>
+        <f t="shared" si="1"/>
+        <v>50996</v>
       </c>
       <c r="D41" s="4">
-        <v>13896</v>
+        <v>9569</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4">
-        <v>40090</v>
+        <v>41427</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42" s="8">
-        <v>44298</v>
+        <v>44299</v>
       </c>
       <c r="B42" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>(月)</v>
+        <f t="shared" ref="B42:B43" si="3">"("&amp;TEXT(A42,"aaa")&amp;")"</f>
+        <v>(火)</v>
       </c>
       <c r="C42" s="4">
-        <f t="shared" si="4"/>
-        <v>96936</v>
+        <f t="shared" ref="C42:C43" si="4">SUM(D42:G42)</f>
+        <v>53986</v>
       </c>
       <c r="D42" s="4">
-        <v>26850</v>
+        <v>13896</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4">
-        <v>70086</v>
+        <v>40090</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A43" s="6"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="5"/>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A43" s="8">
+        <v>44298</v>
+      </c>
+      <c r="B43" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>(月)</v>
+      </c>
+      <c r="C43" s="4">
+        <f t="shared" si="4"/>
+        <v>96936</v>
+      </c>
+      <c r="D43" s="4">
+        <v>26850</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4">
+        <v>70086</v>
+      </c>
+      <c r="G43" s="4"/>
       <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A44" s="12" t="s">
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A45" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="5"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="H45" s="5"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
         <v>6</v>
       </c>
-      <c r="H46" s="5"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A47" s="1" t="s">
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H47" s="5"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
         <v>3</v>
       </c>
-      <c r="H48" s="5"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="H49" s="3"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A51" s="1"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="H50" s="3"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A52" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Flat: latest data (2021-06-10T06:23:39.522Z) {   "date": "2021-06-10T06:23:39.522Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 71,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data2.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -10,14 +10,14 @@
     <sheet name="医療従事者" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$50</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t> 内１回目</t>
   </si>
@@ -282,7 +282,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（6月8日時点）</t>
+    <t>（6月9日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -394,7 +394,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -439,6 +439,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -760,7 +766,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -788,30 +794,30 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23" t="s">
+      <c r="E3" s="24"/>
+      <c r="F3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="22"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="22"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="22"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="14" t="s">
         <v>25</v>
       </c>
@@ -828,22 +834,22 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="22"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C10" si="0">SUM(D5:G5)</f>
-        <v>8655939</v>
+        <f t="shared" ref="C5:C11" si="0">SUM(D5:G5)</f>
+        <v>8823323</v>
       </c>
       <c r="D5" s="4">
-        <v>5021299</v>
+        <v>5088993</v>
       </c>
       <c r="E5" s="4">
-        <v>6312</v>
+        <v>7359</v>
       </c>
       <c r="F5" s="4">
-        <v>3628328</v>
+        <v>3726971</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -852,24 +858,24 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="19">
-        <v>44355</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>27</v>
+      <c r="A6" s="21">
+        <v>44356</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>161922</v>
+        <v>167384</v>
       </c>
       <c r="D6" s="4">
-        <v>71689</v>
+        <v>67694</v>
       </c>
       <c r="E6" s="4">
-        <v>990</v>
+        <v>1047</v>
       </c>
       <c r="F6" s="4">
-        <v>89243</v>
+        <v>98643</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -878,24 +884,24 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="17">
-        <v>44354</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>21</v>
+      <c r="A7" s="19">
+        <v>44355</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>239337</v>
+        <v>161922</v>
       </c>
       <c r="D7" s="4">
-        <v>104435</v>
+        <v>71689</v>
       </c>
       <c r="E7" s="4">
-        <v>2146</v>
+        <v>990</v>
       </c>
       <c r="F7" s="4">
-        <v>132756</v>
+        <v>89243</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -904,24 +910,24 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="15">
-        <v>44351</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>19</v>
+      <c r="A8" s="17">
+        <v>44354</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>159203</v>
+        <v>239337</v>
       </c>
       <c r="D8" s="4">
-        <v>62634</v>
+        <v>104435</v>
       </c>
       <c r="E8" s="4">
-        <v>929</v>
+        <v>2146</v>
       </c>
       <c r="F8" s="4">
-        <v>95640</v>
+        <v>132756</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -930,24 +936,24 @@
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="11">
-        <v>44350</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>20</v>
+      <c r="A9" s="15">
+        <v>44351</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>143157</v>
+        <v>159203</v>
       </c>
       <c r="D9" s="4">
-        <v>59654</v>
+        <v>62634</v>
       </c>
       <c r="E9" s="4">
-        <v>112</v>
+        <v>929</v>
       </c>
       <c r="F9" s="4">
-        <v>83391</v>
+        <v>95640</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -957,23 +963,23 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="11">
-        <v>44349</v>
+        <v>44350</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
-        <v>159126</v>
+        <v>143157</v>
       </c>
       <c r="D10" s="4">
-        <v>71140</v>
+        <v>59654</v>
       </c>
       <c r="E10" s="4">
-        <v>316</v>
+        <v>112</v>
       </c>
       <c r="F10" s="4">
-        <v>87670</v>
+        <v>83391</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -983,23 +989,23 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="11">
-        <v>44348</v>
+        <v>44349</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C11" s="4">
-        <f t="shared" ref="C11:C41" si="1">SUM(D11:G11)</f>
-        <v>159057</v>
+        <f t="shared" si="0"/>
+        <v>159126</v>
       </c>
       <c r="D11" s="4">
-        <v>66264</v>
+        <v>71140</v>
       </c>
       <c r="E11" s="4">
-        <v>123</v>
+        <v>316</v>
       </c>
       <c r="F11" s="4">
-        <v>92670</v>
+        <v>87670</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -1009,23 +1015,23 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="11">
-        <v>44347</v>
+        <v>44348</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C12" s="4">
-        <f t="shared" si="1"/>
-        <v>273255</v>
+        <f t="shared" ref="C12:C42" si="1">SUM(D12:G12)</f>
+        <v>159057</v>
       </c>
       <c r="D12" s="4">
-        <v>131423</v>
+        <v>66264</v>
       </c>
       <c r="E12" s="4">
-        <v>582</v>
+        <v>123</v>
       </c>
       <c r="F12" s="4">
-        <v>141250</v>
+        <v>92670</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -1035,23 +1041,23 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="11">
-        <v>44344</v>
+        <v>44347</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="1"/>
-        <v>164516</v>
+        <v>273255</v>
       </c>
       <c r="D13" s="4">
-        <v>87584</v>
+        <v>131423</v>
       </c>
       <c r="E13" s="4">
-        <v>157</v>
+        <v>582</v>
       </c>
       <c r="F13" s="4">
-        <v>76775</v>
+        <v>141250</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -1061,23 +1067,23 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="11">
-        <v>44343</v>
+        <v>44344</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="1"/>
-        <v>145149</v>
+        <v>164516</v>
       </c>
       <c r="D14" s="4">
-        <v>84217</v>
+        <v>87584</v>
       </c>
       <c r="E14" s="4">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="F14" s="4">
-        <v>60892</v>
+        <v>76775</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -1087,23 +1093,23 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="11">
-        <v>44342</v>
+        <v>44343</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="1"/>
-        <v>142589</v>
+        <v>145149</v>
       </c>
       <c r="D15" s="4">
-        <v>93243</v>
+        <v>84217</v>
       </c>
       <c r="E15" s="4">
-        <v>172</v>
+        <v>40</v>
       </c>
       <c r="F15" s="4">
-        <v>49174</v>
+        <v>60892</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
@@ -1113,23 +1119,23 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="11">
-        <v>44341</v>
+        <v>44342</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="1"/>
-        <v>139652</v>
+        <v>142589</v>
       </c>
       <c r="D16" s="4">
-        <v>87114</v>
+        <v>93243</v>
       </c>
       <c r="E16" s="4">
-        <v>476</v>
+        <v>172</v>
       </c>
       <c r="F16" s="4">
-        <v>52062</v>
+        <v>49174</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
@@ -1139,23 +1145,23 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="11">
-        <v>44340</v>
+        <v>44341</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="1"/>
-        <v>330589</v>
+        <v>139652</v>
       </c>
       <c r="D17" s="4">
-        <v>136491</v>
+        <v>87114</v>
       </c>
       <c r="E17" s="4">
-        <v>269</v>
+        <v>476</v>
       </c>
       <c r="F17" s="4">
-        <v>193829</v>
+        <v>52062</v>
       </c>
       <c r="G17" s="4">
         <v>0</v>
@@ -1165,43 +1171,47 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="11">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="1"/>
-        <v>249021</v>
+        <v>330589</v>
       </c>
       <c r="D18" s="4">
-        <v>99918</v>
-      </c>
-      <c r="E18" s="4"/>
+        <v>136491</v>
+      </c>
+      <c r="E18" s="4">
+        <v>269</v>
+      </c>
       <c r="F18" s="4">
-        <v>149103</v>
-      </c>
-      <c r="G18" s="4"/>
+        <v>193829</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="11">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="1"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D19" s="4">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="5"/>
@@ -1209,21 +1219,21 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="11">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="1"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D20" s="4">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="5"/>
@@ -1231,21 +1241,21 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="11">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="1"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D21" s="4">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="5"/>
@@ -1253,21 +1263,21 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="11">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="1"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D22" s="4">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>
@@ -1275,21 +1285,21 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="11">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="1"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D23" s="4">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="5"/>
@@ -1297,21 +1307,21 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="11">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" si="1"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D24" s="4">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
@@ -1319,21 +1329,21 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="11">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" si="1"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D25" s="4">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
@@ -1341,21 +1351,21 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="11">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="1"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D26" s="4">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5"/>
@@ -1363,21 +1373,21 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="11">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="1"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D27" s="4">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5"/>
@@ -1385,21 +1395,21 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="11">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="1"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D28" s="4">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="5"/>
@@ -1407,21 +1417,21 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="11">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="1"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D29" s="4">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5"/>
@@ -1429,21 +1439,21 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="11">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="1"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D30" s="4">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
@@ -1451,21 +1461,21 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="11">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="1"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D31" s="4">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="5"/>
@@ -1473,21 +1483,21 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="11">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="1"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D32" s="4">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5"/>
@@ -1495,21 +1505,21 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="11">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="1"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D33" s="4">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5"/>
@@ -1517,21 +1527,21 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="11">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="1"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D34" s="4">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="5"/>
@@ -1539,21 +1549,21 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="11">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="1"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D35" s="4">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="5"/>
@@ -1561,21 +1571,21 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="11">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="1"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D36" s="4">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="5"/>
@@ -1583,67 +1593,66 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="11">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="1"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D37" s="4">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A38" s="13">
-        <v>44305</v>
-      </c>
-      <c r="B38" s="10" t="str">
-        <f t="shared" ref="B38:B41" si="2">"("&amp;TEXT(A38,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A38" s="11">
+        <v>44306</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="1"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D38" s="4">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A39" s="11">
-        <v>44302</v>
+      <c r="A39" s="13">
+        <v>44305</v>
       </c>
       <c r="B39" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>(金)</v>
+        <f t="shared" ref="B39:B42" si="2">"("&amp;TEXT(A39,"aaa")&amp;")"</f>
+        <v>(月)</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="1"/>
-        <v>69687</v>
+        <v>119032</v>
       </c>
       <c r="D39" s="4">
-        <v>29696</v>
+        <v>64725</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4">
-        <v>39991</v>
+        <v>54307</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="5"/>
@@ -1651,22 +1660,22 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="11">
-        <v>44301</v>
+        <v>44302</v>
       </c>
       <c r="B40" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(木)</v>
+        <v>(金)</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="1"/>
-        <v>52620</v>
+        <v>69687</v>
       </c>
       <c r="D40" s="4">
-        <v>16637</v>
+        <v>29696</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4">
-        <v>35983</v>
+        <v>39991</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="5"/>
@@ -1674,45 +1683,45 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="11">
-        <v>44300</v>
+        <v>44301</v>
       </c>
       <c r="B41" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(水)</v>
+        <v>(木)</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="1"/>
-        <v>50996</v>
+        <v>52620</v>
       </c>
       <c r="D41" s="4">
-        <v>9569</v>
+        <v>16637</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4">
-        <v>41427</v>
+        <v>35983</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A42" s="8">
-        <v>44299</v>
+      <c r="A42" s="11">
+        <v>44300</v>
       </c>
       <c r="B42" s="10" t="str">
-        <f t="shared" ref="B42:B43" si="3">"("&amp;TEXT(A42,"aaa")&amp;")"</f>
-        <v>(火)</v>
+        <f t="shared" si="2"/>
+        <v>(水)</v>
       </c>
       <c r="C42" s="4">
-        <f t="shared" ref="C42:C43" si="4">SUM(D42:G42)</f>
-        <v>53986</v>
+        <f t="shared" si="1"/>
+        <v>50996</v>
       </c>
       <c r="D42" s="4">
-        <v>13896</v>
+        <v>9569</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4">
-        <v>40090</v>
+        <v>41427</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="5"/>
@@ -1720,86 +1729,109 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43" s="8">
-        <v>44298</v>
+        <v>44299</v>
       </c>
       <c r="B43" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>(月)</v>
+        <f t="shared" ref="B43:B44" si="3">"("&amp;TEXT(A43,"aaa")&amp;")"</f>
+        <v>(火)</v>
       </c>
       <c r="C43" s="4">
-        <f t="shared" si="4"/>
-        <v>96936</v>
+        <f t="shared" ref="C43:C44" si="4">SUM(D43:G43)</f>
+        <v>53986</v>
       </c>
       <c r="D43" s="4">
-        <v>26850</v>
+        <v>13896</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4">
-        <v>70086</v>
+        <v>40090</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A44" s="6"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="5"/>
+      <c r="A44" s="8">
+        <v>44298</v>
+      </c>
+      <c r="B44" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>(月)</v>
+      </c>
+      <c r="C44" s="4">
+        <f t="shared" si="4"/>
+        <v>96936</v>
+      </c>
+      <c r="D44" s="4">
+        <v>26850</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4">
+        <v>70086</v>
+      </c>
+      <c r="G44" s="4"/>
       <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="6"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A46" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="5"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="3"/>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
         <v>6</v>
       </c>
-      <c r="H47" s="5"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A48" s="1" t="s">
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A49" t="s">
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
         <v>3</v>
       </c>
-      <c r="H49" s="5"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="H50" s="3"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A52" s="1"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="H51" s="3"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A53" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Flat: latest data (2021-06-11T06:18:15.923Z) {   "date": "2021-06-11T06:18:15.923Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 75,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data2.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -10,14 +10,14 @@
     <sheet name="医療従事者" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$50</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$51</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t> 内１回目</t>
   </si>
@@ -282,14 +282,14 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（6月9日時点）</t>
+    <t>（6月10日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
-    <rPh sb="4" eb="5">
+    <rPh sb="5" eb="6">
       <t>ニチ</t>
     </rPh>
-    <rPh sb="5" eb="7">
+    <rPh sb="6" eb="8">
       <t>ジテン</t>
     </rPh>
     <phoneticPr fontId="2"/>
@@ -394,7 +394,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -439,6 +439,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -766,7 +772,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -794,30 +800,30 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="25" t="s">
+      <c r="E3" s="26"/>
+      <c r="F3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="24"/>
+      <c r="G3" s="26"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="24"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="14" t="s">
         <v>25</v>
       </c>
@@ -834,22 +840,22 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C11" si="0">SUM(D5:G5)</f>
-        <v>8823323</v>
+        <f t="shared" ref="C5:C12" si="0">SUM(D5:G5)</f>
+        <v>8959914</v>
       </c>
       <c r="D5" s="4">
-        <v>5088993</v>
+        <v>5141243</v>
       </c>
       <c r="E5" s="4">
-        <v>7359</v>
+        <v>9078</v>
       </c>
       <c r="F5" s="4">
-        <v>3726971</v>
+        <v>3809593</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -858,24 +864,24 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="21">
-        <v>44356</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>18</v>
+      <c r="A6" s="23">
+        <v>44357</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>20</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>167384</v>
+        <v>136591</v>
       </c>
       <c r="D6" s="4">
-        <v>67694</v>
+        <v>52250</v>
       </c>
       <c r="E6" s="4">
-        <v>1047</v>
+        <v>1719</v>
       </c>
       <c r="F6" s="4">
-        <v>98643</v>
+        <v>82622</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -884,24 +890,24 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="19">
-        <v>44355</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>27</v>
+      <c r="A7" s="21">
+        <v>44356</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>161922</v>
+        <v>167384</v>
       </c>
       <c r="D7" s="4">
-        <v>71689</v>
+        <v>67694</v>
       </c>
       <c r="E7" s="4">
-        <v>990</v>
+        <v>1047</v>
       </c>
       <c r="F7" s="4">
-        <v>89243</v>
+        <v>98643</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -910,24 +916,24 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="17">
-        <v>44354</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>21</v>
+      <c r="A8" s="19">
+        <v>44355</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>239337</v>
+        <v>161922</v>
       </c>
       <c r="D8" s="4">
-        <v>104435</v>
+        <v>71689</v>
       </c>
       <c r="E8" s="4">
-        <v>2146</v>
+        <v>990</v>
       </c>
       <c r="F8" s="4">
-        <v>132756</v>
+        <v>89243</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -936,24 +942,24 @@
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="15">
-        <v>44351</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>19</v>
+      <c r="A9" s="17">
+        <v>44354</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>159203</v>
+        <v>239337</v>
       </c>
       <c r="D9" s="4">
-        <v>62634</v>
+        <v>104435</v>
       </c>
       <c r="E9" s="4">
-        <v>929</v>
+        <v>2146</v>
       </c>
       <c r="F9" s="4">
-        <v>95640</v>
+        <v>132756</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -962,24 +968,24 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="11">
-        <v>44350</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>20</v>
+      <c r="A10" s="15">
+        <v>44351</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
-        <v>143157</v>
+        <v>159203</v>
       </c>
       <c r="D10" s="4">
-        <v>59654</v>
+        <v>62634</v>
       </c>
       <c r="E10" s="4">
-        <v>112</v>
+        <v>929</v>
       </c>
       <c r="F10" s="4">
-        <v>83391</v>
+        <v>95640</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -989,23 +995,23 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="11">
-        <v>44349</v>
+        <v>44350</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
-        <v>159126</v>
+        <v>143157</v>
       </c>
       <c r="D11" s="4">
-        <v>71140</v>
+        <v>59654</v>
       </c>
       <c r="E11" s="4">
-        <v>316</v>
+        <v>112</v>
       </c>
       <c r="F11" s="4">
-        <v>87670</v>
+        <v>83391</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -1015,23 +1021,23 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="11">
-        <v>44348</v>
+        <v>44349</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C12" s="4">
-        <f t="shared" ref="C12:C42" si="1">SUM(D12:G12)</f>
-        <v>159057</v>
+        <f t="shared" si="0"/>
+        <v>159126</v>
       </c>
       <c r="D12" s="4">
-        <v>66264</v>
+        <v>71140</v>
       </c>
       <c r="E12" s="4">
-        <v>123</v>
+        <v>316</v>
       </c>
       <c r="F12" s="4">
-        <v>92670</v>
+        <v>87670</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -1041,23 +1047,23 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="11">
-        <v>44347</v>
+        <v>44348</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C13" s="4">
-        <f t="shared" si="1"/>
-        <v>273255</v>
+        <f t="shared" ref="C13:C43" si="1">SUM(D13:G13)</f>
+        <v>159057</v>
       </c>
       <c r="D13" s="4">
-        <v>131423</v>
+        <v>66264</v>
       </c>
       <c r="E13" s="4">
-        <v>582</v>
+        <v>123</v>
       </c>
       <c r="F13" s="4">
-        <v>141250</v>
+        <v>92670</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -1067,23 +1073,23 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="11">
-        <v>44344</v>
+        <v>44347</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="1"/>
-        <v>164516</v>
+        <v>273255</v>
       </c>
       <c r="D14" s="4">
-        <v>87584</v>
+        <v>131423</v>
       </c>
       <c r="E14" s="4">
-        <v>157</v>
+        <v>582</v>
       </c>
       <c r="F14" s="4">
-        <v>76775</v>
+        <v>141250</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -1093,23 +1099,23 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="11">
-        <v>44343</v>
+        <v>44344</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="1"/>
-        <v>145149</v>
+        <v>164516</v>
       </c>
       <c r="D15" s="4">
-        <v>84217</v>
+        <v>87584</v>
       </c>
       <c r="E15" s="4">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="F15" s="4">
-        <v>60892</v>
+        <v>76775</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
@@ -1119,23 +1125,23 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="11">
-        <v>44342</v>
+        <v>44343</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="1"/>
-        <v>142589</v>
+        <v>145149</v>
       </c>
       <c r="D16" s="4">
-        <v>93243</v>
+        <v>84217</v>
       </c>
       <c r="E16" s="4">
-        <v>172</v>
+        <v>40</v>
       </c>
       <c r="F16" s="4">
-        <v>49174</v>
+        <v>60892</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
@@ -1145,23 +1151,23 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="11">
-        <v>44341</v>
+        <v>44342</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="1"/>
-        <v>139652</v>
+        <v>142589</v>
       </c>
       <c r="D17" s="4">
-        <v>87114</v>
+        <v>93243</v>
       </c>
       <c r="E17" s="4">
-        <v>476</v>
+        <v>172</v>
       </c>
       <c r="F17" s="4">
-        <v>52062</v>
+        <v>49174</v>
       </c>
       <c r="G17" s="4">
         <v>0</v>
@@ -1171,23 +1177,23 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="11">
-        <v>44340</v>
+        <v>44341</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="1"/>
-        <v>330589</v>
+        <v>139652</v>
       </c>
       <c r="D18" s="4">
-        <v>136491</v>
+        <v>87114</v>
       </c>
       <c r="E18" s="4">
-        <v>269</v>
+        <v>476</v>
       </c>
       <c r="F18" s="4">
-        <v>193829</v>
+        <v>52062</v>
       </c>
       <c r="G18" s="4">
         <v>0</v>
@@ -1197,43 +1203,47 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="11">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="1"/>
-        <v>249021</v>
+        <v>330589</v>
       </c>
       <c r="D19" s="4">
-        <v>99918</v>
-      </c>
-      <c r="E19" s="4"/>
+        <v>136491</v>
+      </c>
+      <c r="E19" s="4">
+        <v>269</v>
+      </c>
       <c r="F19" s="4">
-        <v>149103</v>
-      </c>
-      <c r="G19" s="4"/>
+        <v>193829</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="11">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="1"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D20" s="4">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="5"/>
@@ -1241,21 +1251,21 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="11">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="1"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D21" s="4">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="5"/>
@@ -1263,21 +1273,21 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="11">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="1"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D22" s="4">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>
@@ -1285,21 +1295,21 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="11">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="1"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D23" s="4">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="5"/>
@@ -1307,21 +1317,21 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="11">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" si="1"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D24" s="4">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
@@ -1329,21 +1339,21 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="11">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" si="1"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D25" s="4">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
@@ -1351,21 +1361,21 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="11">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="1"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D26" s="4">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5"/>
@@ -1373,21 +1383,21 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="11">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="1"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D27" s="4">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5"/>
@@ -1395,21 +1405,21 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="11">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="1"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D28" s="4">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="5"/>
@@ -1417,21 +1427,21 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="11">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="1"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D29" s="4">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5"/>
@@ -1439,21 +1449,21 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="11">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="1"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D30" s="4">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
@@ -1461,21 +1471,21 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="11">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="1"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D31" s="4">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="5"/>
@@ -1483,21 +1493,21 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="11">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="1"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D32" s="4">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5"/>
@@ -1505,21 +1515,21 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="11">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="1"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D33" s="4">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5"/>
@@ -1527,21 +1537,21 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="11">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="1"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D34" s="4">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="5"/>
@@ -1549,21 +1559,21 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="11">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="1"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D35" s="4">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="5"/>
@@ -1571,21 +1581,21 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="11">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="1"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D36" s="4">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="5"/>
@@ -1593,21 +1603,21 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="11">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="1"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D37" s="4">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
@@ -1615,67 +1625,66 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="11">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="1"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D38" s="4">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A39" s="13">
-        <v>44305</v>
-      </c>
-      <c r="B39" s="10" t="str">
-        <f t="shared" ref="B39:B42" si="2">"("&amp;TEXT(A39,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A39" s="11">
+        <v>44306</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="1"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D39" s="4">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A40" s="11">
-        <v>44302</v>
+      <c r="A40" s="13">
+        <v>44305</v>
       </c>
       <c r="B40" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>(金)</v>
+        <f t="shared" ref="B40:B43" si="2">"("&amp;TEXT(A40,"aaa")&amp;")"</f>
+        <v>(月)</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="1"/>
-        <v>69687</v>
+        <v>119032</v>
       </c>
       <c r="D40" s="4">
-        <v>29696</v>
+        <v>64725</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4">
-        <v>39991</v>
+        <v>54307</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="5"/>
@@ -1683,22 +1692,22 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="11">
-        <v>44301</v>
+        <v>44302</v>
       </c>
       <c r="B41" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(木)</v>
+        <v>(金)</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="1"/>
-        <v>52620</v>
+        <v>69687</v>
       </c>
       <c r="D41" s="4">
-        <v>16637</v>
+        <v>29696</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4">
-        <v>35983</v>
+        <v>39991</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="5"/>
@@ -1706,45 +1715,45 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42" s="11">
-        <v>44300</v>
+        <v>44301</v>
       </c>
       <c r="B42" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(水)</v>
+        <v>(木)</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" si="1"/>
-        <v>50996</v>
+        <v>52620</v>
       </c>
       <c r="D42" s="4">
-        <v>9569</v>
+        <v>16637</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4">
-        <v>41427</v>
+        <v>35983</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A43" s="8">
-        <v>44299</v>
+      <c r="A43" s="11">
+        <v>44300</v>
       </c>
       <c r="B43" s="10" t="str">
-        <f t="shared" ref="B43:B44" si="3">"("&amp;TEXT(A43,"aaa")&amp;")"</f>
-        <v>(火)</v>
+        <f t="shared" si="2"/>
+        <v>(水)</v>
       </c>
       <c r="C43" s="4">
-        <f t="shared" ref="C43:C44" si="4">SUM(D43:G43)</f>
-        <v>53986</v>
+        <f t="shared" si="1"/>
+        <v>50996</v>
       </c>
       <c r="D43" s="4">
-        <v>13896</v>
+        <v>9569</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4">
-        <v>40090</v>
+        <v>41427</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="5"/>
@@ -1752,86 +1761,109 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44" s="8">
-        <v>44298</v>
+        <v>44299</v>
       </c>
       <c r="B44" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>(月)</v>
+        <f t="shared" ref="B44:B45" si="3">"("&amp;TEXT(A44,"aaa")&amp;")"</f>
+        <v>(火)</v>
       </c>
       <c r="C44" s="4">
-        <f t="shared" si="4"/>
-        <v>96936</v>
+        <f t="shared" ref="C44:C45" si="4">SUM(D44:G44)</f>
+        <v>53986</v>
       </c>
       <c r="D44" s="4">
-        <v>26850</v>
+        <v>13896</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4">
-        <v>70086</v>
+        <v>40090</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A45" s="6"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="5"/>
+      <c r="A45" s="8">
+        <v>44298</v>
+      </c>
+      <c r="B45" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>(月)</v>
+      </c>
+      <c r="C45" s="4">
+        <f t="shared" si="4"/>
+        <v>96936</v>
+      </c>
+      <c r="D45" s="4">
+        <v>26850</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4">
+        <v>70086</v>
+      </c>
+      <c r="G45" s="4"/>
       <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="6"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A47" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="5"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="3"/>
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
         <v>6</v>
       </c>
-      <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A49" s="1" t="s">
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
         <v>3</v>
       </c>
-      <c r="H50" s="5"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="H51" s="3"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A53" s="1"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="H52" s="3"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A54" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Flat: latest data (2021-06-14T06:19:00.211Z) {   "date": "2021-06-14T06:19:00.211Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 72,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data2.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -10,14 +10,14 @@
     <sheet name="医療従事者" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$52</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t> 内１回目</t>
   </si>
@@ -282,7 +282,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（6月10日時点）</t>
+    <t>（6月11日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -394,7 +394,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -439,6 +439,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -772,7 +778,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -800,30 +806,30 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="26"/>
+      <c r="G3" s="28"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="26"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="26"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="14" t="s">
         <v>25</v>
       </c>
@@ -840,22 +846,22 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C12" si="0">SUM(D5:G5)</f>
-        <v>8959914</v>
+        <f t="shared" ref="C5:C13" si="0">SUM(D5:G5)</f>
+        <v>9107897</v>
       </c>
       <c r="D5" s="4">
-        <v>5141243</v>
+        <v>5196077</v>
       </c>
       <c r="E5" s="4">
-        <v>9078</v>
+        <v>10747</v>
       </c>
       <c r="F5" s="4">
-        <v>3809593</v>
+        <v>3901073</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -864,24 +870,24 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="23">
-        <v>44357</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>20</v>
+      <c r="A6" s="25">
+        <v>44358</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>19</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>136591</v>
+        <v>147983</v>
       </c>
       <c r="D6" s="4">
-        <v>52250</v>
+        <v>54834</v>
       </c>
       <c r="E6" s="4">
-        <v>1719</v>
+        <v>1669</v>
       </c>
       <c r="F6" s="4">
-        <v>82622</v>
+        <v>91480</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -890,24 +896,24 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="21">
-        <v>44356</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>18</v>
+      <c r="A7" s="23">
+        <v>44357</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>20</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>167384</v>
+        <v>136591</v>
       </c>
       <c r="D7" s="4">
-        <v>67694</v>
+        <v>52250</v>
       </c>
       <c r="E7" s="4">
-        <v>1047</v>
+        <v>1719</v>
       </c>
       <c r="F7" s="4">
-        <v>98643</v>
+        <v>82622</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -916,24 +922,24 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="19">
-        <v>44355</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>27</v>
+      <c r="A8" s="21">
+        <v>44356</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>161922</v>
+        <v>167384</v>
       </c>
       <c r="D8" s="4">
-        <v>71689</v>
+        <v>67694</v>
       </c>
       <c r="E8" s="4">
-        <v>990</v>
+        <v>1047</v>
       </c>
       <c r="F8" s="4">
-        <v>89243</v>
+        <v>98643</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -942,24 +948,24 @@
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="17">
-        <v>44354</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>21</v>
+      <c r="A9" s="19">
+        <v>44355</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>239337</v>
+        <v>161922</v>
       </c>
       <c r="D9" s="4">
-        <v>104435</v>
+        <v>71689</v>
       </c>
       <c r="E9" s="4">
-        <v>2146</v>
+        <v>990</v>
       </c>
       <c r="F9" s="4">
-        <v>132756</v>
+        <v>89243</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -968,24 +974,24 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="15">
-        <v>44351</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>19</v>
+      <c r="A10" s="17">
+        <v>44354</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
-        <v>159203</v>
+        <v>239337</v>
       </c>
       <c r="D10" s="4">
-        <v>62634</v>
+        <v>104435</v>
       </c>
       <c r="E10" s="4">
-        <v>929</v>
+        <v>2146</v>
       </c>
       <c r="F10" s="4">
-        <v>95640</v>
+        <v>132756</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -994,24 +1000,24 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="11">
-        <v>44350</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>20</v>
+      <c r="A11" s="15">
+        <v>44351</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
-        <v>143157</v>
+        <v>159203</v>
       </c>
       <c r="D11" s="4">
-        <v>59654</v>
+        <v>62634</v>
       </c>
       <c r="E11" s="4">
-        <v>112</v>
+        <v>929</v>
       </c>
       <c r="F11" s="4">
-        <v>83391</v>
+        <v>95640</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -1021,23 +1027,23 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="11">
-        <v>44349</v>
+        <v>44350</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
-        <v>159126</v>
+        <v>143157</v>
       </c>
       <c r="D12" s="4">
-        <v>71140</v>
+        <v>59654</v>
       </c>
       <c r="E12" s="4">
-        <v>316</v>
+        <v>112</v>
       </c>
       <c r="F12" s="4">
-        <v>87670</v>
+        <v>83391</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -1047,23 +1053,23 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="11">
-        <v>44348</v>
+        <v>44349</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C13" s="4">
-        <f t="shared" ref="C13:C43" si="1">SUM(D13:G13)</f>
-        <v>159057</v>
+        <f t="shared" si="0"/>
+        <v>159126</v>
       </c>
       <c r="D13" s="4">
-        <v>66264</v>
+        <v>71140</v>
       </c>
       <c r="E13" s="4">
-        <v>123</v>
+        <v>316</v>
       </c>
       <c r="F13" s="4">
-        <v>92670</v>
+        <v>87670</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -1073,23 +1079,23 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="11">
-        <v>44347</v>
+        <v>44348</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C14" s="4">
-        <f t="shared" si="1"/>
-        <v>273255</v>
+        <f t="shared" ref="C14:C44" si="1">SUM(D14:G14)</f>
+        <v>159057</v>
       </c>
       <c r="D14" s="4">
-        <v>131423</v>
+        <v>66264</v>
       </c>
       <c r="E14" s="4">
-        <v>582</v>
+        <v>123</v>
       </c>
       <c r="F14" s="4">
-        <v>141250</v>
+        <v>92670</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -1099,23 +1105,23 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="11">
-        <v>44344</v>
+        <v>44347</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="1"/>
-        <v>164516</v>
+        <v>273255</v>
       </c>
       <c r="D15" s="4">
-        <v>87584</v>
+        <v>131423</v>
       </c>
       <c r="E15" s="4">
-        <v>157</v>
+        <v>582</v>
       </c>
       <c r="F15" s="4">
-        <v>76775</v>
+        <v>141250</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
@@ -1125,23 +1131,23 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="11">
-        <v>44343</v>
+        <v>44344</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="1"/>
-        <v>145149</v>
+        <v>164516</v>
       </c>
       <c r="D16" s="4">
-        <v>84217</v>
+        <v>87584</v>
       </c>
       <c r="E16" s="4">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="F16" s="4">
-        <v>60892</v>
+        <v>76775</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
@@ -1151,23 +1157,23 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="11">
-        <v>44342</v>
+        <v>44343</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="1"/>
-        <v>142589</v>
+        <v>145149</v>
       </c>
       <c r="D17" s="4">
-        <v>93243</v>
+        <v>84217</v>
       </c>
       <c r="E17" s="4">
-        <v>172</v>
+        <v>40</v>
       </c>
       <c r="F17" s="4">
-        <v>49174</v>
+        <v>60892</v>
       </c>
       <c r="G17" s="4">
         <v>0</v>
@@ -1177,23 +1183,23 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="11">
-        <v>44341</v>
+        <v>44342</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="1"/>
-        <v>139652</v>
+        <v>142589</v>
       </c>
       <c r="D18" s="4">
-        <v>87114</v>
+        <v>93243</v>
       </c>
       <c r="E18" s="4">
-        <v>476</v>
+        <v>172</v>
       </c>
       <c r="F18" s="4">
-        <v>52062</v>
+        <v>49174</v>
       </c>
       <c r="G18" s="4">
         <v>0</v>
@@ -1203,23 +1209,23 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="11">
-        <v>44340</v>
+        <v>44341</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="1"/>
-        <v>330589</v>
+        <v>139652</v>
       </c>
       <c r="D19" s="4">
-        <v>136491</v>
+        <v>87114</v>
       </c>
       <c r="E19" s="4">
-        <v>269</v>
+        <v>476</v>
       </c>
       <c r="F19" s="4">
-        <v>193829</v>
+        <v>52062</v>
       </c>
       <c r="G19" s="4">
         <v>0</v>
@@ -1229,43 +1235,47 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="11">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="1"/>
-        <v>249021</v>
+        <v>330589</v>
       </c>
       <c r="D20" s="4">
-        <v>99918</v>
-      </c>
-      <c r="E20" s="4"/>
+        <v>136491</v>
+      </c>
+      <c r="E20" s="4">
+        <v>269</v>
+      </c>
       <c r="F20" s="4">
-        <v>149103</v>
-      </c>
-      <c r="G20" s="4"/>
+        <v>193829</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="11">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="1"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D21" s="4">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="5"/>
@@ -1273,21 +1283,21 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="11">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="1"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D22" s="4">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>
@@ -1295,21 +1305,21 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="11">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="1"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D23" s="4">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="5"/>
@@ -1317,21 +1327,21 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="11">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" si="1"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D24" s="4">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
@@ -1339,21 +1349,21 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="11">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" si="1"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D25" s="4">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
@@ -1361,21 +1371,21 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="11">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="1"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D26" s="4">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5"/>
@@ -1383,21 +1393,21 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="11">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="1"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D27" s="4">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5"/>
@@ -1405,21 +1415,21 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="11">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="1"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D28" s="4">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="5"/>
@@ -1427,21 +1437,21 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="11">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="1"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D29" s="4">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5"/>
@@ -1449,21 +1459,21 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="11">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="1"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D30" s="4">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
@@ -1471,21 +1481,21 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="11">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="1"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D31" s="4">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="5"/>
@@ -1493,21 +1503,21 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="11">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="1"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D32" s="4">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5"/>
@@ -1515,21 +1525,21 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="11">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="1"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D33" s="4">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5"/>
@@ -1537,21 +1547,21 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="11">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="1"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D34" s="4">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="5"/>
@@ -1559,21 +1569,21 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="11">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="1"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D35" s="4">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="5"/>
@@ -1581,21 +1591,21 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="11">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="1"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D36" s="4">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="5"/>
@@ -1603,21 +1613,21 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="11">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="1"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D37" s="4">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
@@ -1625,21 +1635,21 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="11">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="1"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D38" s="4">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="5"/>
@@ -1647,67 +1657,66 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="11">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="1"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D39" s="4">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A40" s="13">
-        <v>44305</v>
-      </c>
-      <c r="B40" s="10" t="str">
-        <f t="shared" ref="B40:B43" si="2">"("&amp;TEXT(A40,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A40" s="11">
+        <v>44306</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="1"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D40" s="4">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A41" s="11">
-        <v>44302</v>
+      <c r="A41" s="13">
+        <v>44305</v>
       </c>
       <c r="B41" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>(金)</v>
+        <f t="shared" ref="B41:B44" si="2">"("&amp;TEXT(A41,"aaa")&amp;")"</f>
+        <v>(月)</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="1"/>
-        <v>69687</v>
+        <v>119032</v>
       </c>
       <c r="D41" s="4">
-        <v>29696</v>
+        <v>64725</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4">
-        <v>39991</v>
+        <v>54307</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="5"/>
@@ -1715,22 +1724,22 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42" s="11">
-        <v>44301</v>
+        <v>44302</v>
       </c>
       <c r="B42" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(木)</v>
+        <v>(金)</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" si="1"/>
-        <v>52620</v>
+        <v>69687</v>
       </c>
       <c r="D42" s="4">
-        <v>16637</v>
+        <v>29696</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4">
-        <v>35983</v>
+        <v>39991</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="5"/>
@@ -1738,45 +1747,45 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43" s="11">
-        <v>44300</v>
+        <v>44301</v>
       </c>
       <c r="B43" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(水)</v>
+        <v>(木)</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" si="1"/>
-        <v>50996</v>
+        <v>52620</v>
       </c>
       <c r="D43" s="4">
-        <v>9569</v>
+        <v>16637</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4">
-        <v>41427</v>
+        <v>35983</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A44" s="8">
-        <v>44299</v>
+      <c r="A44" s="11">
+        <v>44300</v>
       </c>
       <c r="B44" s="10" t="str">
-        <f t="shared" ref="B44:B45" si="3">"("&amp;TEXT(A44,"aaa")&amp;")"</f>
-        <v>(火)</v>
+        <f t="shared" si="2"/>
+        <v>(水)</v>
       </c>
       <c r="C44" s="4">
-        <f t="shared" ref="C44:C45" si="4">SUM(D44:G44)</f>
-        <v>53986</v>
+        <f t="shared" si="1"/>
+        <v>50996</v>
       </c>
       <c r="D44" s="4">
-        <v>13896</v>
+        <v>9569</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4">
-        <v>40090</v>
+        <v>41427</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="5"/>
@@ -1784,86 +1793,109 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A45" s="8">
-        <v>44298</v>
+        <v>44299</v>
       </c>
       <c r="B45" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>(月)</v>
+        <f t="shared" ref="B45:B46" si="3">"("&amp;TEXT(A45,"aaa")&amp;")"</f>
+        <v>(火)</v>
       </c>
       <c r="C45" s="4">
-        <f t="shared" si="4"/>
-        <v>96936</v>
+        <f t="shared" ref="C45:C46" si="4">SUM(D45:G45)</f>
+        <v>53986</v>
       </c>
       <c r="D45" s="4">
-        <v>26850</v>
+        <v>13896</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4">
-        <v>70086</v>
+        <v>40090</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A46" s="6"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="5"/>
+      <c r="A46" s="8">
+        <v>44298</v>
+      </c>
+      <c r="B46" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>(月)</v>
+      </c>
+      <c r="C46" s="4">
+        <f t="shared" si="4"/>
+        <v>96936</v>
+      </c>
+      <c r="D46" s="4">
+        <v>26850</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4">
+        <v>70086</v>
+      </c>
+      <c r="G46" s="4"/>
       <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="6"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A48" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="5"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="3"/>
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
         <v>6</v>
       </c>
-      <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A50" s="1" t="s">
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H50" s="5"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
         <v>3</v>
       </c>
-      <c r="H51" s="5"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="H52" s="3"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A54" s="1"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="H53" s="3"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A55" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Flat: latest data (2021-06-15T06:18:54.616Z) {   "date": "2021-06-15T06:18:54.616Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 84,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data2.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -10,14 +10,14 @@
     <sheet name="医療従事者" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$53</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t> 内１回目</t>
   </si>
@@ -282,7 +282,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（6月11日時点）</t>
+    <t>（6月14日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -394,7 +394,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -439,6 +439,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -778,7 +784,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -806,30 +812,30 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29" t="s">
+      <c r="E3" s="30"/>
+      <c r="F3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="30"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="28"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="14" t="s">
         <v>25</v>
       </c>
@@ -846,22 +852,22 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C13" si="0">SUM(D5:G5)</f>
-        <v>9107897</v>
+        <f t="shared" ref="C5:C14" si="0">SUM(D5:G5)</f>
+        <v>9322862</v>
       </c>
       <c r="D5" s="4">
-        <v>5196077</v>
+        <v>5281896</v>
       </c>
       <c r="E5" s="4">
-        <v>10747</v>
+        <v>16357</v>
       </c>
       <c r="F5" s="4">
-        <v>3901073</v>
+        <v>4024609</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -870,24 +876,24 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="25">
-        <v>44358</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>19</v>
+      <c r="A6" s="27">
+        <v>44361</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>147983</v>
+        <v>214965</v>
       </c>
       <c r="D6" s="4">
-        <v>54834</v>
+        <v>85819</v>
       </c>
       <c r="E6" s="4">
-        <v>1669</v>
+        <v>5610</v>
       </c>
       <c r="F6" s="4">
-        <v>91480</v>
+        <v>123536</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -896,24 +902,24 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="23">
-        <v>44357</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>20</v>
+      <c r="A7" s="25">
+        <v>44358</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>19</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>136591</v>
+        <v>147983</v>
       </c>
       <c r="D7" s="4">
-        <v>52250</v>
+        <v>54834</v>
       </c>
       <c r="E7" s="4">
-        <v>1719</v>
+        <v>1669</v>
       </c>
       <c r="F7" s="4">
-        <v>82622</v>
+        <v>91480</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -922,24 +928,24 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="21">
-        <v>44356</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>18</v>
+      <c r="A8" s="23">
+        <v>44357</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>20</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>167384</v>
+        <v>136591</v>
       </c>
       <c r="D8" s="4">
-        <v>67694</v>
+        <v>52250</v>
       </c>
       <c r="E8" s="4">
-        <v>1047</v>
+        <v>1719</v>
       </c>
       <c r="F8" s="4">
-        <v>98643</v>
+        <v>82622</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -948,24 +954,24 @@
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="19">
-        <v>44355</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>27</v>
+      <c r="A9" s="21">
+        <v>44356</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>161922</v>
+        <v>167384</v>
       </c>
       <c r="D9" s="4">
-        <v>71689</v>
+        <v>67694</v>
       </c>
       <c r="E9" s="4">
-        <v>990</v>
+        <v>1047</v>
       </c>
       <c r="F9" s="4">
-        <v>89243</v>
+        <v>98643</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -974,24 +980,24 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="17">
-        <v>44354</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>21</v>
+      <c r="A10" s="19">
+        <v>44355</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
-        <v>239337</v>
+        <v>161922</v>
       </c>
       <c r="D10" s="4">
-        <v>104435</v>
+        <v>71689</v>
       </c>
       <c r="E10" s="4">
-        <v>2146</v>
+        <v>990</v>
       </c>
       <c r="F10" s="4">
-        <v>132756</v>
+        <v>89243</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -1000,24 +1006,24 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="15">
-        <v>44351</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>19</v>
+      <c r="A11" s="17">
+        <v>44354</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
-        <v>159203</v>
+        <v>239337</v>
       </c>
       <c r="D11" s="4">
-        <v>62634</v>
+        <v>104435</v>
       </c>
       <c r="E11" s="4">
-        <v>929</v>
+        <v>2146</v>
       </c>
       <c r="F11" s="4">
-        <v>95640</v>
+        <v>132756</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -1026,24 +1032,24 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="11">
-        <v>44350</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>20</v>
+      <c r="A12" s="15">
+        <v>44351</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
-        <v>143157</v>
+        <v>159203</v>
       </c>
       <c r="D12" s="4">
-        <v>59654</v>
+        <v>62634</v>
       </c>
       <c r="E12" s="4">
-        <v>112</v>
+        <v>929</v>
       </c>
       <c r="F12" s="4">
-        <v>83391</v>
+        <v>95640</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -1053,23 +1059,23 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="11">
-        <v>44349</v>
+        <v>44350</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="0"/>
-        <v>159126</v>
+        <v>143157</v>
       </c>
       <c r="D13" s="4">
-        <v>71140</v>
+        <v>59654</v>
       </c>
       <c r="E13" s="4">
-        <v>316</v>
+        <v>112</v>
       </c>
       <c r="F13" s="4">
-        <v>87670</v>
+        <v>83391</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -1079,23 +1085,23 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="11">
-        <v>44348</v>
+        <v>44349</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C14" s="4">
-        <f t="shared" ref="C14:C44" si="1">SUM(D14:G14)</f>
-        <v>159057</v>
+        <f t="shared" si="0"/>
+        <v>159126</v>
       </c>
       <c r="D14" s="4">
-        <v>66264</v>
+        <v>71140</v>
       </c>
       <c r="E14" s="4">
-        <v>123</v>
+        <v>316</v>
       </c>
       <c r="F14" s="4">
-        <v>92670</v>
+        <v>87670</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -1105,23 +1111,23 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="11">
-        <v>44347</v>
+        <v>44348</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C15" s="4">
-        <f t="shared" si="1"/>
-        <v>273255</v>
+        <f t="shared" ref="C15:C45" si="1">SUM(D15:G15)</f>
+        <v>159057</v>
       </c>
       <c r="D15" s="4">
-        <v>131423</v>
+        <v>66264</v>
       </c>
       <c r="E15" s="4">
-        <v>582</v>
+        <v>123</v>
       </c>
       <c r="F15" s="4">
-        <v>141250</v>
+        <v>92670</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
@@ -1131,23 +1137,23 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="11">
-        <v>44344</v>
+        <v>44347</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="1"/>
-        <v>164516</v>
+        <v>273255</v>
       </c>
       <c r="D16" s="4">
-        <v>87584</v>
+        <v>131423</v>
       </c>
       <c r="E16" s="4">
-        <v>157</v>
+        <v>582</v>
       </c>
       <c r="F16" s="4">
-        <v>76775</v>
+        <v>141250</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
@@ -1157,23 +1163,23 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="11">
-        <v>44343</v>
+        <v>44344</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="1"/>
-        <v>145149</v>
+        <v>164516</v>
       </c>
       <c r="D17" s="4">
-        <v>84217</v>
+        <v>87584</v>
       </c>
       <c r="E17" s="4">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="F17" s="4">
-        <v>60892</v>
+        <v>76775</v>
       </c>
       <c r="G17" s="4">
         <v>0</v>
@@ -1183,23 +1189,23 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="11">
-        <v>44342</v>
+        <v>44343</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="1"/>
-        <v>142589</v>
+        <v>145149</v>
       </c>
       <c r="D18" s="4">
-        <v>93243</v>
+        <v>84217</v>
       </c>
       <c r="E18" s="4">
-        <v>172</v>
+        <v>40</v>
       </c>
       <c r="F18" s="4">
-        <v>49174</v>
+        <v>60892</v>
       </c>
       <c r="G18" s="4">
         <v>0</v>
@@ -1209,23 +1215,23 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="11">
-        <v>44341</v>
+        <v>44342</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="1"/>
-        <v>139652</v>
+        <v>142589</v>
       </c>
       <c r="D19" s="4">
-        <v>87114</v>
+        <v>93243</v>
       </c>
       <c r="E19" s="4">
-        <v>476</v>
+        <v>172</v>
       </c>
       <c r="F19" s="4">
-        <v>52062</v>
+        <v>49174</v>
       </c>
       <c r="G19" s="4">
         <v>0</v>
@@ -1235,23 +1241,23 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="11">
-        <v>44340</v>
+        <v>44341</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="1"/>
-        <v>330589</v>
+        <v>139652</v>
       </c>
       <c r="D20" s="4">
-        <v>136491</v>
+        <v>87114</v>
       </c>
       <c r="E20" s="4">
-        <v>269</v>
+        <v>476</v>
       </c>
       <c r="F20" s="4">
-        <v>193829</v>
+        <v>52062</v>
       </c>
       <c r="G20" s="4">
         <v>0</v>
@@ -1261,43 +1267,47 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="11">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="1"/>
-        <v>249021</v>
+        <v>330589</v>
       </c>
       <c r="D21" s="4">
-        <v>99918</v>
-      </c>
-      <c r="E21" s="4"/>
+        <v>136491</v>
+      </c>
+      <c r="E21" s="4">
+        <v>269</v>
+      </c>
       <c r="F21" s="4">
-        <v>149103</v>
-      </c>
-      <c r="G21" s="4"/>
+        <v>193829</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="11">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="1"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D22" s="4">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>
@@ -1305,21 +1315,21 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="11">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="1"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D23" s="4">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="5"/>
@@ -1327,21 +1337,21 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="11">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" si="1"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D24" s="4">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
@@ -1349,21 +1359,21 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="11">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" si="1"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D25" s="4">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
@@ -1371,21 +1381,21 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="11">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="1"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D26" s="4">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5"/>
@@ -1393,21 +1403,21 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="11">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="1"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D27" s="4">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5"/>
@@ -1415,21 +1425,21 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="11">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="1"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D28" s="4">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="5"/>
@@ -1437,21 +1447,21 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="11">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="1"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D29" s="4">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5"/>
@@ -1459,21 +1469,21 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="11">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="1"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D30" s="4">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
@@ -1481,21 +1491,21 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="11">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="1"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D31" s="4">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="5"/>
@@ -1503,21 +1513,21 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="11">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="1"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D32" s="4">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5"/>
@@ -1525,21 +1535,21 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="11">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="1"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D33" s="4">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5"/>
@@ -1547,21 +1557,21 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="11">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="1"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D34" s="4">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="5"/>
@@ -1569,21 +1579,21 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="11">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="1"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D35" s="4">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="5"/>
@@ -1591,21 +1601,21 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="11">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="1"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D36" s="4">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="5"/>
@@ -1613,21 +1623,21 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="11">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="1"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D37" s="4">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
@@ -1635,21 +1645,21 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="11">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="1"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D38" s="4">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="5"/>
@@ -1657,21 +1667,21 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="11">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="1"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D39" s="4">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="5"/>
@@ -1679,67 +1689,66 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="11">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="1"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D40" s="4">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A41" s="13">
-        <v>44305</v>
-      </c>
-      <c r="B41" s="10" t="str">
-        <f t="shared" ref="B41:B44" si="2">"("&amp;TEXT(A41,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A41" s="11">
+        <v>44306</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="1"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D41" s="4">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A42" s="11">
-        <v>44302</v>
+      <c r="A42" s="13">
+        <v>44305</v>
       </c>
       <c r="B42" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>(金)</v>
+        <f t="shared" ref="B42:B45" si="2">"("&amp;TEXT(A42,"aaa")&amp;")"</f>
+        <v>(月)</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" si="1"/>
-        <v>69687</v>
+        <v>119032</v>
       </c>
       <c r="D42" s="4">
-        <v>29696</v>
+        <v>64725</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4">
-        <v>39991</v>
+        <v>54307</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="5"/>
@@ -1747,22 +1756,22 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43" s="11">
-        <v>44301</v>
+        <v>44302</v>
       </c>
       <c r="B43" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(木)</v>
+        <v>(金)</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" si="1"/>
-        <v>52620</v>
+        <v>69687</v>
       </c>
       <c r="D43" s="4">
-        <v>16637</v>
+        <v>29696</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4">
-        <v>35983</v>
+        <v>39991</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="5"/>
@@ -1770,45 +1779,45 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44" s="11">
-        <v>44300</v>
+        <v>44301</v>
       </c>
       <c r="B44" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(水)</v>
+        <v>(木)</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" si="1"/>
-        <v>50996</v>
+        <v>52620</v>
       </c>
       <c r="D44" s="4">
-        <v>9569</v>
+        <v>16637</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4">
-        <v>41427</v>
+        <v>35983</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A45" s="8">
-        <v>44299</v>
+      <c r="A45" s="11">
+        <v>44300</v>
       </c>
       <c r="B45" s="10" t="str">
-        <f t="shared" ref="B45:B46" si="3">"("&amp;TEXT(A45,"aaa")&amp;")"</f>
-        <v>(火)</v>
+        <f t="shared" si="2"/>
+        <v>(水)</v>
       </c>
       <c r="C45" s="4">
-        <f t="shared" ref="C45:C46" si="4">SUM(D45:G45)</f>
-        <v>53986</v>
+        <f t="shared" si="1"/>
+        <v>50996</v>
       </c>
       <c r="D45" s="4">
-        <v>13896</v>
+        <v>9569</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4">
-        <v>40090</v>
+        <v>41427</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="5"/>
@@ -1816,86 +1825,109 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A46" s="8">
-        <v>44298</v>
+        <v>44299</v>
       </c>
       <c r="B46" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>(月)</v>
+        <f t="shared" ref="B46:B47" si="3">"("&amp;TEXT(A46,"aaa")&amp;")"</f>
+        <v>(火)</v>
       </c>
       <c r="C46" s="4">
-        <f t="shared" si="4"/>
-        <v>96936</v>
+        <f t="shared" ref="C46:C47" si="4">SUM(D46:G46)</f>
+        <v>53986</v>
       </c>
       <c r="D46" s="4">
-        <v>26850</v>
+        <v>13896</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4">
-        <v>70086</v>
+        <v>40090</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A47" s="6"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="5"/>
+      <c r="A47" s="8">
+        <v>44298</v>
+      </c>
+      <c r="B47" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>(月)</v>
+      </c>
+      <c r="C47" s="4">
+        <f t="shared" si="4"/>
+        <v>96936</v>
+      </c>
+      <c r="D47" s="4">
+        <v>26850</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4">
+        <v>70086</v>
+      </c>
+      <c r="G47" s="4"/>
       <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A48" s="12" t="s">
+      <c r="A48" s="6"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A49" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A49" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="3"/>
       <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
         <v>6</v>
       </c>
-      <c r="H50" s="5"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A51" s="1" t="s">
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H51" s="5"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
         <v>3</v>
       </c>
-      <c r="H52" s="5"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="H53" s="3"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A55" s="1"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="H54" s="3"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A56" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Flat: latest data (2021-06-17T06:19:17.786Z) {   "date": "2021-06-17T06:19:17.786Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 139,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data2.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -10,14 +10,14 @@
     <sheet name="医療従事者" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$55</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
   <si>
     <t> 内１回目</t>
   </si>
@@ -282,7 +282,11 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（6月14日時点）</t>
+    <t>(火)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>（6月16日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -394,7 +398,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -439,6 +443,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -784,7 +800,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -808,34 +824,34 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="G2" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31" t="s">
+      <c r="E3" s="34"/>
+      <c r="F3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="30"/>
+      <c r="G3" s="34"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="30"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="14" t="s">
         <v>25</v>
       </c>
@@ -852,22 +868,22 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="30"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C14" si="0">SUM(D5:G5)</f>
-        <v>9322862</v>
+        <f t="shared" ref="C5:C16" si="0">SUM(D5:G5)</f>
+        <v>9556960</v>
       </c>
       <c r="D5" s="4">
-        <v>5281896</v>
+        <v>5366267</v>
       </c>
       <c r="E5" s="4">
-        <v>16357</v>
+        <v>22095</v>
       </c>
       <c r="F5" s="4">
-        <v>4024609</v>
+        <v>4168598</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -876,24 +892,24 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="27">
-        <v>44361</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>21</v>
+      <c r="A6" s="31">
+        <v>44363</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>18</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>214965</v>
+        <v>118735</v>
       </c>
       <c r="D6" s="4">
-        <v>85819</v>
+        <v>43912</v>
       </c>
       <c r="E6" s="4">
-        <v>5610</v>
+        <v>2782</v>
       </c>
       <c r="F6" s="4">
-        <v>123536</v>
+        <v>72041</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -902,24 +918,24 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="25">
-        <v>44358</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>19</v>
+      <c r="A7" s="29">
+        <v>44362</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>28</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>147983</v>
+        <v>115363</v>
       </c>
       <c r="D7" s="4">
-        <v>54834</v>
+        <v>40459</v>
       </c>
       <c r="E7" s="4">
-        <v>1669</v>
+        <v>2956</v>
       </c>
       <c r="F7" s="4">
-        <v>91480</v>
+        <v>71948</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -928,24 +944,24 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="23">
-        <v>44357</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>20</v>
+      <c r="A8" s="27">
+        <v>44361</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>21</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>136591</v>
+        <v>214965</v>
       </c>
       <c r="D8" s="4">
-        <v>52250</v>
+        <v>85819</v>
       </c>
       <c r="E8" s="4">
-        <v>1719</v>
+        <v>5610</v>
       </c>
       <c r="F8" s="4">
-        <v>82622</v>
+        <v>123536</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -954,24 +970,24 @@
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="21">
-        <v>44356</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>18</v>
+      <c r="A9" s="25">
+        <v>44358</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>19</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>167384</v>
+        <v>147983</v>
       </c>
       <c r="D9" s="4">
-        <v>67694</v>
+        <v>54834</v>
       </c>
       <c r="E9" s="4">
-        <v>1047</v>
+        <v>1669</v>
       </c>
       <c r="F9" s="4">
-        <v>98643</v>
+        <v>91480</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -980,24 +996,24 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="19">
-        <v>44355</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>27</v>
+      <c r="A10" s="23">
+        <v>44357</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>20</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
-        <v>161922</v>
+        <v>136591</v>
       </c>
       <c r="D10" s="4">
-        <v>71689</v>
+        <v>52250</v>
       </c>
       <c r="E10" s="4">
-        <v>990</v>
+        <v>1719</v>
       </c>
       <c r="F10" s="4">
-        <v>89243</v>
+        <v>82622</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -1006,24 +1022,24 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="17">
-        <v>44354</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>21</v>
+      <c r="A11" s="21">
+        <v>44356</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
-        <v>239337</v>
+        <v>167384</v>
       </c>
       <c r="D11" s="4">
-        <v>104435</v>
+        <v>67694</v>
       </c>
       <c r="E11" s="4">
-        <v>2146</v>
+        <v>1047</v>
       </c>
       <c r="F11" s="4">
-        <v>132756</v>
+        <v>98643</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -1032,24 +1048,24 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="15">
-        <v>44351</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>19</v>
+      <c r="A12" s="19">
+        <v>44355</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
-        <v>159203</v>
+        <v>161922</v>
       </c>
       <c r="D12" s="4">
-        <v>62634</v>
+        <v>71689</v>
       </c>
       <c r="E12" s="4">
-        <v>929</v>
+        <v>990</v>
       </c>
       <c r="F12" s="4">
-        <v>95640</v>
+        <v>89243</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -1058,24 +1074,24 @@
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A13" s="11">
-        <v>44350</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>20</v>
+      <c r="A13" s="17">
+        <v>44354</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="0"/>
-        <v>143157</v>
+        <v>239337</v>
       </c>
       <c r="D13" s="4">
-        <v>59654</v>
+        <v>104435</v>
       </c>
       <c r="E13" s="4">
-        <v>112</v>
+        <v>2146</v>
       </c>
       <c r="F13" s="4">
-        <v>83391</v>
+        <v>132756</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -1084,24 +1100,24 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A14" s="11">
-        <v>44349</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>18</v>
+      <c r="A14" s="15">
+        <v>44351</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="0"/>
-        <v>159126</v>
+        <v>159203</v>
       </c>
       <c r="D14" s="4">
-        <v>71140</v>
+        <v>62634</v>
       </c>
       <c r="E14" s="4">
-        <v>316</v>
+        <v>929</v>
       </c>
       <c r="F14" s="4">
-        <v>87670</v>
+        <v>95640</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -1111,23 +1127,23 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="11">
-        <v>44348</v>
+        <v>44350</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C15" s="4">
-        <f t="shared" ref="C15:C45" si="1">SUM(D15:G15)</f>
-        <v>159057</v>
+        <f t="shared" si="0"/>
+        <v>143157</v>
       </c>
       <c r="D15" s="4">
-        <v>66264</v>
+        <v>59654</v>
       </c>
       <c r="E15" s="4">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F15" s="4">
-        <v>92670</v>
+        <v>83391</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
@@ -1137,23 +1153,23 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="11">
-        <v>44347</v>
+        <v>44349</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C16" s="4">
-        <f t="shared" si="1"/>
-        <v>273255</v>
+        <f t="shared" si="0"/>
+        <v>159126</v>
       </c>
       <c r="D16" s="4">
-        <v>131423</v>
+        <v>71140</v>
       </c>
       <c r="E16" s="4">
-        <v>582</v>
+        <v>316</v>
       </c>
       <c r="F16" s="4">
-        <v>141250</v>
+        <v>87670</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
@@ -1163,23 +1179,23 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="11">
-        <v>44344</v>
+        <v>44348</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C17" s="4">
-        <f t="shared" si="1"/>
-        <v>164516</v>
+        <f t="shared" ref="C17:C47" si="1">SUM(D17:G17)</f>
+        <v>159057</v>
       </c>
       <c r="D17" s="4">
-        <v>87584</v>
+        <v>66264</v>
       </c>
       <c r="E17" s="4">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="F17" s="4">
-        <v>76775</v>
+        <v>92670</v>
       </c>
       <c r="G17" s="4">
         <v>0</v>
@@ -1189,23 +1205,23 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="11">
-        <v>44343</v>
+        <v>44347</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="1"/>
-        <v>145149</v>
+        <v>273255</v>
       </c>
       <c r="D18" s="4">
-        <v>84217</v>
+        <v>131423</v>
       </c>
       <c r="E18" s="4">
-        <v>40</v>
+        <v>582</v>
       </c>
       <c r="F18" s="4">
-        <v>60892</v>
+        <v>141250</v>
       </c>
       <c r="G18" s="4">
         <v>0</v>
@@ -1215,23 +1231,23 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="11">
-        <v>44342</v>
+        <v>44344</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="1"/>
-        <v>142589</v>
+        <v>164516</v>
       </c>
       <c r="D19" s="4">
-        <v>93243</v>
+        <v>87584</v>
       </c>
       <c r="E19" s="4">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="F19" s="4">
-        <v>49174</v>
+        <v>76775</v>
       </c>
       <c r="G19" s="4">
         <v>0</v>
@@ -1241,23 +1257,23 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="11">
-        <v>44341</v>
+        <v>44343</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="1"/>
-        <v>139652</v>
+        <v>145149</v>
       </c>
       <c r="D20" s="4">
-        <v>87114</v>
+        <v>84217</v>
       </c>
       <c r="E20" s="4">
-        <v>476</v>
+        <v>40</v>
       </c>
       <c r="F20" s="4">
-        <v>52062</v>
+        <v>60892</v>
       </c>
       <c r="G20" s="4">
         <v>0</v>
@@ -1267,23 +1283,23 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="11">
-        <v>44340</v>
+        <v>44342</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="1"/>
-        <v>330589</v>
+        <v>142589</v>
       </c>
       <c r="D21" s="4">
-        <v>136491</v>
+        <v>93243</v>
       </c>
       <c r="E21" s="4">
-        <v>269</v>
+        <v>172</v>
       </c>
       <c r="F21" s="4">
-        <v>193829</v>
+        <v>49174</v>
       </c>
       <c r="G21" s="4">
         <v>0</v>
@@ -1293,65 +1309,73 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="11">
-        <v>44337</v>
+        <v>44341</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="1"/>
-        <v>249021</v>
+        <v>139652</v>
       </c>
       <c r="D22" s="4">
-        <v>99918</v>
-      </c>
-      <c r="E22" s="4"/>
+        <v>87114</v>
+      </c>
+      <c r="E22" s="4">
+        <v>476</v>
+      </c>
       <c r="F22" s="4">
-        <v>149103</v>
-      </c>
-      <c r="G22" s="4"/>
+        <v>52062</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0</v>
+      </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="11">
-        <v>44336</v>
+        <v>44340</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="1"/>
-        <v>190533</v>
+        <v>330589</v>
       </c>
       <c r="D23" s="4">
-        <v>81422</v>
-      </c>
-      <c r="E23" s="4"/>
+        <v>136491</v>
+      </c>
+      <c r="E23" s="4">
+        <v>269</v>
+      </c>
       <c r="F23" s="4">
-        <v>109111</v>
-      </c>
-      <c r="G23" s="4"/>
+        <v>193829</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="11">
-        <v>44335</v>
+        <v>44337</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" si="1"/>
-        <v>267866</v>
+        <v>249021</v>
       </c>
       <c r="D24" s="4">
-        <v>88163</v>
+        <v>99918</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4">
-        <v>179703</v>
+        <v>149103</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
@@ -1359,21 +1383,21 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="11">
-        <v>44334</v>
+        <v>44336</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" si="1"/>
-        <v>250244</v>
+        <v>190533</v>
       </c>
       <c r="D25" s="4">
-        <v>94577</v>
+        <v>81422</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4">
-        <v>155667</v>
+        <v>109111</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
@@ -1381,21 +1405,21 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="11">
-        <v>44333</v>
+        <v>44335</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="1"/>
-        <v>349566</v>
+        <v>267866</v>
       </c>
       <c r="D26" s="4">
-        <v>133843</v>
+        <v>88163</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4">
-        <v>215723</v>
+        <v>179703</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5"/>
@@ -1403,21 +1427,21 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="11">
-        <v>44330</v>
+        <v>44334</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="1"/>
-        <v>242878</v>
+        <v>250244</v>
       </c>
       <c r="D27" s="4">
-        <v>99493</v>
+        <v>94577</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4">
-        <v>143385</v>
+        <v>155667</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5"/>
@@ -1425,21 +1449,21 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="11">
-        <v>44329</v>
+        <v>44333</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="1"/>
-        <v>219139</v>
+        <v>349566</v>
       </c>
       <c r="D28" s="4">
-        <v>93429</v>
+        <v>133843</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4">
-        <v>125710</v>
+        <v>215723</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="5"/>
@@ -1447,21 +1471,21 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="11">
-        <v>44328</v>
+        <v>44330</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="1"/>
-        <v>181720</v>
+        <v>242878</v>
       </c>
       <c r="D29" s="4">
-        <v>82959</v>
+        <v>99493</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4">
-        <v>98761</v>
+        <v>143385</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5"/>
@@ -1469,21 +1493,21 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="11">
-        <v>44327</v>
+        <v>44329</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="1"/>
-        <v>168738</v>
+        <v>219139</v>
       </c>
       <c r="D30" s="4">
-        <v>90287</v>
+        <v>93429</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4">
-        <v>78451</v>
+        <v>125710</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
@@ -1491,21 +1515,21 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="11">
-        <v>44326</v>
+        <v>44328</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="1"/>
-        <v>223504</v>
+        <v>181720</v>
       </c>
       <c r="D31" s="4">
-        <v>155255</v>
+        <v>82959</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4">
-        <v>68249</v>
+        <v>98761</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="5"/>
@@ -1513,21 +1537,21 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="11">
-        <v>44323</v>
+        <v>44327</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="1"/>
-        <v>140344</v>
+        <v>168738</v>
       </c>
       <c r="D32" s="4">
-        <v>97165</v>
+        <v>90287</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4">
-        <v>43179</v>
+        <v>78451</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5"/>
@@ -1535,21 +1559,21 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="11">
-        <v>44322</v>
+        <v>44326</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="1"/>
-        <v>331914</v>
+        <v>223504</v>
       </c>
       <c r="D33" s="4">
-        <v>268978</v>
+        <v>155255</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4">
-        <v>62936</v>
+        <v>68249</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5"/>
@@ -1557,21 +1581,21 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="11">
-        <v>44316</v>
+        <v>44323</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="1"/>
-        <v>274907</v>
+        <v>140344</v>
       </c>
       <c r="D34" s="4">
-        <v>227667</v>
+        <v>97165</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4">
-        <v>47240</v>
+        <v>43179</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="5"/>
@@ -1579,21 +1603,21 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="11">
-        <v>44314</v>
+        <v>44322</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="1"/>
-        <v>238273</v>
+        <v>331914</v>
       </c>
       <c r="D35" s="4">
-        <v>194005</v>
+        <v>268978</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4">
-        <v>44268</v>
+        <v>62936</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="5"/>
@@ -1601,21 +1625,21 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="11">
-        <v>44313</v>
+        <v>44316</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="1"/>
-        <v>203174</v>
+        <v>274907</v>
       </c>
       <c r="D36" s="4">
-        <v>172069</v>
+        <v>227667</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4">
-        <v>31105</v>
+        <v>47240</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="5"/>
@@ -1623,21 +1647,21 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="11">
-        <v>44312</v>
+        <v>44314</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="1"/>
-        <v>263328</v>
+        <v>238273</v>
       </c>
       <c r="D37" s="4">
-        <v>221677</v>
+        <v>194005</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4">
-        <v>41651</v>
+        <v>44268</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
@@ -1645,21 +1669,21 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="11">
-        <v>44309</v>
+        <v>44313</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="1"/>
-        <v>177672</v>
+        <v>203174</v>
       </c>
       <c r="D38" s="4">
-        <v>147989</v>
+        <v>172069</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4">
-        <v>29683</v>
+        <v>31105</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="5"/>
@@ -1667,21 +1691,21 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="11">
-        <v>44308</v>
+        <v>44312</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="1"/>
-        <v>150489</v>
+        <v>263328</v>
       </c>
       <c r="D39" s="4">
-        <v>128634</v>
+        <v>221677</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4">
-        <v>21855</v>
+        <v>41651</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="5"/>
@@ -1689,21 +1713,21 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="11">
-        <v>44307</v>
+        <v>44309</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="1"/>
-        <v>152884</v>
+        <v>177672</v>
       </c>
       <c r="D40" s="4">
-        <v>126188</v>
+        <v>147989</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4">
-        <v>26696</v>
+        <v>29683</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="5"/>
@@ -1711,44 +1735,43 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="11">
-        <v>44306</v>
+        <v>44308</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="1"/>
-        <v>126419</v>
+        <v>150489</v>
       </c>
       <c r="D41" s="4">
-        <v>98622</v>
+        <v>128634</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4">
-        <v>27797</v>
+        <v>21855</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A42" s="13">
-        <v>44305</v>
-      </c>
-      <c r="B42" s="10" t="str">
-        <f t="shared" ref="B42:B45" si="2">"("&amp;TEXT(A42,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A42" s="11">
+        <v>44307</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" si="1"/>
-        <v>119032</v>
+        <v>152884</v>
       </c>
       <c r="D42" s="4">
-        <v>64725</v>
+        <v>126188</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4">
-        <v>54307</v>
+        <v>26696</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="5"/>
@@ -1756,45 +1779,44 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43" s="11">
-        <v>44302</v>
-      </c>
-      <c r="B43" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>(金)</v>
+        <v>44306</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" si="1"/>
-        <v>69687</v>
+        <v>126419</v>
       </c>
       <c r="D43" s="4">
-        <v>29696</v>
+        <v>98622</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4">
-        <v>39991</v>
+        <v>27797</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A44" s="11">
-        <v>44301</v>
+      <c r="A44" s="13">
+        <v>44305</v>
       </c>
       <c r="B44" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>(木)</v>
+        <f t="shared" ref="B44:B47" si="2">"("&amp;TEXT(A44,"aaa")&amp;")"</f>
+        <v>(月)</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" si="1"/>
-        <v>52620</v>
+        <v>119032</v>
       </c>
       <c r="D44" s="4">
-        <v>16637</v>
+        <v>64725</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4">
-        <v>35983</v>
+        <v>54307</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="5"/>
@@ -1802,132 +1824,178 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A45" s="11">
-        <v>44300</v>
+        <v>44302</v>
       </c>
       <c r="B45" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(水)</v>
+        <v>(金)</v>
       </c>
       <c r="C45" s="4">
         <f t="shared" si="1"/>
-        <v>50996</v>
+        <v>69687</v>
       </c>
       <c r="D45" s="4">
-        <v>9569</v>
+        <v>29696</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4">
-        <v>41427</v>
+        <v>39991</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A46" s="8">
-        <v>44299</v>
+      <c r="A46" s="11">
+        <v>44301</v>
       </c>
       <c r="B46" s="10" t="str">
-        <f t="shared" ref="B46:B47" si="3">"("&amp;TEXT(A46,"aaa")&amp;")"</f>
-        <v>(火)</v>
+        <f t="shared" si="2"/>
+        <v>(木)</v>
       </c>
       <c r="C46" s="4">
-        <f t="shared" ref="C46:C47" si="4">SUM(D46:G46)</f>
-        <v>53986</v>
+        <f t="shared" si="1"/>
+        <v>52620</v>
       </c>
       <c r="D46" s="4">
-        <v>13896</v>
+        <v>16637</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4">
-        <v>40090</v>
+        <v>35983</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A47" s="8">
-        <v>44298</v>
+      <c r="A47" s="11">
+        <v>44300</v>
       </c>
       <c r="B47" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>(月)</v>
+        <f t="shared" si="2"/>
+        <v>(水)</v>
       </c>
       <c r="C47" s="4">
-        <f t="shared" si="4"/>
-        <v>96936</v>
+        <f t="shared" si="1"/>
+        <v>50996</v>
       </c>
       <c r="D47" s="4">
-        <v>26850</v>
+        <v>9569</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4">
-        <v>70086</v>
+        <v>41427</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A48" s="6"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="5"/>
+      <c r="A48" s="8">
+        <v>44299</v>
+      </c>
+      <c r="B48" s="10" t="str">
+        <f t="shared" ref="B48:B49" si="3">"("&amp;TEXT(A48,"aaa")&amp;")"</f>
+        <v>(火)</v>
+      </c>
+      <c r="C48" s="4">
+        <f t="shared" ref="C48:C49" si="4">SUM(D48:G48)</f>
+        <v>53986</v>
+      </c>
+      <c r="D48" s="4">
+        <v>13896</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4">
+        <v>40090</v>
+      </c>
+      <c r="G48" s="4"/>
       <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="8">
+        <v>44298</v>
+      </c>
+      <c r="B49" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>(月)</v>
+      </c>
+      <c r="C49" s="4">
+        <f t="shared" si="4"/>
+        <v>96936</v>
+      </c>
+      <c r="D49" s="4">
+        <v>26850</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4">
+        <v>70086</v>
+      </c>
+      <c r="G49" s="4"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A50" s="6"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A51" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="H50" s="5"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
-        <v>6</v>
-      </c>
-      <c r="H51" s="5"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A52" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
       <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
         <v>3</v>
       </c>
-      <c r="H53" s="5"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="H54" s="3"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A56" s="1"/>
+      <c r="H56" s="3"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A58" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Flat: latest data (2021-06-18T06:19:03.680Z) {   "date": "2021-06-18T06:19:03.680Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 75,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data2.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -10,14 +10,14 @@
     <sheet name="医療従事者" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$56</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t> 内１回目</t>
   </si>
@@ -286,7 +286,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（6月16日時点）</t>
+    <t>（6月17日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -398,7 +398,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -443,6 +443,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -800,7 +806,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -828,30 +834,30 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35" t="s">
+      <c r="E3" s="36"/>
+      <c r="F3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="34"/>
+      <c r="G3" s="36"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="34"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="34"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="14" t="s">
         <v>25</v>
       </c>
@@ -868,22 +874,22 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="34"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C16" si="0">SUM(D5:G5)</f>
-        <v>9556960</v>
+        <f t="shared" ref="C5:C17" si="0">SUM(D5:G5)</f>
+        <v>9686290</v>
       </c>
       <c r="D5" s="4">
-        <v>5366267</v>
+        <v>5413193</v>
       </c>
       <c r="E5" s="4">
-        <v>22095</v>
+        <v>26706</v>
       </c>
       <c r="F5" s="4">
-        <v>4168598</v>
+        <v>4246391</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -892,24 +898,24 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="31">
-        <v>44363</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>18</v>
+      <c r="A6" s="33">
+        <v>44364</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>20</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>118735</v>
+        <v>129330</v>
       </c>
       <c r="D6" s="4">
-        <v>43912</v>
+        <v>46926</v>
       </c>
       <c r="E6" s="4">
-        <v>2782</v>
+        <v>4611</v>
       </c>
       <c r="F6" s="4">
-        <v>72041</v>
+        <v>77793</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -918,24 +924,24 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="29">
-        <v>44362</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>28</v>
+      <c r="A7" s="31">
+        <v>44363</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>115363</v>
+        <v>118735</v>
       </c>
       <c r="D7" s="4">
-        <v>40459</v>
+        <v>43912</v>
       </c>
       <c r="E7" s="4">
-        <v>2956</v>
+        <v>2782</v>
       </c>
       <c r="F7" s="4">
-        <v>71948</v>
+        <v>72041</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -944,24 +950,24 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="27">
-        <v>44361</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>21</v>
+      <c r="A8" s="29">
+        <v>44362</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>28</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>214965</v>
+        <v>115363</v>
       </c>
       <c r="D8" s="4">
-        <v>85819</v>
+        <v>40459</v>
       </c>
       <c r="E8" s="4">
-        <v>5610</v>
+        <v>2956</v>
       </c>
       <c r="F8" s="4">
-        <v>123536</v>
+        <v>71948</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -970,24 +976,24 @@
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="25">
-        <v>44358</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>19</v>
+      <c r="A9" s="27">
+        <v>44361</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>21</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>147983</v>
+        <v>214965</v>
       </c>
       <c r="D9" s="4">
-        <v>54834</v>
+        <v>85819</v>
       </c>
       <c r="E9" s="4">
-        <v>1669</v>
+        <v>5610</v>
       </c>
       <c r="F9" s="4">
-        <v>91480</v>
+        <v>123536</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -996,24 +1002,24 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="23">
-        <v>44357</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>20</v>
+      <c r="A10" s="25">
+        <v>44358</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>19</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
-        <v>136591</v>
+        <v>147983</v>
       </c>
       <c r="D10" s="4">
-        <v>52250</v>
+        <v>54834</v>
       </c>
       <c r="E10" s="4">
-        <v>1719</v>
+        <v>1669</v>
       </c>
       <c r="F10" s="4">
-        <v>82622</v>
+        <v>91480</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -1022,24 +1028,24 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="21">
-        <v>44356</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>18</v>
+      <c r="A11" s="23">
+        <v>44357</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>20</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
-        <v>167384</v>
+        <v>136591</v>
       </c>
       <c r="D11" s="4">
-        <v>67694</v>
+        <v>52250</v>
       </c>
       <c r="E11" s="4">
-        <v>1047</v>
+        <v>1719</v>
       </c>
       <c r="F11" s="4">
-        <v>98643</v>
+        <v>82622</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -1048,24 +1054,24 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="19">
-        <v>44355</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>27</v>
+      <c r="A12" s="21">
+        <v>44356</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
-        <v>161922</v>
+        <v>167384</v>
       </c>
       <c r="D12" s="4">
-        <v>71689</v>
+        <v>67694</v>
       </c>
       <c r="E12" s="4">
-        <v>990</v>
+        <v>1047</v>
       </c>
       <c r="F12" s="4">
-        <v>89243</v>
+        <v>98643</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -1074,24 +1080,24 @@
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A13" s="17">
-        <v>44354</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>21</v>
+      <c r="A13" s="19">
+        <v>44355</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="0"/>
-        <v>239337</v>
+        <v>161922</v>
       </c>
       <c r="D13" s="4">
-        <v>104435</v>
+        <v>71689</v>
       </c>
       <c r="E13" s="4">
-        <v>2146</v>
+        <v>990</v>
       </c>
       <c r="F13" s="4">
-        <v>132756</v>
+        <v>89243</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -1100,24 +1106,24 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A14" s="15">
-        <v>44351</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>19</v>
+      <c r="A14" s="17">
+        <v>44354</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="0"/>
-        <v>159203</v>
+        <v>239337</v>
       </c>
       <c r="D14" s="4">
-        <v>62634</v>
+        <v>104435</v>
       </c>
       <c r="E14" s="4">
-        <v>929</v>
+        <v>2146</v>
       </c>
       <c r="F14" s="4">
-        <v>95640</v>
+        <v>132756</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -1126,24 +1132,24 @@
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A15" s="11">
-        <v>44350</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>20</v>
+      <c r="A15" s="15">
+        <v>44351</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="0"/>
-        <v>143157</v>
+        <v>159203</v>
       </c>
       <c r="D15" s="4">
-        <v>59654</v>
+        <v>62634</v>
       </c>
       <c r="E15" s="4">
-        <v>112</v>
+        <v>929</v>
       </c>
       <c r="F15" s="4">
-        <v>83391</v>
+        <v>95640</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
@@ -1153,23 +1159,23 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="11">
-        <v>44349</v>
+        <v>44350</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="0"/>
-        <v>159126</v>
+        <v>143157</v>
       </c>
       <c r="D16" s="4">
-        <v>71140</v>
+        <v>59654</v>
       </c>
       <c r="E16" s="4">
-        <v>316</v>
+        <v>112</v>
       </c>
       <c r="F16" s="4">
-        <v>87670</v>
+        <v>83391</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
@@ -1179,23 +1185,23 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="11">
-        <v>44348</v>
+        <v>44349</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C17" s="4">
-        <f t="shared" ref="C17:C47" si="1">SUM(D17:G17)</f>
-        <v>159057</v>
+        <f t="shared" si="0"/>
+        <v>159126</v>
       </c>
       <c r="D17" s="4">
-        <v>66264</v>
+        <v>71140</v>
       </c>
       <c r="E17" s="4">
-        <v>123</v>
+        <v>316</v>
       </c>
       <c r="F17" s="4">
-        <v>92670</v>
+        <v>87670</v>
       </c>
       <c r="G17" s="4">
         <v>0</v>
@@ -1205,23 +1211,23 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="11">
-        <v>44347</v>
+        <v>44348</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C18" s="4">
-        <f t="shared" si="1"/>
-        <v>273255</v>
+        <f t="shared" ref="C18:C48" si="1">SUM(D18:G18)</f>
+        <v>159057</v>
       </c>
       <c r="D18" s="4">
-        <v>131423</v>
+        <v>66264</v>
       </c>
       <c r="E18" s="4">
-        <v>582</v>
+        <v>123</v>
       </c>
       <c r="F18" s="4">
-        <v>141250</v>
+        <v>92670</v>
       </c>
       <c r="G18" s="4">
         <v>0</v>
@@ -1231,23 +1237,23 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="11">
-        <v>44344</v>
+        <v>44347</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="1"/>
-        <v>164516</v>
+        <v>273255</v>
       </c>
       <c r="D19" s="4">
-        <v>87584</v>
+        <v>131423</v>
       </c>
       <c r="E19" s="4">
-        <v>157</v>
+        <v>582</v>
       </c>
       <c r="F19" s="4">
-        <v>76775</v>
+        <v>141250</v>
       </c>
       <c r="G19" s="4">
         <v>0</v>
@@ -1257,23 +1263,23 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="11">
-        <v>44343</v>
+        <v>44344</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="1"/>
-        <v>145149</v>
+        <v>164516</v>
       </c>
       <c r="D20" s="4">
-        <v>84217</v>
+        <v>87584</v>
       </c>
       <c r="E20" s="4">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="F20" s="4">
-        <v>60892</v>
+        <v>76775</v>
       </c>
       <c r="G20" s="4">
         <v>0</v>
@@ -1283,23 +1289,23 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="11">
-        <v>44342</v>
+        <v>44343</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="1"/>
-        <v>142589</v>
+        <v>145149</v>
       </c>
       <c r="D21" s="4">
-        <v>93243</v>
+        <v>84217</v>
       </c>
       <c r="E21" s="4">
-        <v>172</v>
+        <v>40</v>
       </c>
       <c r="F21" s="4">
-        <v>49174</v>
+        <v>60892</v>
       </c>
       <c r="G21" s="4">
         <v>0</v>
@@ -1309,23 +1315,23 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="11">
-        <v>44341</v>
+        <v>44342</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="1"/>
-        <v>139652</v>
+        <v>142589</v>
       </c>
       <c r="D22" s="4">
-        <v>87114</v>
+        <v>93243</v>
       </c>
       <c r="E22" s="4">
-        <v>476</v>
+        <v>172</v>
       </c>
       <c r="F22" s="4">
-        <v>52062</v>
+        <v>49174</v>
       </c>
       <c r="G22" s="4">
         <v>0</v>
@@ -1335,23 +1341,23 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="11">
-        <v>44340</v>
+        <v>44341</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="1"/>
-        <v>330589</v>
+        <v>139652</v>
       </c>
       <c r="D23" s="4">
-        <v>136491</v>
+        <v>87114</v>
       </c>
       <c r="E23" s="4">
-        <v>269</v>
+        <v>476</v>
       </c>
       <c r="F23" s="4">
-        <v>193829</v>
+        <v>52062</v>
       </c>
       <c r="G23" s="4">
         <v>0</v>
@@ -1361,43 +1367,47 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="11">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" si="1"/>
-        <v>249021</v>
+        <v>330589</v>
       </c>
       <c r="D24" s="4">
-        <v>99918</v>
-      </c>
-      <c r="E24" s="4"/>
+        <v>136491</v>
+      </c>
+      <c r="E24" s="4">
+        <v>269</v>
+      </c>
       <c r="F24" s="4">
-        <v>149103</v>
-      </c>
-      <c r="G24" s="4"/>
+        <v>193829</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0</v>
+      </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="11">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" si="1"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D25" s="4">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
@@ -1405,21 +1415,21 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="11">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="1"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D26" s="4">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5"/>
@@ -1427,21 +1437,21 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="11">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="1"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D27" s="4">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5"/>
@@ -1449,21 +1459,21 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="11">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="1"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D28" s="4">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="5"/>
@@ -1471,21 +1481,21 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="11">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="1"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D29" s="4">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5"/>
@@ -1493,21 +1503,21 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="11">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="1"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D30" s="4">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
@@ -1515,21 +1525,21 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="11">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="1"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D31" s="4">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="5"/>
@@ -1537,21 +1547,21 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="11">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="1"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D32" s="4">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5"/>
@@ -1559,21 +1569,21 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="11">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="1"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D33" s="4">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5"/>
@@ -1581,21 +1591,21 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="11">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="1"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D34" s="4">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="5"/>
@@ -1603,21 +1613,21 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="11">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="1"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D35" s="4">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="5"/>
@@ -1625,21 +1635,21 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="11">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="1"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D36" s="4">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="5"/>
@@ -1647,21 +1657,21 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="11">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="1"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D37" s="4">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
@@ -1669,21 +1679,21 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="11">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="1"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D38" s="4">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="5"/>
@@ -1691,21 +1701,21 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="11">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="1"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D39" s="4">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="5"/>
@@ -1713,21 +1723,21 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="11">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="1"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D40" s="4">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="5"/>
@@ -1735,21 +1745,21 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="11">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="1"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D41" s="4">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="5"/>
@@ -1757,21 +1767,21 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42" s="11">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" si="1"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D42" s="4">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="5"/>
@@ -1779,67 +1789,66 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43" s="11">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" si="1"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D43" s="4">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A44" s="13">
-        <v>44305</v>
-      </c>
-      <c r="B44" s="10" t="str">
-        <f t="shared" ref="B44:B47" si="2">"("&amp;TEXT(A44,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A44" s="11">
+        <v>44306</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" si="1"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D44" s="4">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A45" s="11">
-        <v>44302</v>
+      <c r="A45" s="13">
+        <v>44305</v>
       </c>
       <c r="B45" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>(金)</v>
+        <f t="shared" ref="B45:B48" si="2">"("&amp;TEXT(A45,"aaa")&amp;")"</f>
+        <v>(月)</v>
       </c>
       <c r="C45" s="4">
         <f t="shared" si="1"/>
-        <v>69687</v>
+        <v>119032</v>
       </c>
       <c r="D45" s="4">
-        <v>29696</v>
+        <v>64725</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4">
-        <v>39991</v>
+        <v>54307</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="5"/>
@@ -1847,22 +1856,22 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A46" s="11">
-        <v>44301</v>
+        <v>44302</v>
       </c>
       <c r="B46" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(木)</v>
+        <v>(金)</v>
       </c>
       <c r="C46" s="4">
         <f t="shared" si="1"/>
-        <v>52620</v>
+        <v>69687</v>
       </c>
       <c r="D46" s="4">
-        <v>16637</v>
+        <v>29696</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4">
-        <v>35983</v>
+        <v>39991</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="5"/>
@@ -1870,45 +1879,45 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47" s="11">
-        <v>44300</v>
+        <v>44301</v>
       </c>
       <c r="B47" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(水)</v>
+        <v>(木)</v>
       </c>
       <c r="C47" s="4">
         <f t="shared" si="1"/>
-        <v>50996</v>
+        <v>52620</v>
       </c>
       <c r="D47" s="4">
-        <v>9569</v>
+        <v>16637</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4">
-        <v>41427</v>
+        <v>35983</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A48" s="8">
-        <v>44299</v>
+      <c r="A48" s="11">
+        <v>44300</v>
       </c>
       <c r="B48" s="10" t="str">
-        <f t="shared" ref="B48:B49" si="3">"("&amp;TEXT(A48,"aaa")&amp;")"</f>
-        <v>(火)</v>
+        <f t="shared" si="2"/>
+        <v>(水)</v>
       </c>
       <c r="C48" s="4">
-        <f t="shared" ref="C48:C49" si="4">SUM(D48:G48)</f>
-        <v>53986</v>
+        <f t="shared" si="1"/>
+        <v>50996</v>
       </c>
       <c r="D48" s="4">
-        <v>13896</v>
+        <v>9569</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4">
-        <v>40090</v>
+        <v>41427</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="5"/>
@@ -1916,86 +1925,109 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A49" s="8">
-        <v>44298</v>
+        <v>44299</v>
       </c>
       <c r="B49" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>(月)</v>
+        <f t="shared" ref="B49:B50" si="3">"("&amp;TEXT(A49,"aaa")&amp;")"</f>
+        <v>(火)</v>
       </c>
       <c r="C49" s="4">
-        <f t="shared" si="4"/>
-        <v>96936</v>
+        <f t="shared" ref="C49:C50" si="4">SUM(D49:G49)</f>
+        <v>53986</v>
       </c>
       <c r="D49" s="4">
-        <v>26850</v>
+        <v>13896</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4">
-        <v>70086</v>
+        <v>40090</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A50" s="6"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="5"/>
+      <c r="A50" s="8">
+        <v>44298</v>
+      </c>
+      <c r="B50" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>(月)</v>
+      </c>
+      <c r="C50" s="4">
+        <f t="shared" si="4"/>
+        <v>96936</v>
+      </c>
+      <c r="D50" s="4">
+        <v>26850</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4">
+        <v>70086</v>
+      </c>
+      <c r="G50" s="4"/>
       <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="6"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A52" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="5"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="3"/>
       <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
         <v>6</v>
       </c>
-      <c r="H53" s="5"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A54" s="1" t="s">
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H54" s="5"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
         <v>3</v>
       </c>
-      <c r="H55" s="5"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="H56" s="3"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A58" s="1"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="H57" s="3"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A59" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Flat: latest data (2021-06-22T06:18:53.130Z) {   "date": "2021-06-22T06:18:53.130Z",   "files": [     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 77,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data2.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="医療従事者" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$56</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">医療従事者!$A$1:$G$57</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t> 内１回目</t>
   </si>
@@ -163,6 +163,114 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>(火)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(水)</t>
+    <rPh sb="1" eb="2">
+      <t>スイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(木)</t>
+    <rPh sb="1" eb="2">
+      <t>モク</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(金)</t>
+    <rPh sb="1" eb="2">
+      <t>キン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(月)</t>
+    <rPh sb="1" eb="2">
+      <t>ゲツ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(火)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(水)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(金)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(木)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(月)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(火)</t>
+    <rPh sb="1" eb="2">
+      <t>ヒ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(火)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(火)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ファイザー社</t>
+    <rPh sb="5" eb="6">
+      <t>シャ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>武田/モデルナ社</t>
+    <rPh sb="0" eb="2">
+      <t>タケダ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>シャ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(火)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(火)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(木)</t>
+  </si>
+  <si>
+    <t>（6月18日時点）</t>
+    <rPh sb="2" eb="3">
+      <t>ゲツ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ニチ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ジテン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>注：ワクチン接種円滑化システム（V-SYS）への報告（17時時点）を集計（高齢者等を除く）。</t>
     <rPh sb="6" eb="8">
       <t>セッシュ</t>
@@ -190,111 +298,6 @@
     </rPh>
     <rPh sb="42" eb="43">
       <t>ノゾ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(火)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(水)</t>
-    <rPh sb="1" eb="2">
-      <t>スイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(木)</t>
-    <rPh sb="1" eb="2">
-      <t>モク</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(金)</t>
-    <rPh sb="1" eb="2">
-      <t>キン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(月)</t>
-    <rPh sb="1" eb="2">
-      <t>ゲツ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(火)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(水)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(金)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(木)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(月)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(火)</t>
-    <rPh sb="1" eb="2">
-      <t>ヒ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(火)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(火)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>ファイザー社</t>
-    <rPh sb="5" eb="6">
-      <t>シャ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>武田/モデルナ社</t>
-    <rPh sb="0" eb="2">
-      <t>タケダ</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>シャ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(火)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>(火)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>（6月17日時点）</t>
-    <rPh sb="2" eb="3">
-      <t>ゲツ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ニチ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ジテン</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -806,10 +809,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -859,16 +862,16 @@
       <c r="B4" s="39"/>
       <c r="C4" s="36"/>
       <c r="D4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>26</v>
-      </c>
       <c r="F4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>26</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -879,17 +882,17 @@
       </c>
       <c r="B5" s="36"/>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C17" si="0">SUM(D5:G5)</f>
-        <v>9686290</v>
+        <f t="shared" ref="C5:C18" si="0">SUM(D5:G5)</f>
+        <v>9812238</v>
       </c>
       <c r="D5" s="4">
-        <v>5413193</v>
+        <v>5463305</v>
       </c>
       <c r="E5" s="4">
-        <v>26706</v>
+        <v>28851</v>
       </c>
       <c r="F5" s="4">
-        <v>4246391</v>
+        <v>4320082</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -899,23 +902,23 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="33">
-        <v>44364</v>
+        <v>44365</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>129330</v>
+        <v>125948</v>
       </c>
       <c r="D6" s="4">
-        <v>46926</v>
+        <v>50112</v>
       </c>
       <c r="E6" s="4">
-        <v>4611</v>
+        <v>2145</v>
       </c>
       <c r="F6" s="4">
-        <v>77793</v>
+        <v>73691</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -924,24 +927,24 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="31">
-        <v>44363</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>18</v>
+      <c r="A7" s="33">
+        <v>44364</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>28</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>118735</v>
+        <v>129330</v>
       </c>
       <c r="D7" s="4">
-        <v>43912</v>
+        <v>46926</v>
       </c>
       <c r="E7" s="4">
-        <v>2782</v>
+        <v>4611</v>
       </c>
       <c r="F7" s="4">
-        <v>72041</v>
+        <v>77793</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -950,24 +953,24 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="29">
-        <v>44362</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>28</v>
+      <c r="A8" s="31">
+        <v>44363</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>17</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>115363</v>
+        <v>118735</v>
       </c>
       <c r="D8" s="4">
-        <v>40459</v>
+        <v>43912</v>
       </c>
       <c r="E8" s="4">
-        <v>2956</v>
+        <v>2782</v>
       </c>
       <c r="F8" s="4">
-        <v>71948</v>
+        <v>72041</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -976,24 +979,24 @@
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="27">
-        <v>44361</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>21</v>
+      <c r="A9" s="29">
+        <v>44362</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>214965</v>
+        <v>115363</v>
       </c>
       <c r="D9" s="4">
-        <v>85819</v>
+        <v>40459</v>
       </c>
       <c r="E9" s="4">
-        <v>5610</v>
+        <v>2956</v>
       </c>
       <c r="F9" s="4">
-        <v>123536</v>
+        <v>71948</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -1002,24 +1005,24 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="25">
-        <v>44358</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>19</v>
+      <c r="A10" s="27">
+        <v>44361</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>20</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
-        <v>147983</v>
+        <v>214965</v>
       </c>
       <c r="D10" s="4">
-        <v>54834</v>
+        <v>85819</v>
       </c>
       <c r="E10" s="4">
-        <v>1669</v>
+        <v>5610</v>
       </c>
       <c r="F10" s="4">
-        <v>91480</v>
+        <v>123536</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -1028,24 +1031,24 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="23">
-        <v>44357</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>20</v>
+      <c r="A11" s="25">
+        <v>44358</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>18</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
-        <v>136591</v>
+        <v>147983</v>
       </c>
       <c r="D11" s="4">
-        <v>52250</v>
+        <v>54834</v>
       </c>
       <c r="E11" s="4">
-        <v>1719</v>
+        <v>1669</v>
       </c>
       <c r="F11" s="4">
-        <v>82622</v>
+        <v>91480</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -1054,24 +1057,24 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="21">
-        <v>44356</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>18</v>
+      <c r="A12" s="23">
+        <v>44357</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>19</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
-        <v>167384</v>
+        <v>136591</v>
       </c>
       <c r="D12" s="4">
-        <v>67694</v>
+        <v>52250</v>
       </c>
       <c r="E12" s="4">
-        <v>1047</v>
+        <v>1719</v>
       </c>
       <c r="F12" s="4">
-        <v>98643</v>
+        <v>82622</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -1080,24 +1083,24 @@
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A13" s="19">
-        <v>44355</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>27</v>
+      <c r="A13" s="21">
+        <v>44356</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>17</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="0"/>
-        <v>161922</v>
+        <v>167384</v>
       </c>
       <c r="D13" s="4">
-        <v>71689</v>
+        <v>67694</v>
       </c>
       <c r="E13" s="4">
-        <v>990</v>
+        <v>1047</v>
       </c>
       <c r="F13" s="4">
-        <v>89243</v>
+        <v>98643</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -1106,24 +1109,24 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A14" s="17">
-        <v>44354</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>21</v>
+      <c r="A14" s="19">
+        <v>44355</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="0"/>
-        <v>239337</v>
+        <v>161922</v>
       </c>
       <c r="D14" s="4">
-        <v>104435</v>
+        <v>71689</v>
       </c>
       <c r="E14" s="4">
-        <v>2146</v>
+        <v>990</v>
       </c>
       <c r="F14" s="4">
-        <v>132756</v>
+        <v>89243</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -1132,24 +1135,24 @@
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A15" s="15">
-        <v>44351</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>19</v>
+      <c r="A15" s="17">
+        <v>44354</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>20</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="0"/>
-        <v>159203</v>
+        <v>239337</v>
       </c>
       <c r="D15" s="4">
-        <v>62634</v>
+        <v>104435</v>
       </c>
       <c r="E15" s="4">
-        <v>929</v>
+        <v>2146</v>
       </c>
       <c r="F15" s="4">
-        <v>95640</v>
+        <v>132756</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
@@ -1158,24 +1161,24 @@
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A16" s="11">
-        <v>44350</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>20</v>
+      <c r="A16" s="15">
+        <v>44351</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="0"/>
-        <v>143157</v>
+        <v>159203</v>
       </c>
       <c r="D16" s="4">
-        <v>59654</v>
+        <v>62634</v>
       </c>
       <c r="E16" s="4">
-        <v>112</v>
+        <v>929</v>
       </c>
       <c r="F16" s="4">
-        <v>83391</v>
+        <v>95640</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
@@ -1185,23 +1188,23 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="11">
-        <v>44349</v>
+        <v>44350</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="0"/>
-        <v>159126</v>
+        <v>143157</v>
       </c>
       <c r="D17" s="4">
-        <v>71140</v>
+        <v>59654</v>
       </c>
       <c r="E17" s="4">
-        <v>316</v>
+        <v>112</v>
       </c>
       <c r="F17" s="4">
-        <v>87670</v>
+        <v>83391</v>
       </c>
       <c r="G17" s="4">
         <v>0</v>
@@ -1211,23 +1214,23 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="11">
-        <v>44348</v>
+        <v>44349</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C18" s="4">
-        <f t="shared" ref="C18:C48" si="1">SUM(D18:G18)</f>
-        <v>159057</v>
+        <f t="shared" si="0"/>
+        <v>159126</v>
       </c>
       <c r="D18" s="4">
-        <v>66264</v>
+        <v>71140</v>
       </c>
       <c r="E18" s="4">
-        <v>123</v>
+        <v>316</v>
       </c>
       <c r="F18" s="4">
-        <v>92670</v>
+        <v>87670</v>
       </c>
       <c r="G18" s="4">
         <v>0</v>
@@ -1237,23 +1240,23 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="11">
-        <v>44347</v>
+        <v>44348</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C19" s="4">
-        <f t="shared" si="1"/>
-        <v>273255</v>
+        <f t="shared" ref="C19:C49" si="1">SUM(D19:G19)</f>
+        <v>159057</v>
       </c>
       <c r="D19" s="4">
-        <v>131423</v>
+        <v>66264</v>
       </c>
       <c r="E19" s="4">
-        <v>582</v>
+        <v>123</v>
       </c>
       <c r="F19" s="4">
-        <v>141250</v>
+        <v>92670</v>
       </c>
       <c r="G19" s="4">
         <v>0</v>
@@ -1263,23 +1266,23 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="11">
-        <v>44344</v>
+        <v>44347</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="1"/>
-        <v>164516</v>
+        <v>273255</v>
       </c>
       <c r="D20" s="4">
-        <v>87584</v>
+        <v>131423</v>
       </c>
       <c r="E20" s="4">
-        <v>157</v>
+        <v>582</v>
       </c>
       <c r="F20" s="4">
-        <v>76775</v>
+        <v>141250</v>
       </c>
       <c r="G20" s="4">
         <v>0</v>
@@ -1289,23 +1292,23 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="11">
-        <v>44343</v>
+        <v>44344</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="1"/>
-        <v>145149</v>
+        <v>164516</v>
       </c>
       <c r="D21" s="4">
-        <v>84217</v>
+        <v>87584</v>
       </c>
       <c r="E21" s="4">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="F21" s="4">
-        <v>60892</v>
+        <v>76775</v>
       </c>
       <c r="G21" s="4">
         <v>0</v>
@@ -1315,23 +1318,23 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="11">
-        <v>44342</v>
+        <v>44343</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="1"/>
-        <v>142589</v>
+        <v>145149</v>
       </c>
       <c r="D22" s="4">
-        <v>93243</v>
+        <v>84217</v>
       </c>
       <c r="E22" s="4">
-        <v>172</v>
+        <v>40</v>
       </c>
       <c r="F22" s="4">
-        <v>49174</v>
+        <v>60892</v>
       </c>
       <c r="G22" s="4">
         <v>0</v>
@@ -1341,23 +1344,23 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="11">
-        <v>44341</v>
+        <v>44342</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="1"/>
-        <v>139652</v>
+        <v>142589</v>
       </c>
       <c r="D23" s="4">
-        <v>87114</v>
+        <v>93243</v>
       </c>
       <c r="E23" s="4">
-        <v>476</v>
+        <v>172</v>
       </c>
       <c r="F23" s="4">
-        <v>52062</v>
+        <v>49174</v>
       </c>
       <c r="G23" s="4">
         <v>0</v>
@@ -1367,23 +1370,23 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="11">
-        <v>44340</v>
+        <v>44341</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" si="1"/>
-        <v>330589</v>
+        <v>139652</v>
       </c>
       <c r="D24" s="4">
-        <v>136491</v>
+        <v>87114</v>
       </c>
       <c r="E24" s="4">
-        <v>269</v>
+        <v>476</v>
       </c>
       <c r="F24" s="4">
-        <v>193829</v>
+        <v>52062</v>
       </c>
       <c r="G24" s="4">
         <v>0</v>
@@ -1393,43 +1396,47 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="11">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" si="1"/>
-        <v>249021</v>
+        <v>330589</v>
       </c>
       <c r="D25" s="4">
-        <v>99918</v>
-      </c>
-      <c r="E25" s="4"/>
+        <v>136491</v>
+      </c>
+      <c r="E25" s="4">
+        <v>269</v>
+      </c>
       <c r="F25" s="4">
-        <v>149103</v>
-      </c>
-      <c r="G25" s="4"/>
+        <v>193829</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="11">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="1"/>
-        <v>190533</v>
+        <v>249021</v>
       </c>
       <c r="D26" s="4">
-        <v>81422</v>
+        <v>99918</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4">
-        <v>109111</v>
+        <v>149103</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5"/>
@@ -1437,21 +1444,21 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="11">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="1"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D27" s="4">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5"/>
@@ -1459,21 +1466,21 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="11">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="1"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D28" s="4">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="5"/>
@@ -1481,21 +1488,21 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="11">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="1"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D29" s="4">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5"/>
@@ -1503,21 +1510,21 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="11">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="1"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D30" s="4">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
@@ -1525,21 +1532,21 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="11">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="1"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D31" s="4">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="5"/>
@@ -1547,21 +1554,21 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="11">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="1"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D32" s="4">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5"/>
@@ -1569,21 +1576,21 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="11">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="1"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D33" s="4">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5"/>
@@ -1591,21 +1598,21 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="11">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="1"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D34" s="4">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="5"/>
@@ -1613,21 +1620,21 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="11">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="1"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D35" s="4">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="5"/>
@@ -1635,21 +1642,21 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="11">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="1"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D36" s="4">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="5"/>
@@ -1657,21 +1664,21 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="11">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="1"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D37" s="4">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
@@ -1679,21 +1686,21 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="11">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="1"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D38" s="4">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="5"/>
@@ -1701,21 +1708,21 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="11">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="1"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D39" s="4">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="5"/>
@@ -1723,21 +1730,21 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="11">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="1"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D40" s="4">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="5"/>
@@ -1745,21 +1752,21 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="11">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="1"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D41" s="4">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="5"/>
@@ -1767,21 +1774,21 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42" s="11">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" si="1"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D42" s="4">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="5"/>
@@ -1789,21 +1796,21 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43" s="11">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" si="1"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D43" s="4">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="5"/>
@@ -1811,67 +1818,66 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44" s="11">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" si="1"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D44" s="4">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A45" s="13">
-        <v>44305</v>
-      </c>
-      <c r="B45" s="10" t="str">
-        <f t="shared" ref="B45:B48" si="2">"("&amp;TEXT(A45,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A45" s="11">
+        <v>44306</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="C45" s="4">
         <f t="shared" si="1"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D45" s="4">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A46" s="11">
-        <v>44302</v>
+      <c r="A46" s="13">
+        <v>44305</v>
       </c>
       <c r="B46" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>(金)</v>
+        <f t="shared" ref="B46:B49" si="2">"("&amp;TEXT(A46,"aaa")&amp;")"</f>
+        <v>(月)</v>
       </c>
       <c r="C46" s="4">
         <f t="shared" si="1"/>
-        <v>69687</v>
+        <v>119032</v>
       </c>
       <c r="D46" s="4">
-        <v>29696</v>
+        <v>64725</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4">
-        <v>39991</v>
+        <v>54307</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="5"/>
@@ -1879,22 +1885,22 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47" s="11">
-        <v>44301</v>
+        <v>44302</v>
       </c>
       <c r="B47" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(木)</v>
+        <v>(金)</v>
       </c>
       <c r="C47" s="4">
         <f t="shared" si="1"/>
-        <v>52620</v>
+        <v>69687</v>
       </c>
       <c r="D47" s="4">
-        <v>16637</v>
+        <v>29696</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4">
-        <v>35983</v>
+        <v>39991</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="5"/>
@@ -1902,45 +1908,45 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A48" s="11">
-        <v>44300</v>
+        <v>44301</v>
       </c>
       <c r="B48" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>(水)</v>
+        <v>(木)</v>
       </c>
       <c r="C48" s="4">
         <f t="shared" si="1"/>
-        <v>50996</v>
+        <v>52620</v>
       </c>
       <c r="D48" s="4">
-        <v>9569</v>
+        <v>16637</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4">
-        <v>41427</v>
+        <v>35983</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A49" s="8">
-        <v>44299</v>
+      <c r="A49" s="11">
+        <v>44300</v>
       </c>
       <c r="B49" s="10" t="str">
-        <f t="shared" ref="B49:B50" si="3">"("&amp;TEXT(A49,"aaa")&amp;")"</f>
-        <v>(火)</v>
+        <f t="shared" si="2"/>
+        <v>(水)</v>
       </c>
       <c r="C49" s="4">
-        <f t="shared" ref="C49:C50" si="4">SUM(D49:G49)</f>
-        <v>53986</v>
+        <f t="shared" si="1"/>
+        <v>50996</v>
       </c>
       <c r="D49" s="4">
-        <v>13896</v>
+        <v>9569</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4">
-        <v>40090</v>
+        <v>41427</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="5"/>
@@ -1948,86 +1954,109 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A50" s="8">
-        <v>44298</v>
+        <v>44299</v>
       </c>
       <c r="B50" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>(月)</v>
+        <f t="shared" ref="B50:B51" si="3">"("&amp;TEXT(A50,"aaa")&amp;")"</f>
+        <v>(火)</v>
       </c>
       <c r="C50" s="4">
-        <f t="shared" si="4"/>
-        <v>96936</v>
+        <f t="shared" ref="C50:C51" si="4">SUM(D50:G50)</f>
+        <v>53986</v>
       </c>
       <c r="D50" s="4">
-        <v>26850</v>
+        <v>13896</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4">
-        <v>70086</v>
+        <v>40090</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A51" s="6"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="5"/>
+      <c r="A51" s="8">
+        <v>44298</v>
+      </c>
+      <c r="B51" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>(月)</v>
+      </c>
+      <c r="C51" s="4">
+        <f t="shared" si="4"/>
+        <v>96936</v>
+      </c>
+      <c r="D51" s="4">
+        <v>26850</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4">
+        <v>70086</v>
+      </c>
+      <c r="G51" s="4"/>
       <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A52" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="3"/>
+      <c r="A52" s="6"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="5"/>
       <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
+      <c r="A53" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="3"/>
       <c r="H53" s="5"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
         <v>6</v>
       </c>
-      <c r="H54" s="5"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A55" s="1" t="s">
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H55" s="5"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
         <v>3</v>
       </c>
-      <c r="H56" s="5"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="H57" s="3"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A59" s="1"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="H58" s="3"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A60" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>